<commit_message>
adding J. McMahon to EC, fixing duplicates and format typos
</commit_message>
<xml_diff>
--- a/ReferenceDocuments/ReportAuthors.xlsx
+++ b/ReferenceDocuments/ReportAuthors.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="321">
   <si>
     <t>Report Authors</t>
   </si>
@@ -205,12 +205,6 @@
     <t>Feeney</t>
   </si>
   <si>
-    <t>Jeff</t>
-  </si>
-  <si>
-    <t>Fillippini</t>
-  </si>
-  <si>
     <t>Laura</t>
   </si>
   <si>
@@ -586,9 +580,6 @@
     <t>LBNL</t>
   </si>
   <si>
-    <t>Shirokoff,</t>
-  </si>
-  <si>
     <t>Erik</t>
   </si>
   <si>
@@ -980,6 +971,12 @@
   </si>
   <si>
     <t>Column goes to latex</t>
+  </si>
+  <si>
+    <t>Douglas</t>
+  </si>
+  <si>
+    <t>Shirokoff</t>
   </si>
 </sst>
 </file>
@@ -1412,8 +1409,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:K179"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35:XFD35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -1443,25 +1440,25 @@
       </c>
       <c r="B3"/>
       <c r="C3" s="1" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="2" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="B4"/>
       <c r="C4" s="1" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="2" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="B5"/>
       <c r="C5" s="1" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -1469,10 +1466,10 @@
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="4" t="s">
+        <v>276</v>
+      </c>
+      <c r="B7" t="s">
         <v>279</v>
-      </c>
-      <c r="B7" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -1493,16 +1490,16 @@
         <v>5</v>
       </c>
       <c r="G9" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="I9" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="J9" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="K9" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -1546,19 +1543,19 @@
         <v>11</v>
       </c>
       <c r="G11" t="str">
-        <f t="shared" ref="G11:G74" si="0">CONCATENATE(B11," ",C11,K11,"\\")</f>
+        <f t="shared" ref="G11:G72" si="0">CONCATENATE(B11," ",C11,K11,"\\")</f>
         <v>Peter Ashton                    \\</v>
       </c>
       <c r="I11">
-        <f t="shared" ref="I11:I74" si="1">LEN(B11) + LEN(C11) +1</f>
+        <f t="shared" ref="I11:I72" si="1">LEN(B11) + LEN(C11) +1</f>
         <v>12</v>
       </c>
       <c r="J11">
-        <f t="shared" ref="J11:J74" si="2">IF(I11&lt;30,(32-I11),3)</f>
+        <f t="shared" ref="J11:J72" si="2">IF(I11&lt;30,(32-I11),3)</f>
         <v>20</v>
       </c>
       <c r="K11" t="str">
-        <f t="shared" ref="K11:K74" si="3">REPT(" ",J11)</f>
+        <f t="shared" ref="K11:K72" si="3">REPT(" ",J11)</f>
         <v xml:space="preserve">                    </v>
       </c>
     </row>
@@ -1732,17 +1729,17 @@
     </row>
     <row r="18" spans="2:11">
       <c r="B18" t="s">
+        <v>171</v>
+      </c>
+      <c r="C18" t="s">
+        <v>172</v>
+      </c>
+      <c r="D18" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" t="s">
         <v>173</v>
       </c>
-      <c r="C18" t="s">
-        <v>174</v>
-      </c>
-      <c r="D18" t="s">
-        <v>8</v>
-      </c>
-      <c r="E18" t="s">
-        <v>175</v>
-      </c>
       <c r="G18" t="str">
         <f t="shared" si="0"/>
         <v>Jamie Bock                      \\</v>
@@ -1761,1006 +1758,1009 @@
       </c>
     </row>
     <row r="19" spans="2:11">
-      <c r="B19" s="1" t="s">
-        <v>26</v>
+      <c r="B19" t="s">
+        <v>28</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D19" t="s">
         <v>8</v>
       </c>
+      <c r="E19" t="s">
+        <v>30</v>
+      </c>
       <c r="G19" t="str">
         <f t="shared" si="0"/>
-        <v>Kim Boddy                       \\</v>
+        <v>Matteo Bonato                   \\</v>
       </c>
       <c r="I19">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="J19">
         <f t="shared" si="2"/>
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="K19" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">                       </v>
+        <v xml:space="preserve">                   </v>
       </c>
     </row>
     <row r="20" spans="2:11">
-      <c r="B20" t="s">
-        <v>28</v>
+      <c r="B20" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D20" t="s">
         <v>8</v>
       </c>
-      <c r="E20" t="s">
-        <v>30</v>
-      </c>
       <c r="G20" t="str">
         <f t="shared" si="0"/>
-        <v>Matteo Bonato                   \\</v>
+        <v>Julian Borrill                  \\</v>
       </c>
       <c r="I20">
         <f t="shared" si="1"/>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="J20">
         <f t="shared" si="2"/>
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K20" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">                   </v>
+        <v xml:space="preserve">                  </v>
       </c>
     </row>
     <row r="21" spans="2:11">
       <c r="B21" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D21" t="s">
         <v>8</v>
       </c>
       <c r="G21" t="str">
         <f t="shared" si="0"/>
-        <v>Julian Borrill                  \\</v>
+        <v>Francois Boulanger              \\</v>
       </c>
       <c r="I21">
         <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
-      <c r="J21">
-        <f t="shared" si="2"/>
+      <c r="K21" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">              </v>
+      </c>
+    </row>
+    <row r="22" spans="2:11">
+      <c r="B22" t="s">
+        <v>35</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D22" t="s">
+        <v>8</v>
+      </c>
+      <c r="E22" t="s">
+        <v>37</v>
+      </c>
+      <c r="G22" t="str">
+        <f t="shared" si="0"/>
+        <v>Blakesley Burkhart              \\</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="1"/>
         <v>18</v>
       </c>
-      <c r="K21" t="str">
+      <c r="J22">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="K22" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">              </v>
+      </c>
+    </row>
+    <row r="23" spans="2:11">
+      <c r="B23" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D23" t="s">
+        <v>8</v>
+      </c>
+      <c r="G23" t="str">
+        <f t="shared" si="0"/>
+        <v>David Chuss                     \\</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="J23">
+        <f t="shared" si="2"/>
+        <v>21</v>
+      </c>
+      <c r="K23" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">                     </v>
+      </c>
+    </row>
+    <row r="24" spans="2:11">
+      <c r="B24" t="s">
+        <v>40</v>
+      </c>
+      <c r="C24" t="s">
+        <v>41</v>
+      </c>
+      <c r="D24" t="s">
+        <v>8</v>
+      </c>
+      <c r="E24" t="s">
+        <v>42</v>
+      </c>
+      <c r="G24" t="str">
+        <f t="shared" si="0"/>
+        <v>Susan E. Clark                  \\</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="J24">
+        <f t="shared" si="2"/>
+        <v>18</v>
+      </c>
+      <c r="K24" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve">                  </v>
       </c>
     </row>
-    <row r="22" spans="2:11">
-      <c r="B22" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D22" t="s">
-        <v>8</v>
-      </c>
-      <c r="G22" t="str">
-        <f t="shared" si="0"/>
-        <v>Francois Boulanger              \\</v>
-      </c>
-      <c r="I22">
-        <f t="shared" si="1"/>
-        <v>18</v>
-      </c>
-      <c r="J22">
-        <f t="shared" si="2"/>
-        <v>14</v>
-      </c>
-      <c r="K22" t="str">
-        <f t="shared" si="3"/>
-        <v xml:space="preserve">              </v>
-      </c>
-    </row>
-    <row r="23" spans="2:11">
-      <c r="B23" t="s">
-        <v>35</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D23" t="s">
-        <v>8</v>
-      </c>
-      <c r="E23" t="s">
-        <v>37</v>
-      </c>
-      <c r="G23" t="str">
-        <f t="shared" si="0"/>
-        <v>Blakesley Burkhart              \\</v>
-      </c>
-      <c r="I23">
-        <f t="shared" si="1"/>
-        <v>18</v>
-      </c>
-      <c r="J23">
-        <f t="shared" si="2"/>
-        <v>14</v>
-      </c>
-      <c r="K23" t="str">
-        <f t="shared" si="3"/>
-        <v xml:space="preserve">              </v>
-      </c>
-    </row>
-    <row r="24" spans="2:11">
-      <c r="B24" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D24" t="s">
-        <v>8</v>
-      </c>
-      <c r="G24" t="str">
-        <f t="shared" si="0"/>
-        <v>David Chuss                     \\</v>
-      </c>
-      <c r="I24">
-        <f t="shared" si="1"/>
-        <v>11</v>
-      </c>
-      <c r="J24">
-        <f t="shared" si="2"/>
-        <v>21</v>
-      </c>
-      <c r="K24" t="str">
-        <f t="shared" si="3"/>
-        <v xml:space="preserve">                     </v>
-      </c>
-    </row>
     <row r="25" spans="2:11">
-      <c r="B25" t="s">
-        <v>40</v>
-      </c>
-      <c r="C25" t="s">
-        <v>41</v>
+      <c r="B25" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>44</v>
       </c>
       <c r="D25" t="s">
         <v>8</v>
       </c>
-      <c r="E25" t="s">
-        <v>42</v>
-      </c>
       <c r="G25" t="str">
         <f t="shared" si="0"/>
-        <v>Susan E. Clark                  \\</v>
+        <v>Brendan Crill                   \\</v>
       </c>
       <c r="I25">
         <f t="shared" si="1"/>
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J25">
         <f t="shared" si="2"/>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="K25" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">                  </v>
+        <v xml:space="preserve">                   </v>
       </c>
     </row>
     <row r="26" spans="2:11">
-      <c r="B26" s="1" t="s">
-        <v>43</v>
+      <c r="B26" t="s">
+        <v>313</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>44</v>
+        <v>312</v>
       </c>
       <c r="D26" t="s">
         <v>8</v>
       </c>
+      <c r="E26" t="s">
+        <v>45</v>
+      </c>
       <c r="G26" t="str">
         <f t="shared" si="0"/>
-        <v>Brendan Crill                   \\</v>
+        <v>Gianfranco De Zotti             \\</v>
       </c>
       <c r="I26">
         <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="J26">
+        <f t="shared" si="2"/>
         <v>13</v>
       </c>
-      <c r="J26">
-        <f t="shared" si="2"/>
-        <v>19</v>
-      </c>
       <c r="K26" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">                   </v>
+        <v xml:space="preserve">             </v>
       </c>
     </row>
     <row r="27" spans="2:11">
       <c r="B27" t="s">
-        <v>316</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>315</v>
+        <v>46</v>
+      </c>
+      <c r="C27" t="s">
+        <v>47</v>
       </c>
       <c r="D27" t="s">
         <v>8</v>
       </c>
       <c r="E27" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="G27" t="str">
         <f t="shared" si="0"/>
-        <v>Gianfranco De Zotti             \\</v>
+        <v>Jacques Delabrouille            \\</v>
       </c>
       <c r="I27">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J27">
         <f t="shared" si="2"/>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K27" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">             </v>
+        <v xml:space="preserve">            </v>
       </c>
     </row>
     <row r="28" spans="2:11">
       <c r="B28" t="s">
-        <v>46</v>
-      </c>
-      <c r="C28" t="s">
-        <v>47</v>
+        <v>49</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>50</v>
       </c>
       <c r="D28" t="s">
         <v>8</v>
       </c>
       <c r="E28" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="G28" t="str">
         <f t="shared" si="0"/>
-        <v>Jacques Delabrouille            \\</v>
+        <v>Eleonora Di Valentino           \\</v>
       </c>
       <c r="I28">
         <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
+      <c r="J28">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="K28" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">           </v>
+      </c>
+    </row>
+    <row r="29" spans="2:11">
+      <c r="B29" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D29" t="s">
+        <v>8</v>
+      </c>
+      <c r="G29" t="str">
+        <f t="shared" si="0"/>
+        <v>Joy Didier                      \\</v>
+      </c>
+      <c r="I29">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="J29">
+        <f t="shared" si="2"/>
+        <v>22</v>
+      </c>
+      <c r="K29" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">                      </v>
+      </c>
+    </row>
+    <row r="30" spans="2:11">
+      <c r="B30" t="s">
+        <v>54</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="D30" t="s">
+        <v>8</v>
+      </c>
+      <c r="E30" t="s">
+        <v>55</v>
+      </c>
+      <c r="G30" t="str">
+        <f t="shared" si="0"/>
+        <v>Olivier Dor\'e                  \\</v>
+      </c>
+      <c r="I30">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="J30">
+        <f t="shared" si="2"/>
+        <v>18</v>
+      </c>
+      <c r="K30" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">                  </v>
+      </c>
+    </row>
+    <row r="31" spans="2:11">
+      <c r="B31" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D31" t="s">
+        <v>8</v>
+      </c>
+      <c r="G31" t="str">
+        <f t="shared" si="0"/>
+        <v>Josquin Errard                  \\</v>
+      </c>
+      <c r="I31">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="J31">
+        <f t="shared" si="2"/>
+        <v>18</v>
+      </c>
+      <c r="K31" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">                  </v>
+      </c>
+    </row>
+    <row r="32" spans="2:11">
+      <c r="B32" t="s">
+        <v>58</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D32" t="s">
+        <v>8</v>
+      </c>
+      <c r="E32" t="s">
+        <v>60</v>
+      </c>
+      <c r="G32" t="str">
+        <f t="shared" si="0"/>
+        <v>Tom Essinger-Hileman            \\</v>
+      </c>
+      <c r="I32">
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="J28">
+      <c r="J32">
         <f t="shared" si="2"/>
         <v>12</v>
       </c>
-      <c r="K28" t="str">
+      <c r="K32" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve">            </v>
       </c>
     </row>
-    <row r="29" spans="2:11">
-      <c r="B29" t="s">
-        <v>49</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D29" t="s">
-        <v>8</v>
-      </c>
-      <c r="E29" t="s">
-        <v>51</v>
-      </c>
-      <c r="G29" t="str">
-        <f t="shared" si="0"/>
-        <v>Eleonora Di Valentino           \\</v>
-      </c>
-      <c r="I29">
-        <f t="shared" si="1"/>
-        <v>21</v>
-      </c>
-      <c r="J29">
-        <f t="shared" si="2"/>
-        <v>11</v>
-      </c>
-      <c r="K29" t="str">
-        <f t="shared" si="3"/>
-        <v xml:space="preserve">           </v>
-      </c>
-    </row>
-    <row r="30" spans="2:11">
-      <c r="B30" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D30" t="s">
-        <v>8</v>
-      </c>
-      <c r="G30" t="str">
-        <f t="shared" si="0"/>
-        <v>Joy Didier                      \\</v>
-      </c>
-      <c r="I30">
-        <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
-      <c r="J30">
-        <f t="shared" si="2"/>
-        <v>22</v>
-      </c>
-      <c r="K30" t="str">
-        <f t="shared" si="3"/>
-        <v xml:space="preserve">                      </v>
-      </c>
-    </row>
-    <row r="31" spans="2:11">
-      <c r="B31" t="s">
-        <v>54</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>317</v>
-      </c>
-      <c r="D31" t="s">
-        <v>8</v>
-      </c>
-      <c r="E31" t="s">
-        <v>55</v>
-      </c>
-      <c r="G31" t="str">
-        <f t="shared" si="0"/>
-        <v>Olivier Dor\'e                  \\</v>
-      </c>
-      <c r="I31">
+    <row r="33" spans="2:11">
+      <c r="B33" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D33" t="s">
+        <v>8</v>
+      </c>
+      <c r="G33" t="str">
+        <f t="shared" si="0"/>
+        <v>Stephen Feeney                  \\</v>
+      </c>
+      <c r="I33">
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="J31">
+      <c r="J33">
         <f t="shared" si="2"/>
         <v>18</v>
       </c>
-      <c r="K31" t="str">
+      <c r="K33" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve">                  </v>
       </c>
     </row>
-    <row r="32" spans="2:11">
-      <c r="B32" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D32" t="s">
-        <v>8</v>
-      </c>
-      <c r="G32" t="str">
-        <f t="shared" si="0"/>
-        <v>Josquin Errard                  \\</v>
-      </c>
-      <c r="I32">
-        <f t="shared" si="1"/>
-        <v>14</v>
-      </c>
-      <c r="J32">
-        <f t="shared" si="2"/>
-        <v>18</v>
-      </c>
-      <c r="K32" t="str">
-        <f t="shared" si="3"/>
-        <v xml:space="preserve">                  </v>
-      </c>
-    </row>
-    <row r="33" spans="2:11">
-      <c r="B33" t="s">
-        <v>58</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="D33" t="s">
-        <v>8</v>
-      </c>
-      <c r="E33" t="s">
-        <v>60</v>
-      </c>
-      <c r="G33" t="str">
-        <f t="shared" si="0"/>
-        <v>Tom Essinger-Hileman            \\</v>
-      </c>
-      <c r="I33">
-        <f t="shared" si="1"/>
-        <v>20</v>
-      </c>
-      <c r="J33">
-        <f t="shared" si="2"/>
-        <v>12</v>
-      </c>
-      <c r="K33" t="str">
-        <f t="shared" si="3"/>
-        <v xml:space="preserve">            </v>
-      </c>
-    </row>
     <row r="34" spans="2:11">
-      <c r="B34" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>62</v>
+      <c r="B34" t="s">
+        <v>305</v>
+      </c>
+      <c r="C34" t="s">
+        <v>306</v>
       </c>
       <c r="D34" t="s">
         <v>8</v>
       </c>
+      <c r="E34" t="s">
+        <v>290</v>
+      </c>
       <c r="G34" t="str">
         <f t="shared" si="0"/>
-        <v>Stephen Feeney                  \\</v>
+        <v>Jeffrey Filippini               \\</v>
       </c>
       <c r="I34">
         <f t="shared" si="1"/>
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="J34">
         <f t="shared" si="2"/>
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="K34" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">                  </v>
+        <v xml:space="preserve">               </v>
       </c>
     </row>
     <row r="35" spans="2:11">
       <c r="B35" t="s">
-        <v>308</v>
-      </c>
-      <c r="C35" t="s">
-        <v>309</v>
+        <v>63</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>64</v>
       </c>
       <c r="D35" t="s">
         <v>8</v>
       </c>
       <c r="E35" t="s">
-        <v>293</v>
+        <v>65</v>
       </c>
       <c r="G35" t="str">
         <f t="shared" si="0"/>
-        <v>Jeffrey Filippini               \\</v>
+        <v>Laura Fissel                    \\</v>
       </c>
       <c r="I35">
         <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="J35">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="K35" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">                    </v>
+      </c>
+    </row>
+    <row r="36" spans="2:11">
+      <c r="B36" t="s">
+        <v>66</v>
+      </c>
+      <c r="C36" t="s">
+        <v>67</v>
+      </c>
+      <c r="D36" t="s">
+        <v>8</v>
+      </c>
+      <c r="E36" t="s">
+        <v>68</v>
+      </c>
+      <c r="G36" t="str">
+        <f t="shared" si="0"/>
+        <v>Raphael Flauger                 \\</v>
+      </c>
+      <c r="I36">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="J36">
+        <f t="shared" si="2"/>
         <v>17</v>
       </c>
-      <c r="J35">
-        <f t="shared" si="2"/>
-        <v>15</v>
-      </c>
-      <c r="K35" t="str">
-        <f t="shared" si="3"/>
-        <v xml:space="preserve">               </v>
-      </c>
-    </row>
-    <row r="36" spans="2:11">
-      <c r="B36" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D36" t="s">
-        <v>8</v>
-      </c>
-      <c r="G36" t="str">
-        <f t="shared" si="0"/>
-        <v>Jeff Fillippini                 \\</v>
-      </c>
-      <c r="I36">
-        <f t="shared" si="1"/>
-        <v>15</v>
-      </c>
-      <c r="J36">
-        <f t="shared" si="2"/>
-        <v>17</v>
-      </c>
       <c r="K36" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve">                 </v>
       </c>
     </row>
     <row r="37" spans="2:11">
-      <c r="B37" t="s">
-        <v>65</v>
+      <c r="B37" s="1" t="s">
+        <v>69</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="D37" t="s">
         <v>8</v>
       </c>
-      <c r="E37" t="s">
-        <v>67</v>
-      </c>
       <c r="G37" t="str">
         <f t="shared" si="0"/>
-        <v>Laura Fissel                    \\</v>
+        <v>Vera Gluscevic                  \\</v>
       </c>
       <c r="I37">
         <f t="shared" si="1"/>
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="J37">
         <f t="shared" si="2"/>
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="K37" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">                    </v>
+        <v xml:space="preserve">                  </v>
       </c>
     </row>
     <row r="38" spans="2:11">
-      <c r="B38" t="s">
-        <v>68</v>
-      </c>
-      <c r="C38" t="s">
-        <v>69</v>
+      <c r="B38" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>72</v>
       </c>
       <c r="D38" t="s">
         <v>8</v>
       </c>
-      <c r="E38" t="s">
-        <v>70</v>
-      </c>
       <c r="G38" t="str">
         <f t="shared" si="0"/>
-        <v>Raphael Flauger                 \\</v>
+        <v>Kris Gorski                     \\</v>
       </c>
       <c r="I38">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="J38">
         <f t="shared" si="2"/>
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="K38" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">                 </v>
+        <v xml:space="preserve">                     </v>
       </c>
     </row>
     <row r="39" spans="2:11">
       <c r="B39" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D39" t="s">
         <v>8</v>
       </c>
       <c r="G39" t="str">
         <f t="shared" si="0"/>
-        <v>Vera Gluscevic                  \\</v>
+        <v>Dan Green                       \\</v>
       </c>
       <c r="I39">
         <f t="shared" si="1"/>
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="J39">
         <f t="shared" si="2"/>
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="K39" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">                  </v>
+        <v xml:space="preserve">                       </v>
       </c>
     </row>
     <row r="40" spans="2:11">
       <c r="B40" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D40" t="s">
         <v>8</v>
       </c>
       <c r="G40" t="str">
         <f t="shared" si="0"/>
-        <v>Kris Gorski                     \\</v>
+        <v>Brandon Hensley                 \\</v>
       </c>
       <c r="I40">
         <f t="shared" si="1"/>
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="J40">
         <f t="shared" si="2"/>
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="K40" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">                     </v>
+        <v xml:space="preserve">                 </v>
       </c>
     </row>
     <row r="41" spans="2:11">
-      <c r="B41" s="1" t="s">
-        <v>75</v>
+      <c r="B41" t="s">
+        <v>77</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D41" t="s">
         <v>8</v>
       </c>
+      <c r="E41" t="s">
+        <v>79</v>
+      </c>
       <c r="G41" t="str">
         <f t="shared" si="0"/>
-        <v>Dan Green                       \\</v>
+        <v>Diego Herranz                   \\</v>
       </c>
       <c r="I41">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="J41">
         <f t="shared" si="2"/>
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="K41" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">                       </v>
+        <v xml:space="preserve">                   </v>
       </c>
     </row>
     <row r="42" spans="2:11">
       <c r="B42" s="1" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="D42" t="s">
         <v>8</v>
       </c>
       <c r="G42" t="str">
         <f t="shared" si="0"/>
-        <v>Brandon Hensley                 \\</v>
+        <v>Colin Hill                      \\</v>
       </c>
       <c r="I42">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="J42">
         <f t="shared" si="2"/>
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="K42" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">                 </v>
+        <v xml:space="preserve">                      </v>
       </c>
     </row>
     <row r="43" spans="2:11">
       <c r="B43" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="D43" t="s">
         <v>8</v>
       </c>
       <c r="E43" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="G43" t="str">
         <f t="shared" si="0"/>
-        <v>Diego Herranz                   \\</v>
+        <v>Eric Hivon                      \\</v>
       </c>
       <c r="I43">
         <f t="shared" si="1"/>
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="J43">
         <f t="shared" si="2"/>
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="K43" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">                   </v>
+        <v xml:space="preserve">                      </v>
       </c>
     </row>
     <row r="44" spans="2:11">
-      <c r="B44" s="1" t="s">
-        <v>82</v>
+      <c r="B44" t="s">
+        <v>85</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="D44" t="s">
         <v>8</v>
       </c>
+      <c r="E44" t="s">
+        <v>87</v>
+      </c>
       <c r="G44" t="str">
         <f t="shared" si="0"/>
-        <v>Colin Hill                      \\</v>
+        <v>Johannes Hubmayr                \\</v>
       </c>
       <c r="I44">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="J44">
         <f t="shared" si="2"/>
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="K44" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">                      </v>
+        <v xml:space="preserve">                </v>
       </c>
     </row>
     <row r="45" spans="2:11">
       <c r="B45" t="s">
-        <v>84</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>85</v>
+        <v>88</v>
+      </c>
+      <c r="C45" t="s">
+        <v>89</v>
       </c>
       <c r="D45" t="s">
         <v>8</v>
       </c>
       <c r="E45" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="G45" t="str">
         <f t="shared" si="0"/>
-        <v>Eric Hivon                      \\</v>
+        <v>Brad Johnson                    \\</v>
       </c>
       <c r="I45">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="J45">
         <f t="shared" si="2"/>
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K45" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">                      </v>
+        <v xml:space="preserve">                    </v>
       </c>
     </row>
     <row r="46" spans="2:11">
       <c r="B46" t="s">
-        <v>87</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>88</v>
+        <v>91</v>
+      </c>
+      <c r="C46" t="s">
+        <v>92</v>
       </c>
       <c r="D46" t="s">
         <v>8</v>
       </c>
       <c r="E46" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="G46" t="str">
         <f t="shared" si="0"/>
-        <v>Johannes Hubmayr                \\</v>
+        <v>William Jones                   \\</v>
       </c>
       <c r="I46">
         <f t="shared" si="1"/>
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="J46">
         <f t="shared" si="2"/>
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="K46" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">                </v>
+        <v xml:space="preserve">                   </v>
       </c>
     </row>
     <row r="47" spans="2:11">
       <c r="B47" t="s">
-        <v>90</v>
-      </c>
-      <c r="C47" t="s">
-        <v>91</v>
+        <v>94</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>92</v>
       </c>
       <c r="D47" t="s">
         <v>8</v>
       </c>
       <c r="E47" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="G47" t="str">
         <f t="shared" si="0"/>
-        <v>Brad Johnson                    \\</v>
+        <v>Terry Jones                     \\</v>
       </c>
       <c r="I47">
         <f t="shared" si="1"/>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J47">
         <f t="shared" si="2"/>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K47" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">                    </v>
+        <v xml:space="preserve">                     </v>
       </c>
     </row>
     <row r="48" spans="2:11">
-      <c r="B48" t="s">
-        <v>93</v>
-      </c>
-      <c r="C48" t="s">
-        <v>94</v>
+      <c r="B48" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>96</v>
       </c>
       <c r="D48" t="s">
         <v>8</v>
       </c>
-      <c r="E48" t="s">
-        <v>95</v>
-      </c>
       <c r="G48" t="str">
         <f t="shared" si="0"/>
-        <v>William Jones                   \\</v>
+        <v>Lloyd Knox                      \\</v>
       </c>
       <c r="I48">
         <f t="shared" si="1"/>
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="J48">
         <f t="shared" si="2"/>
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="K48" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">                   </v>
+        <v xml:space="preserve">                      </v>
       </c>
     </row>
     <row r="49" spans="2:11">
-      <c r="B49" t="s">
-        <v>96</v>
+      <c r="B49" s="1" t="s">
+        <v>97</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="D49" t="s">
         <v>8</v>
       </c>
-      <c r="E49" t="s">
-        <v>97</v>
-      </c>
       <c r="G49" t="str">
         <f t="shared" si="0"/>
-        <v>Terry Jones                     \\</v>
+        <v>Al Kogut                        \\</v>
       </c>
       <c r="I49">
         <f t="shared" si="1"/>
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="J49">
         <f t="shared" si="2"/>
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="K49" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">                     </v>
+        <v xml:space="preserve">                        </v>
       </c>
     </row>
     <row r="50" spans="2:11">
       <c r="B50" s="1" t="s">
-        <v>320</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
+      </c>
+      <c r="C50" t="s">
+        <v>100</v>
       </c>
       <c r="D50" t="s">
         <v>8</v>
       </c>
       <c r="G50" t="str">
         <f t="shared" si="0"/>
-        <v>Lloyd Knox                      \\</v>
+        <v>Charles Lawrence                \\</v>
       </c>
       <c r="I50">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="J50">
         <f t="shared" si="2"/>
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="K50" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">                      </v>
+        <v xml:space="preserve">                </v>
       </c>
     </row>
     <row r="51" spans="2:11">
       <c r="B51" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
+      </c>
+      <c r="C51" t="s">
+        <v>102</v>
       </c>
       <c r="D51" t="s">
         <v>8</v>
       </c>
       <c r="G51" t="str">
         <f t="shared" si="0"/>
-        <v>Al Kogut                        \\</v>
+        <v>Alex Lazarian                   \\</v>
       </c>
       <c r="I51">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="J51">
         <f t="shared" si="2"/>
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="K51" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">                        </v>
+        <v xml:space="preserve">                   </v>
       </c>
     </row>
     <row r="52" spans="2:11">
       <c r="B52" s="1" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C52" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="D52" t="s">
         <v>8</v>
       </c>
       <c r="G52" t="str">
         <f t="shared" si="0"/>
-        <v>Charles Lawrence                \\</v>
+        <v>Zack Li                         \\</v>
       </c>
       <c r="I52">
         <f t="shared" si="1"/>
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="J52">
         <f t="shared" si="2"/>
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="K52" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">                </v>
+        <v xml:space="preserve">                         </v>
       </c>
     </row>
     <row r="53" spans="2:11">
-      <c r="B53" s="1" t="s">
-        <v>103</v>
+      <c r="B53" t="s">
+        <v>297</v>
       </c>
       <c r="C53" t="s">
-        <v>104</v>
+        <v>316</v>
       </c>
       <c r="D53" t="s">
         <v>8</v>
       </c>
+      <c r="E53" t="s">
+        <v>285</v>
+      </c>
       <c r="G53" t="str">
         <f t="shared" si="0"/>
-        <v>Alex Lazarian                   \\</v>
+        <v>Marcos L\'{o}pez-Caniego        \\</v>
       </c>
       <c r="I53">
         <f t="shared" si="1"/>
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="J53">
         <f t="shared" si="2"/>
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="K53" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">                   </v>
+        <v xml:space="preserve">        </v>
       </c>
     </row>
     <row r="54" spans="2:11">
       <c r="B54" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C54" s="1" t="s">
         <v>106</v>
       </c>
       <c r="D54" t="s">
@@ -2768,151 +2768,151 @@
       </c>
       <c r="G54" t="str">
         <f t="shared" si="0"/>
-        <v>Zack Li                         \\</v>
+        <v>Mathew Madhavacheril            \\</v>
       </c>
       <c r="I54">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="J54">
         <f t="shared" si="2"/>
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="K54" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">                         </v>
+        <v xml:space="preserve">            </v>
       </c>
     </row>
     <row r="55" spans="2:11">
-      <c r="B55" t="s">
-        <v>300</v>
+      <c r="B55" s="1" t="s">
+        <v>107</v>
       </c>
       <c r="C55" t="s">
-        <v>319</v>
+        <v>108</v>
       </c>
       <c r="D55" t="s">
         <v>8</v>
       </c>
-      <c r="E55" t="s">
-        <v>288</v>
-      </c>
       <c r="G55" t="str">
         <f t="shared" si="0"/>
-        <v>Marcos L\'{o}pez-Caniego        \\</v>
+        <v>Jean-Baptiste Melin             \\</v>
       </c>
       <c r="I55">
         <f t="shared" si="1"/>
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="J55">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="K55" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">        </v>
+        <v xml:space="preserve">             </v>
       </c>
     </row>
     <row r="56" spans="2:11">
-      <c r="B56" s="1" t="s">
-        <v>107</v>
+      <c r="B56" t="s">
+        <v>109</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="D56" t="s">
         <v>8</v>
       </c>
+      <c r="E56" t="s">
+        <v>111</v>
+      </c>
       <c r="G56" t="str">
         <f t="shared" si="0"/>
-        <v>Mathew Madhavacheril            \\</v>
+        <v>Mattia Negrello                 \\</v>
       </c>
       <c r="I56">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="J56">
         <f t="shared" si="2"/>
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="K56" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">            </v>
+        <v xml:space="preserve">                 </v>
       </c>
     </row>
     <row r="57" spans="2:11">
-      <c r="B57" s="1" t="s">
-        <v>109</v>
+      <c r="B57" t="s">
+        <v>112</v>
       </c>
       <c r="C57" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="D57" t="s">
         <v>8</v>
       </c>
+      <c r="E57" t="s">
+        <v>114</v>
+      </c>
       <c r="G57" t="str">
         <f t="shared" si="0"/>
-        <v>Jean-Baptiste Melin             \\</v>
+        <v>Giles Novak                     \\</v>
       </c>
       <c r="I57">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="J57">
         <f t="shared" si="2"/>
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="K57" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">             </v>
+        <v xml:space="preserve">                     </v>
       </c>
     </row>
     <row r="58" spans="2:11">
       <c r="B58" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="D58" t="s">
         <v>8</v>
       </c>
       <c r="E58" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="G58" t="str">
         <f t="shared" si="0"/>
-        <v>Mattia Negrello                 \\</v>
+        <v>Roger O'Brient                  \\</v>
       </c>
       <c r="I58">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J58">
         <f t="shared" si="2"/>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K58" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">                 </v>
+        <v xml:space="preserve">                  </v>
       </c>
     </row>
     <row r="59" spans="2:11">
-      <c r="B59" t="s">
-        <v>114</v>
-      </c>
-      <c r="C59" t="s">
-        <v>115</v>
+      <c r="B59" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>119</v>
       </c>
       <c r="D59" t="s">
         <v>8</v>
       </c>
-      <c r="E59" t="s">
-        <v>116</v>
-      </c>
       <c r="G59" t="str">
         <f t="shared" si="0"/>
-        <v>Giles Novak                     \\</v>
+        <v>Chris Paine                     \\</v>
       </c>
       <c r="I59">
         <f t="shared" si="1"/>
@@ -2928,318 +2928,315 @@
       </c>
     </row>
     <row r="60" spans="2:11">
-      <c r="B60" t="s">
-        <v>117</v>
+      <c r="B60" s="1" t="s">
+        <v>120</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="D60" t="s">
         <v>8</v>
       </c>
-      <c r="E60" t="s">
-        <v>119</v>
-      </c>
       <c r="G60" t="str">
         <f t="shared" si="0"/>
-        <v>Roger O'Brient                  \\</v>
+        <v>Tim Pearson                     \\</v>
       </c>
       <c r="I60">
         <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="J60">
+        <f t="shared" si="2"/>
+        <v>21</v>
+      </c>
+      <c r="K60" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">                     </v>
+      </c>
+    </row>
+    <row r="61" spans="2:11">
+      <c r="B61" t="s">
+        <v>122</v>
+      </c>
+      <c r="C61" t="s">
+        <v>123</v>
+      </c>
+      <c r="D61" t="s">
+        <v>8</v>
+      </c>
+      <c r="E61" t="s">
+        <v>124</v>
+      </c>
+      <c r="G61" t="str">
+        <f t="shared" si="0"/>
+        <v>Levon Pogosian                  \\</v>
+      </c>
+      <c r="I61">
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="J60">
+      <c r="J61">
         <f t="shared" si="2"/>
         <v>18</v>
       </c>
-      <c r="K60" t="str">
+      <c r="K61" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve">                  </v>
-      </c>
-    </row>
-    <row r="61" spans="2:11">
-      <c r="B61" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="D61" t="s">
-        <v>8</v>
-      </c>
-      <c r="G61" t="str">
-        <f t="shared" si="0"/>
-        <v>Chris Paine                     \\</v>
-      </c>
-      <c r="I61">
-        <f t="shared" si="1"/>
-        <v>11</v>
-      </c>
-      <c r="J61">
-        <f t="shared" si="2"/>
-        <v>21</v>
-      </c>
-      <c r="K61" t="str">
-        <f t="shared" si="3"/>
-        <v xml:space="preserve">                     </v>
       </c>
     </row>
     <row r="62" spans="2:11">
       <c r="B62" s="1" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="D62" t="s">
         <v>8</v>
       </c>
       <c r="G62" t="str">
         <f t="shared" si="0"/>
-        <v>Tim Pearson                     \\</v>
+        <v>Clem Pryke                      \\</v>
       </c>
       <c r="I62">
         <f t="shared" si="1"/>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J62">
         <f t="shared" si="2"/>
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="K62" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">                     </v>
+        <v xml:space="preserve">                      </v>
       </c>
     </row>
     <row r="63" spans="2:11">
       <c r="B63" t="s">
-        <v>124</v>
-      </c>
-      <c r="C63" t="s">
-        <v>125</v>
+        <v>127</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>128</v>
       </c>
       <c r="D63" t="s">
         <v>8</v>
       </c>
       <c r="E63" t="s">
-        <v>126</v>
+        <v>51</v>
       </c>
       <c r="G63" t="str">
         <f t="shared" si="0"/>
-        <v>Levon Pogosian                  \\</v>
+        <v>Mathieu Remazeilles             \\</v>
       </c>
       <c r="I63">
         <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="J63">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
+      <c r="K63" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">             </v>
+      </c>
+    </row>
+    <row r="64" spans="2:11">
+      <c r="B64" t="s">
+        <v>129</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D64" t="s">
+        <v>8</v>
+      </c>
+      <c r="E64" t="s">
+        <v>55</v>
+      </c>
+      <c r="G64" t="str">
+        <f t="shared" si="0"/>
+        <v>Graca Rocha                     \\</v>
+      </c>
+      <c r="I64">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="J64">
+        <f t="shared" si="2"/>
+        <v>21</v>
+      </c>
+      <c r="K64" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">                     </v>
+      </c>
+    </row>
+    <row r="65" spans="2:11">
+      <c r="B65" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D65" t="s">
+        <v>8</v>
+      </c>
+      <c r="G65" t="str">
+        <f t="shared" si="0"/>
+        <v>Marcel Schmittfull              \\</v>
+      </c>
+      <c r="I65">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="J65">
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
-      <c r="J63">
-        <f t="shared" si="2"/>
-        <v>18</v>
-      </c>
-      <c r="K63" t="str">
-        <f t="shared" si="3"/>
-        <v xml:space="preserve">                  </v>
-      </c>
-    </row>
-    <row r="64" spans="2:11">
-      <c r="B64" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="C64" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="D64" t="s">
-        <v>8</v>
-      </c>
-      <c r="G64" t="str">
-        <f t="shared" si="0"/>
-        <v>Clem Pryke                      \\</v>
-      </c>
-      <c r="I64">
-        <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
-      <c r="J64">
-        <f t="shared" si="2"/>
-        <v>22</v>
-      </c>
-      <c r="K64" t="str">
-        <f t="shared" si="3"/>
-        <v xml:space="preserve">                      </v>
-      </c>
-    </row>
-    <row r="65" spans="2:11">
-      <c r="B65" t="s">
-        <v>129</v>
-      </c>
-      <c r="C65" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="D65" t="s">
-        <v>8</v>
-      </c>
-      <c r="E65" t="s">
-        <v>51</v>
-      </c>
-      <c r="G65" t="str">
-        <f t="shared" si="0"/>
-        <v>Mathieu Remazeilles             \\</v>
-      </c>
-      <c r="I65">
-        <f t="shared" si="1"/>
-        <v>19</v>
-      </c>
-      <c r="J65">
-        <f t="shared" si="2"/>
-        <v>13</v>
-      </c>
       <c r="K65" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">             </v>
+        <v xml:space="preserve">              </v>
       </c>
     </row>
     <row r="66" spans="2:11">
       <c r="B66" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D66" t="s">
         <v>8</v>
       </c>
       <c r="E66" t="s">
-        <v>55</v>
+        <v>135</v>
       </c>
       <c r="G66" t="str">
         <f t="shared" si="0"/>
-        <v>Graca Rocha                     \\</v>
+        <v>Ian Stephens                    \\</v>
       </c>
       <c r="I66">
         <f t="shared" si="1"/>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J66">
         <f t="shared" si="2"/>
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K66" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">                     </v>
+        <v xml:space="preserve">                    </v>
       </c>
     </row>
     <row r="67" spans="2:11">
       <c r="B67" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="C67" s="1" t="s">
-        <v>134</v>
+        <v>136</v>
+      </c>
+      <c r="C67" t="s">
+        <v>137</v>
       </c>
       <c r="D67" t="s">
         <v>8</v>
       </c>
       <c r="G67" t="str">
         <f t="shared" si="0"/>
-        <v>Marcel Schmittfull              \\</v>
+        <v>Brian Sutin                     \\</v>
       </c>
       <c r="I67">
         <f t="shared" si="1"/>
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="J67">
         <f t="shared" si="2"/>
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="K67" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">              </v>
+        <v xml:space="preserve">                     </v>
       </c>
     </row>
     <row r="68" spans="2:11">
       <c r="B68" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="D68" t="s">
         <v>8</v>
       </c>
       <c r="E68" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="G68" t="str">
         <f t="shared" si="0"/>
-        <v>Ian Stephens                    \\</v>
+        <v>Maurizio Tomasi                 \\</v>
       </c>
       <c r="I68">
         <f t="shared" si="1"/>
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="J68">
         <f t="shared" si="2"/>
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="K68" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">                    </v>
+        <v xml:space="preserve">                 </v>
       </c>
     </row>
     <row r="69" spans="2:11">
       <c r="B69" s="1" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="C69" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="D69" t="s">
         <v>8</v>
       </c>
       <c r="G69" t="str">
         <f t="shared" si="0"/>
-        <v>Brian Sutin                     \\</v>
+        <v>Amy Trangsrud                   \\</v>
       </c>
       <c r="I69">
         <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="J69">
+        <f t="shared" si="2"/>
+        <v>19</v>
+      </c>
+      <c r="K69" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">                   </v>
+      </c>
+    </row>
+    <row r="70" spans="2:11">
+      <c r="B70" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="C70" t="s">
+        <v>310</v>
+      </c>
+      <c r="D70" t="s">
+        <v>8</v>
+      </c>
+      <c r="G70" t="str">
+        <f t="shared" si="0"/>
+        <v>Alexander van Engelen           \\</v>
+      </c>
+      <c r="I70">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
+      <c r="J70">
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
-      <c r="J69">
-        <f t="shared" si="2"/>
-        <v>21</v>
-      </c>
-      <c r="K69" t="str">
-        <f t="shared" si="3"/>
-        <v xml:space="preserve">                     </v>
-      </c>
-    </row>
-    <row r="70" spans="2:11">
-      <c r="B70" t="s">
-        <v>140</v>
-      </c>
-      <c r="C70" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="D70" t="s">
-        <v>8</v>
-      </c>
-      <c r="E70" t="s">
-        <v>142</v>
-      </c>
-      <c r="G70" t="str">
-        <f t="shared" si="0"/>
-        <v>Maurizio Tomasi                 \\</v>
-      </c>
-      <c r="I70">
-        <f t="shared" si="1"/>
-        <v>15</v>
-      </c>
-      <c r="J70">
-        <f t="shared" si="2"/>
-        <v>17</v>
-      </c>
       <c r="K70" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">                 </v>
+        <v xml:space="preserve">           </v>
       </c>
     </row>
     <row r="71" spans="2:11">
@@ -3254,1109 +3251,1115 @@
       </c>
       <c r="G71" t="str">
         <f t="shared" si="0"/>
-        <v>Amy Trangsrud                   \\</v>
+        <v>Flavien Vansyngel               \\</v>
       </c>
       <c r="I71">
         <f t="shared" si="1"/>
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="J71">
         <f t="shared" si="2"/>
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="K71" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">                   </v>
+        <v xml:space="preserve">               </v>
       </c>
     </row>
     <row r="72" spans="2:11">
-      <c r="B72" s="1" t="s">
-        <v>314</v>
-      </c>
-      <c r="C72" t="s">
-        <v>313</v>
+      <c r="B72" t="s">
+        <v>145</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>146</v>
       </c>
       <c r="D72" t="s">
         <v>8</v>
       </c>
+      <c r="E72" t="s">
+        <v>147</v>
+      </c>
       <c r="G72" t="str">
         <f t="shared" si="0"/>
-        <v>Alexander van Engelen           \\</v>
+        <v>Qi Wen                          \\</v>
       </c>
       <c r="I72">
         <f t="shared" si="1"/>
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="J72">
         <f t="shared" si="2"/>
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="K72" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">           </v>
+        <v xml:space="preserve">                          </v>
       </c>
     </row>
     <row r="73" spans="2:11">
-      <c r="B73" s="1" t="s">
-        <v>145</v>
+      <c r="B73" s="3" t="s">
+        <v>150</v>
       </c>
       <c r="C73" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="D73" t="s">
         <v>8</v>
       </c>
       <c r="G73" t="str">
-        <f t="shared" si="0"/>
-        <v>Flavien Vansyngel               \\</v>
+        <f t="shared" ref="G73:G137" si="4">CONCATENATE(B73," ",C73,K73,"\\")</f>
+        <v>Siyao Xu                        \\</v>
       </c>
       <c r="I73">
-        <f t="shared" si="1"/>
-        <v>17</v>
+        <f t="shared" ref="I73:I137" si="5">LEN(B73) + LEN(C73) +1</f>
+        <v>8</v>
       </c>
       <c r="J73">
-        <f t="shared" si="2"/>
-        <v>15</v>
+        <f t="shared" ref="J73:J137" si="6">IF(I73&lt;30,(32-I73),3)</f>
+        <v>24</v>
       </c>
       <c r="K73" t="str">
-        <f t="shared" si="3"/>
-        <v xml:space="preserve">               </v>
+        <f t="shared" ref="K73:K137" si="7">REPT(" ",J73)</f>
+        <v xml:space="preserve">                        </v>
       </c>
     </row>
     <row r="74" spans="2:11">
-      <c r="B74" t="s">
-        <v>147</v>
-      </c>
-      <c r="C74" s="1" t="s">
-        <v>148</v>
+      <c r="B74" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="C74" t="s">
+        <v>153</v>
       </c>
       <c r="D74" t="s">
         <v>8</v>
       </c>
-      <c r="E74" t="s">
-        <v>149</v>
-      </c>
       <c r="G74" t="str">
-        <f t="shared" si="0"/>
-        <v>Qi Wen                          \\</v>
+        <f t="shared" si="4"/>
+        <v>Karl Young                      \\</v>
       </c>
       <c r="I74">
-        <f t="shared" si="1"/>
-        <v>6</v>
+        <f t="shared" si="5"/>
+        <v>10</v>
       </c>
       <c r="J74">
-        <f t="shared" si="2"/>
-        <v>26</v>
+        <f t="shared" si="6"/>
+        <v>22</v>
       </c>
       <c r="K74" t="str">
-        <f t="shared" si="3"/>
-        <v xml:space="preserve">                          </v>
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">                      </v>
       </c>
     </row>
     <row r="75" spans="2:11">
       <c r="B75" s="3" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="C75" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="D75" t="s">
         <v>8</v>
       </c>
       <c r="G75" t="str">
-        <f t="shared" ref="G75:G138" si="4">CONCATENATE(B75," ",C75,K75,"\\")</f>
-        <v>Siyao Xu                        \\</v>
+        <f t="shared" si="4"/>
+        <v>Andrea Zonca                    \\</v>
       </c>
       <c r="I75">
-        <f t="shared" ref="I75:I138" si="5">LEN(B75) + LEN(C75) +1</f>
-        <v>8</v>
+        <f t="shared" si="5"/>
+        <v>12</v>
       </c>
       <c r="J75">
-        <f t="shared" ref="J75:J138" si="6">IF(I75&lt;30,(32-I75),3)</f>
-        <v>24</v>
+        <f t="shared" si="6"/>
+        <v>20</v>
       </c>
       <c r="K75" t="str">
-        <f t="shared" ref="K75:K138" si="7">REPT(" ",J75)</f>
-        <v xml:space="preserve">                        </v>
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">                    </v>
       </c>
     </row>
     <row r="76" spans="2:11">
-      <c r="B76" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="C76" t="s">
-        <v>155</v>
-      </c>
-      <c r="D76" t="s">
-        <v>8</v>
-      </c>
+      <c r="B76" s="3"/>
+      <c r="C76"/>
       <c r="G76" t="str">
         <f t="shared" si="4"/>
-        <v>Karl Young                      \\</v>
+        <v xml:space="preserve">                                \\</v>
       </c>
       <c r="I76">
         <f t="shared" si="5"/>
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="J76">
         <f t="shared" si="6"/>
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="K76" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">                      </v>
+        <v xml:space="preserve">                               </v>
       </c>
     </row>
     <row r="77" spans="2:11">
-      <c r="B77" s="3" t="s">
+      <c r="B77" s="3"/>
+      <c r="C77"/>
+      <c r="G77" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">                                \\</v>
+      </c>
+      <c r="I77">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="J77">
+        <f t="shared" si="6"/>
+        <v>31</v>
+      </c>
+      <c r="K77" t="str">
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">                               </v>
+      </c>
+    </row>
+    <row r="78" spans="2:11">
+      <c r="B78" t="s">
         <v>156</v>
       </c>
-      <c r="C77" t="s">
+      <c r="C78" t="s">
         <v>157</v>
       </c>
-      <c r="D77" t="s">
-        <v>8</v>
-      </c>
-      <c r="G77" t="str">
-        <f t="shared" si="4"/>
-        <v>Andrea Zonca                    \\</v>
-      </c>
-      <c r="I77">
-        <f t="shared" si="5"/>
-        <v>12</v>
-      </c>
-      <c r="J77">
-        <f t="shared" si="6"/>
-        <v>20</v>
-      </c>
-      <c r="K77" t="str">
-        <f t="shared" si="7"/>
-        <v xml:space="preserve">                    </v>
-      </c>
-    </row>
-    <row r="78" spans="2:11">
-      <c r="B78" s="3"/>
-      <c r="C78"/>
+      <c r="D78" t="s">
+        <v>158</v>
+      </c>
+      <c r="E78" t="s">
+        <v>159</v>
+      </c>
       <c r="G78" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">                                \\</v>
+        <v>Zeeshan Ahmed                   \\</v>
       </c>
       <c r="I78">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="J78">
         <f t="shared" si="6"/>
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="K78" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">                               </v>
+        <v xml:space="preserve">                   </v>
       </c>
     </row>
     <row r="79" spans="2:11">
-      <c r="B79" s="3"/>
-      <c r="C79"/>
+      <c r="B79" t="s">
+        <v>160</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="D79" t="s">
+        <v>158</v>
+      </c>
+      <c r="E79" t="s">
+        <v>162</v>
+      </c>
       <c r="G79" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">                                \\</v>
+        <v>Jason Austermann                \\</v>
       </c>
       <c r="I79">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="J79">
         <f t="shared" si="6"/>
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="K79" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">                               </v>
+        <v xml:space="preserve">                </v>
       </c>
     </row>
     <row r="80" spans="2:11">
       <c r="B80" t="s">
+        <v>163</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="D80" t="s">
         <v>158</v>
       </c>
-      <c r="C80" t="s">
-        <v>159</v>
-      </c>
-      <c r="D80" t="s">
-        <v>160</v>
-      </c>
       <c r="E80" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="G80" t="str">
         <f t="shared" si="4"/>
-        <v>Zeeshan Ahmed                   \\</v>
+        <v>Darcy Barron                    \\</v>
       </c>
       <c r="I80">
         <f t="shared" si="5"/>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J80">
         <f t="shared" si="6"/>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="K80" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">                   </v>
+        <v xml:space="preserve">                    </v>
       </c>
     </row>
     <row r="81" spans="2:11">
       <c r="B81" t="s">
-        <v>162</v>
-      </c>
-      <c r="C81" s="1" t="s">
-        <v>163</v>
+        <v>166</v>
+      </c>
+      <c r="C81" t="s">
+        <v>167</v>
       </c>
       <c r="D81" t="s">
-        <v>160</v>
-      </c>
-      <c r="E81" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="G81" t="str">
         <f t="shared" si="4"/>
-        <v>Jason Austermann                \\</v>
+        <v>Karim Benabed                   \\</v>
       </c>
       <c r="I81">
         <f t="shared" si="5"/>
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="J81">
         <f t="shared" si="6"/>
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="K81" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">                </v>
+        <v xml:space="preserve">                   </v>
       </c>
     </row>
     <row r="82" spans="2:11">
       <c r="B82" t="s">
-        <v>165</v>
-      </c>
-      <c r="C82" s="1" t="s">
-        <v>166</v>
+        <v>168</v>
+      </c>
+      <c r="C82" t="s">
+        <v>169</v>
       </c>
       <c r="D82" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E82" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="G82" t="str">
         <f t="shared" si="4"/>
-        <v>Darcy Barron                    \\</v>
+        <v>Federico Bianchini              \\</v>
       </c>
       <c r="I82">
         <f t="shared" si="5"/>
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="J82">
         <f t="shared" si="6"/>
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="K82" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">                    </v>
+        <v xml:space="preserve">              </v>
       </c>
     </row>
     <row r="83" spans="2:11">
-      <c r="B83" t="s">
-        <v>168</v>
-      </c>
-      <c r="C83" t="s">
-        <v>169</v>
+      <c r="B83" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>296</v>
       </c>
       <c r="D83" t="s">
-        <v>160</v>
+        <v>158</v>
+      </c>
+      <c r="E83" t="s">
+        <v>284</v>
       </c>
       <c r="G83" t="str">
         <f t="shared" si="4"/>
-        <v>Karim Benabed                   \\</v>
+        <v>Colin Bischoff                  \\</v>
       </c>
       <c r="I83">
         <f t="shared" si="5"/>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="J83">
         <f t="shared" si="6"/>
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K83" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">                   </v>
+        <v xml:space="preserve">                  </v>
       </c>
     </row>
     <row r="84" spans="2:11">
       <c r="B84" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="C84" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="D84" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E84" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="G84" t="str">
         <f t="shared" si="4"/>
-        <v>Federico Bianchini              \\</v>
+        <v>J. Richard Bond                 \\</v>
       </c>
       <c r="I84">
         <f t="shared" si="5"/>
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="J84">
         <f t="shared" si="6"/>
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="K84" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">              </v>
+        <v xml:space="preserve">                 </v>
       </c>
     </row>
     <row r="85" spans="2:11">
       <c r="B85" s="1" t="s">
-        <v>82</v>
+        <v>293</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="D85" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E85" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="G85" t="str">
         <f t="shared" si="4"/>
-        <v>Colin Bischoff                  \\</v>
+        <v>Robert Caldwell                 \\</v>
       </c>
       <c r="I85">
         <f t="shared" si="5"/>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J85">
         <f t="shared" si="6"/>
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K85" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">                  </v>
+        <v xml:space="preserve">                 </v>
       </c>
     </row>
     <row r="86" spans="2:11">
       <c r="B86" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C86" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="D86" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E86" t="s">
-        <v>178</v>
+        <v>135</v>
       </c>
       <c r="G86" t="str">
         <f t="shared" si="4"/>
-        <v>J. Richard Bond                 \\</v>
+        <v>Xingang Chen                    \\</v>
       </c>
       <c r="I86">
         <f t="shared" si="5"/>
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="J86">
         <f t="shared" si="6"/>
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="K86" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">                 </v>
+        <v xml:space="preserve">                    </v>
       </c>
     </row>
     <row r="87" spans="2:11">
-      <c r="B87" s="1" t="s">
-        <v>296</v>
-      </c>
-      <c r="C87" s="1" t="s">
-        <v>297</v>
+      <c r="B87" t="s">
+        <v>179</v>
+      </c>
+      <c r="C87" t="s">
+        <v>180</v>
       </c>
       <c r="D87" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E87" t="s">
-        <v>285</v>
+        <v>181</v>
       </c>
       <c r="G87" t="str">
         <f t="shared" si="4"/>
-        <v>Robert Caldwell                 \\</v>
+        <v>Jens Chluba                     \\</v>
       </c>
       <c r="I87">
         <f t="shared" si="5"/>
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="J87">
         <f t="shared" si="6"/>
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="K87" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">                 </v>
+        <v xml:space="preserve">                     </v>
       </c>
     </row>
     <row r="88" spans="2:11">
       <c r="B88" t="s">
-        <v>179</v>
-      </c>
-      <c r="C88" t="s">
-        <v>180</v>
+        <v>182</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>183</v>
       </c>
       <c r="D88" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E88" t="s">
-        <v>137</v>
+        <v>184</v>
       </c>
       <c r="G88" t="str">
         <f t="shared" si="4"/>
-        <v>Xingang Chen                    \\</v>
+        <v>Francis-Yan Cyr-Racine          \\</v>
       </c>
       <c r="I88">
         <f t="shared" si="5"/>
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="J88">
         <f t="shared" si="6"/>
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="K88" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">                    </v>
+        <v xml:space="preserve">          </v>
       </c>
     </row>
     <row r="89" spans="2:11">
       <c r="B89" t="s">
-        <v>181</v>
-      </c>
-      <c r="C89" t="s">
-        <v>182</v>
+        <v>185</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>186</v>
       </c>
       <c r="D89" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E89" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="G89" t="str">
         <f t="shared" si="4"/>
-        <v>Jens Chluba                     \\</v>
+        <v>Tijmen de Haan                  \\</v>
       </c>
       <c r="I89">
         <f t="shared" si="5"/>
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="J89">
         <f t="shared" si="6"/>
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="K89" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">                     </v>
+        <v xml:space="preserve">                  </v>
       </c>
     </row>
     <row r="90" spans="2:11">
       <c r="B90" t="s">
-        <v>184</v>
-      </c>
-      <c r="C90" s="1" t="s">
-        <v>185</v>
+        <v>188</v>
+      </c>
+      <c r="C90" t="s">
+        <v>320</v>
       </c>
       <c r="D90" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E90" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="G90" t="str">
-        <f t="shared" si="4"/>
-        <v>Francis-Yan Cyr-Racine          \\</v>
+        <f>CONCATENATE(C90," ",B90,K90,"\\")</f>
+        <v>Shirokoff Erik                  \\</v>
       </c>
       <c r="I90">
-        <f t="shared" si="5"/>
-        <v>22</v>
+        <f>LEN(C90) + LEN(B90) +1</f>
+        <v>14</v>
       </c>
       <c r="J90">
         <f t="shared" si="6"/>
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="K90" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">          </v>
+        <v xml:space="preserve">                  </v>
       </c>
     </row>
     <row r="91" spans="2:11">
       <c r="B91" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="D91" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E91" t="s">
-        <v>189</v>
+        <v>93</v>
       </c>
       <c r="G91" t="str">
         <f t="shared" si="4"/>
-        <v>Tijmen de Haan                  \\</v>
+        <v>Aurelien Fraisse                \\</v>
       </c>
       <c r="I91">
         <f t="shared" si="5"/>
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="J91">
         <f t="shared" si="6"/>
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="K91" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">                  </v>
+        <v xml:space="preserve">                </v>
       </c>
     </row>
     <row r="92" spans="2:11">
-      <c r="B92" t="s">
-        <v>190</v>
+      <c r="B92" s="1" t="s">
+        <v>193</v>
       </c>
       <c r="C92" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="D92" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E92" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="G92" t="str">
-        <f t="shared" si="4"/>
-        <v>Shirokoff, Erik                 \\</v>
+        <f>CONCATENATE(C92," ",B92,K92,"\\")</f>
+        <v>Piacentini Francesco            \\</v>
       </c>
       <c r="I92">
-        <f t="shared" si="5"/>
-        <v>15</v>
+        <f>LEN(C92) + LEN(B92) +1</f>
+        <v>20</v>
       </c>
       <c r="J92">
         <f t="shared" si="6"/>
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="K92" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">                 </v>
+        <v xml:space="preserve">            </v>
       </c>
     </row>
     <row r="93" spans="2:11">
-      <c r="B93" t="s">
-        <v>193</v>
-      </c>
-      <c r="C93" s="1" t="s">
-        <v>194</v>
+      <c r="B93" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="C93" t="s">
+        <v>195</v>
       </c>
       <c r="D93" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E93" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="G93" t="str">
-        <f t="shared" si="4"/>
-        <v>Aurelien Fraisse                \\</v>
+        <f>CONCATENATE(C93," ",B93,K93,"\\")</f>
+        <v>Bouchet Fran\c{c}ois            \\</v>
       </c>
       <c r="I93">
-        <f t="shared" si="5"/>
-        <v>16</v>
+        <f>LEN(C93) + LEN(B93) +1</f>
+        <v>20</v>
       </c>
       <c r="J93">
         <f t="shared" si="6"/>
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="K93" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">                </v>
+        <v xml:space="preserve">            </v>
       </c>
     </row>
     <row r="94" spans="2:11">
-      <c r="B94" s="1" t="s">
+      <c r="B94" t="s">
         <v>196</v>
       </c>
-      <c r="C94" t="s">
-        <v>195</v>
+      <c r="C94" s="1" t="s">
+        <v>197</v>
       </c>
       <c r="D94" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E94" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="G94" t="str">
-        <f>CONCATENATE(C94," ",B94,K94,"\\")</f>
-        <v>Piacentini Francesco            \\</v>
+        <f t="shared" si="4"/>
+        <v>Silvia Galli                    \\</v>
       </c>
       <c r="I94">
-        <f>LEN(C94) + LEN(B94) +1</f>
+        <f t="shared" si="5"/>
+        <v>12</v>
+      </c>
+      <c r="J94">
+        <f t="shared" si="6"/>
         <v>20</v>
       </c>
-      <c r="J94">
-        <f t="shared" si="6"/>
-        <v>12</v>
-      </c>
       <c r="K94" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">            </v>
+        <v xml:space="preserve">                    </v>
       </c>
     </row>
     <row r="95" spans="2:11">
-      <c r="B95" s="1" t="s">
-        <v>318</v>
+      <c r="B95" t="s">
+        <v>199</v>
       </c>
       <c r="C95" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="D95" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E95" t="s">
-        <v>86</v>
+        <v>201</v>
       </c>
       <c r="G95" t="str">
-        <f>CONCATENATE(C95," ",B95,K95,"\\")</f>
-        <v>Bouchet Fran\c{c}ois            \\</v>
+        <f t="shared" si="4"/>
+        <v>Ken Ganga                       \\</v>
       </c>
       <c r="I95">
-        <f>LEN(C95) + LEN(B95) +1</f>
-        <v>20</v>
+        <f t="shared" si="5"/>
+        <v>9</v>
       </c>
       <c r="J95">
         <f t="shared" si="6"/>
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="K95" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">            </v>
+        <v xml:space="preserve">                       </v>
       </c>
     </row>
     <row r="96" spans="2:11">
       <c r="B96" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="D96" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E96" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="G96" t="str">
         <f t="shared" si="4"/>
-        <v>Silvia Galli                    \\</v>
+        <v>Tuhin Ghosh                     \\</v>
       </c>
       <c r="I96">
         <f t="shared" si="5"/>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J96">
         <f t="shared" si="6"/>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K96" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">                    </v>
+        <v xml:space="preserve">                     </v>
       </c>
     </row>
     <row r="97" spans="2:11">
       <c r="B97" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="C97" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="D97" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E97" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="G97" t="str">
         <f t="shared" si="4"/>
-        <v>Ken Ganga                       \\</v>
+        <v>Jon E. Gudmundsson              \\</v>
       </c>
       <c r="I97">
         <f t="shared" si="5"/>
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="J97">
         <f t="shared" si="6"/>
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="K97" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">                       </v>
+        <v xml:space="preserve">              </v>
       </c>
     </row>
     <row r="98" spans="2:11">
       <c r="B98" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="D98" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E98" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="G98" t="str">
         <f t="shared" si="4"/>
-        <v>Tuhin Ghosh                     \\</v>
+        <v>Marc Kamionkowski               \\</v>
       </c>
       <c r="I98">
         <f t="shared" si="5"/>
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="J98">
         <f t="shared" si="6"/>
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="K98" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">                     </v>
+        <v xml:space="preserve">               </v>
       </c>
     </row>
     <row r="99" spans="2:11">
       <c r="B99" t="s">
-        <v>208</v>
-      </c>
-      <c r="C99" t="s">
-        <v>209</v>
+        <v>211</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>212</v>
       </c>
       <c r="D99" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E99" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="G99" t="str">
         <f t="shared" si="4"/>
-        <v>Jon E. Gudmundsson              \\</v>
+        <v>Reijo Keskitalo                 \\</v>
       </c>
       <c r="I99">
         <f t="shared" si="5"/>
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="J99">
         <f t="shared" si="6"/>
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="K99" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">              </v>
+        <v xml:space="preserve">                 </v>
       </c>
     </row>
     <row r="100" spans="2:11">
       <c r="B100" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="D100" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E100" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="G100" t="str">
         <f t="shared" si="4"/>
-        <v>Marc Kamionkowski               \\</v>
+        <v>Rishi Khatri                    \\</v>
       </c>
       <c r="I100">
         <f t="shared" si="5"/>
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="J100">
         <f t="shared" si="6"/>
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="K100" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">               </v>
+        <v xml:space="preserve">                    </v>
       </c>
     </row>
     <row r="101" spans="2:11">
       <c r="B101" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="D101" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E101" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="G101" t="str">
         <f t="shared" si="4"/>
-        <v>Reijo Keskitalo                 \\</v>
+        <v>Ely Kovetz                      \\</v>
       </c>
       <c r="I101">
         <f t="shared" si="5"/>
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="J101">
         <f t="shared" si="6"/>
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="K101" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">                 </v>
+        <v xml:space="preserve">                      </v>
       </c>
     </row>
     <row r="102" spans="2:11">
       <c r="B102" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="D102" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E102" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="G102" t="str">
         <f t="shared" si="4"/>
-        <v>Rishi Khatri                    \\</v>
+        <v>Daniel Lenz                     \\</v>
       </c>
       <c r="I102">
         <f t="shared" si="5"/>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J102">
         <f t="shared" si="6"/>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K102" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">                    </v>
+        <v xml:space="preserve">                     </v>
       </c>
     </row>
     <row r="103" spans="2:11">
       <c r="B103" t="s">
-        <v>220</v>
-      </c>
-      <c r="C103" s="1" t="s">
-        <v>221</v>
+        <v>222</v>
+      </c>
+      <c r="C103" t="s">
+        <v>223</v>
       </c>
       <c r="D103" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E103" t="s">
-        <v>213</v>
+        <v>224</v>
       </c>
       <c r="G103" t="str">
         <f t="shared" si="4"/>
-        <v>Ely Kovetz                      \\</v>
+        <v>Marilena Loverde                \\</v>
       </c>
       <c r="I103">
         <f t="shared" si="5"/>
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="J103">
         <f t="shared" si="6"/>
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="K103" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">                      </v>
+        <v xml:space="preserve">                </v>
       </c>
     </row>
     <row r="104" spans="2:11">
       <c r="B104" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="D104" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E104" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="G104" t="str">
         <f t="shared" si="4"/>
-        <v>Daniel Lenz                     \\</v>
+        <v>Carlos Martins                  \\</v>
       </c>
       <c r="I104">
         <f t="shared" si="5"/>
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="J104">
         <f t="shared" si="6"/>
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="K104" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">                     </v>
+        <v xml:space="preserve">                  </v>
       </c>
     </row>
     <row r="105" spans="2:11">
       <c r="B105" t="s">
-        <v>225</v>
+        <v>196</v>
       </c>
       <c r="C105" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="D105" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E105" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="G105" t="str">
         <f t="shared" si="4"/>
-        <v>Marilena Loverde                \\</v>
+        <v>Silvia Masi                     \\</v>
       </c>
       <c r="I105">
         <f t="shared" si="5"/>
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="J105">
         <f t="shared" si="6"/>
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="K105" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">                </v>
+        <v xml:space="preserve">                     </v>
       </c>
     </row>
     <row r="106" spans="2:11">
-      <c r="B106" t="s">
-        <v>228</v>
+      <c r="B106" s="1" t="s">
+        <v>298</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>229</v>
+        <v>299</v>
       </c>
       <c r="D106" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E106" t="s">
-        <v>230</v>
+        <v>286</v>
       </c>
       <c r="G106" t="str">
         <f t="shared" si="4"/>
-        <v>Carlos Martins                  \\</v>
+        <v>Joel Meyers                     \\</v>
       </c>
       <c r="I106">
         <f t="shared" si="5"/>
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="J106">
         <f t="shared" si="6"/>
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="K106" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">                  </v>
+        <v xml:space="preserve">                     </v>
       </c>
     </row>
     <row r="107" spans="2:11">
       <c r="B107" t="s">
-        <v>199</v>
-      </c>
-      <c r="C107" t="s">
+        <v>230</v>
+      </c>
+      <c r="C107" s="1" t="s">
         <v>231</v>
       </c>
       <c r="D107" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E107" t="s">
         <v>232</v>
       </c>
       <c r="G107" t="str">
         <f t="shared" si="4"/>
-        <v>Silvia Masi                     \\</v>
+        <v>Lorenzo Moncelsi                \\</v>
       </c>
       <c r="I107">
         <f t="shared" si="5"/>
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="J107">
         <f t="shared" si="6"/>
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="K107" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">                     </v>
+        <v xml:space="preserve">                </v>
       </c>
     </row>
     <row r="108" spans="2:11">
-      <c r="B108" s="1" t="s">
-        <v>301</v>
+      <c r="B108" t="s">
+        <v>233</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>302</v>
+        <v>234</v>
       </c>
       <c r="D108" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E108" t="s">
-        <v>289</v>
+        <v>235</v>
       </c>
       <c r="G108" t="str">
         <f t="shared" si="4"/>
-        <v>Joel Meyers                     \\</v>
+        <v>Pavel Motloch                   \\</v>
       </c>
       <c r="I108">
         <f t="shared" si="5"/>
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="J108">
         <f t="shared" si="6"/>
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="K108" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">                     </v>
+        <v xml:space="preserve">                   </v>
       </c>
     </row>
     <row r="109" spans="2:11">
       <c r="B109" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="D109" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E109" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="G109" t="str">
         <f t="shared" si="4"/>
-        <v>Lorenzo Moncelsi                \\</v>
+        <v>Tony Mroczkowski                \\</v>
       </c>
       <c r="I109">
         <f t="shared" si="5"/>
@@ -4373,320 +4376,317 @@
     </row>
     <row r="110" spans="2:11">
       <c r="B110" t="s">
-        <v>236</v>
-      </c>
-      <c r="C110" s="1" t="s">
-        <v>237</v>
+        <v>233</v>
+      </c>
+      <c r="C110" t="s">
+        <v>239</v>
       </c>
       <c r="D110" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E110" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="G110" t="str">
         <f t="shared" si="4"/>
-        <v>Pavel Motloch                   \\</v>
+        <v>Pavel Naselsky                  \\</v>
       </c>
       <c r="I110">
         <f t="shared" si="5"/>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="J110">
         <f t="shared" si="6"/>
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K110" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">                   </v>
+        <v xml:space="preserve">                  </v>
       </c>
     </row>
     <row r="111" spans="2:11">
       <c r="B111" t="s">
-        <v>239</v>
+        <v>168</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="D111" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E111" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="G111" t="str">
         <f t="shared" si="4"/>
-        <v>Tony Mroczkowski                \\</v>
+        <v>Federico Nati                   \\</v>
       </c>
       <c r="I111">
         <f t="shared" si="5"/>
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="J111">
         <f t="shared" si="6"/>
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="K111" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">                </v>
+        <v xml:space="preserve">                   </v>
       </c>
     </row>
     <row r="112" spans="2:11">
       <c r="B112" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="C112" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="D112" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E112" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="G112" t="str">
         <f t="shared" si="4"/>
-        <v>Pavel Naselsky                  \\</v>
+        <v>Elena Orlando                   \\</v>
       </c>
       <c r="I112">
         <f t="shared" si="5"/>
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J112">
         <f t="shared" si="6"/>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="K112" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">                  </v>
+        <v xml:space="preserve">                   </v>
       </c>
     </row>
     <row r="113" spans="2:11">
       <c r="B113" t="s">
-        <v>170</v>
+        <v>246</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="D113" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E113" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="G113" t="str">
         <f t="shared" si="4"/>
-        <v>Federico Nati                   \\</v>
+        <v>Giuseppe Puglisi                \\</v>
       </c>
       <c r="I113">
         <f t="shared" si="5"/>
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="J113">
         <f t="shared" si="6"/>
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="K113" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">                   </v>
+        <v xml:space="preserve">                </v>
       </c>
     </row>
     <row r="114" spans="2:11">
       <c r="B114" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="C114" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="D114" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E114" t="s">
-        <v>248</v>
+        <v>170</v>
       </c>
       <c r="G114" t="str">
         <f t="shared" si="4"/>
-        <v>Elena Orlando                   \\</v>
+        <v>Christian Reichardt             \\</v>
       </c>
       <c r="I114">
         <f t="shared" si="5"/>
+        <v>19</v>
+      </c>
+      <c r="J114">
+        <f t="shared" si="6"/>
         <v>13</v>
       </c>
-      <c r="J114">
-        <f t="shared" si="6"/>
-        <v>19</v>
-      </c>
       <c r="K114" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">                   </v>
+        <v xml:space="preserve">             </v>
       </c>
     </row>
     <row r="115" spans="2:11">
       <c r="B115" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="D115" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E115" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="G115" t="str">
         <f t="shared" si="4"/>
-        <v>Giuseppe Puglisi                \\</v>
+        <v>Anirban Roy                     \\</v>
       </c>
       <c r="I115">
         <f t="shared" si="5"/>
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="J115">
         <f t="shared" si="6"/>
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="K115" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">                </v>
+        <v xml:space="preserve">                     </v>
       </c>
     </row>
     <row r="116" spans="2:11">
       <c r="B116" t="s">
-        <v>252</v>
-      </c>
-      <c r="C116" t="s">
-        <v>253</v>
+        <v>254</v>
+      </c>
+      <c r="C116" s="1" t="s">
+        <v>255</v>
       </c>
       <c r="D116" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E116" t="s">
-        <v>172</v>
+        <v>256</v>
       </c>
       <c r="G116" t="str">
         <f t="shared" si="4"/>
-        <v>Christian Reichardt             \\</v>
+        <v>Maria Salatino                  \\</v>
       </c>
       <c r="I116">
         <f t="shared" si="5"/>
+        <v>14</v>
+      </c>
+      <c r="J116">
+        <f t="shared" si="6"/>
+        <v>18</v>
+      </c>
+      <c r="K116" t="str">
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">                  </v>
+      </c>
+    </row>
+    <row r="117" spans="2:11">
+      <c r="B117" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="C117" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="D117" t="s">
+        <v>158</v>
+      </c>
+      <c r="E117" t="s">
+        <v>281</v>
+      </c>
+      <c r="G117" t="str">
+        <f t="shared" si="4"/>
+        <v>Benjamin Saliwanchik            \\</v>
+      </c>
+      <c r="I117">
+        <f t="shared" si="5"/>
+        <v>20</v>
+      </c>
+      <c r="J117">
+        <f t="shared" si="6"/>
+        <v>12</v>
+      </c>
+      <c r="K117" t="str">
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">            </v>
+      </c>
+    </row>
+    <row r="118" spans="2:11">
+      <c r="B118" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="D118" t="s">
+        <v>158</v>
+      </c>
+      <c r="G118" t="str">
+        <f t="shared" si="4"/>
+        <v>Douglas Scott                   \\</v>
+      </c>
+      <c r="I118">
+        <f t="shared" si="5"/>
+        <v>13</v>
+      </c>
+      <c r="J118">
+        <f t="shared" si="6"/>
         <v>19</v>
       </c>
-      <c r="J116">
-        <f t="shared" si="6"/>
-        <v>13</v>
-      </c>
-      <c r="K116" t="str">
-        <f t="shared" si="7"/>
-        <v xml:space="preserve">             </v>
-      </c>
-    </row>
-    <row r="117" spans="2:11">
-      <c r="B117" t="s">
-        <v>254</v>
-      </c>
-      <c r="C117" s="1" t="s">
-        <v>255</v>
-      </c>
-      <c r="D117" t="s">
-        <v>160</v>
-      </c>
-      <c r="E117" t="s">
-        <v>256</v>
-      </c>
-      <c r="G117" t="str">
-        <f t="shared" si="4"/>
-        <v>Anirban Roy                     \\</v>
-      </c>
-      <c r="I117">
-        <f t="shared" si="5"/>
-        <v>11</v>
-      </c>
-      <c r="J117">
-        <f t="shared" si="6"/>
-        <v>21</v>
-      </c>
-      <c r="K117" t="str">
-        <f t="shared" si="7"/>
-        <v xml:space="preserve">                     </v>
-      </c>
-    </row>
-    <row r="118" spans="2:11">
-      <c r="B118" t="s">
-        <v>257</v>
-      </c>
-      <c r="C118" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="D118" t="s">
-        <v>160</v>
-      </c>
-      <c r="E118" t="s">
-        <v>259</v>
-      </c>
-      <c r="G118" t="str">
-        <f t="shared" si="4"/>
-        <v>Maria Salatino                  \\</v>
-      </c>
-      <c r="I118">
-        <f t="shared" si="5"/>
-        <v>14</v>
-      </c>
-      <c r="J118">
-        <f t="shared" si="6"/>
-        <v>18</v>
-      </c>
       <c r="K118" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">                  </v>
+        <v xml:space="preserve">                   </v>
       </c>
     </row>
     <row r="119" spans="2:11">
       <c r="B119" s="1" t="s">
-        <v>294</v>
+        <v>302</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>295</v>
+        <v>303</v>
       </c>
       <c r="D119" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E119" t="s">
-        <v>284</v>
+        <v>224</v>
       </c>
       <c r="G119" t="str">
         <f t="shared" si="4"/>
-        <v>Benjamin Saliwanchik            \\</v>
+        <v>Neelima Sehgal                  \\</v>
       </c>
       <c r="I119">
         <f t="shared" si="5"/>
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="J119">
         <f t="shared" si="6"/>
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="K119" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">            </v>
+        <v xml:space="preserve">                  </v>
       </c>
     </row>
     <row r="120" spans="2:11">
-      <c r="B120" s="1" t="s">
-        <v>305</v>
+      <c r="B120" t="s">
+        <v>257</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>306</v>
+        <v>258</v>
       </c>
       <c r="D120" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E120" t="s">
-        <v>227</v>
+        <v>259</v>
       </c>
       <c r="G120" t="str">
         <f t="shared" si="4"/>
-        <v>Neelima Sehgal                  \\</v>
+        <v>Sarah Shandera                  \\</v>
       </c>
       <c r="I120">
         <f t="shared" si="5"/>
@@ -4709,26 +4709,26 @@
         <v>261</v>
       </c>
       <c r="D121" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E121" t="s">
         <v>262</v>
       </c>
       <c r="G121" t="str">
         <f t="shared" si="4"/>
-        <v>Sarah Shandera                  \\</v>
+        <v>An\v{z}e Slosar                 \\</v>
       </c>
       <c r="I121">
         <f t="shared" si="5"/>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J121">
         <f t="shared" si="6"/>
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K121" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">                  </v>
+        <v xml:space="preserve">                 </v>
       </c>
     </row>
     <row r="122" spans="2:11">
@@ -4739,236 +4739,236 @@
         <v>264</v>
       </c>
       <c r="D122" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E122" t="s">
-        <v>265</v>
+        <v>187</v>
       </c>
       <c r="G122" t="str">
         <f t="shared" si="4"/>
-        <v>An\v{z}e Slosar                 \\</v>
+        <v>Aritoki Suzuki                  \\</v>
       </c>
       <c r="I122">
         <f t="shared" si="5"/>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J122">
         <f t="shared" si="6"/>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K122" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">                 </v>
+        <v xml:space="preserve">                  </v>
       </c>
     </row>
     <row r="123" spans="2:11">
-      <c r="B123" t="s">
-        <v>266</v>
+      <c r="B123" s="1" t="s">
+        <v>82</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>267</v>
+        <v>300</v>
       </c>
       <c r="D123" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E123" t="s">
-        <v>189</v>
+        <v>287</v>
       </c>
       <c r="G123" t="str">
         <f t="shared" si="4"/>
-        <v>Aritoki Suzuki                  \\</v>
+        <v>Eric Switzer                    \\</v>
       </c>
       <c r="I123">
         <f t="shared" si="5"/>
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="J123">
         <f t="shared" si="6"/>
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="K123" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">                  </v>
+        <v xml:space="preserve">                    </v>
       </c>
     </row>
     <row r="124" spans="2:11">
       <c r="B124" s="1" t="s">
-        <v>84</v>
+        <v>154</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="D124" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E124" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="G124" t="str">
         <f t="shared" si="4"/>
-        <v>Eric Switzer                    \\</v>
+        <v>Andrea Tartari                  \\</v>
       </c>
       <c r="I124">
         <f t="shared" si="5"/>
+        <v>14</v>
+      </c>
+      <c r="J124">
+        <f t="shared" si="6"/>
+        <v>18</v>
+      </c>
+      <c r="K124" t="str">
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">                  </v>
+      </c>
+    </row>
+    <row r="125" spans="2:11">
+      <c r="B125" t="s">
+        <v>265</v>
+      </c>
+      <c r="C125" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="D125" t="s">
+        <v>158</v>
+      </c>
+      <c r="E125" t="s">
+        <v>267</v>
+      </c>
+      <c r="G125" t="str">
+        <f t="shared" si="4"/>
+        <v>Grant Teply                     \\</v>
+      </c>
+      <c r="I125">
+        <f t="shared" si="5"/>
+        <v>11</v>
+      </c>
+      <c r="J125">
+        <f t="shared" si="6"/>
+        <v>21</v>
+      </c>
+      <c r="K125" t="str">
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">                     </v>
+      </c>
+    </row>
+    <row r="126" spans="2:11">
+      <c r="B126" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C126" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="D126" t="s">
+        <v>158</v>
+      </c>
+      <c r="E126" t="s">
+        <v>289</v>
+      </c>
+      <c r="G126" t="str">
+        <f t="shared" si="4"/>
+        <v>Peter Timbie                    \\</v>
+      </c>
+      <c r="I126">
+        <f t="shared" si="5"/>
         <v>12</v>
       </c>
-      <c r="J124">
+      <c r="J126">
         <f t="shared" si="6"/>
         <v>20</v>
       </c>
-      <c r="K124" t="str">
+      <c r="K126" t="str">
         <f t="shared" si="7"/>
         <v xml:space="preserve">                    </v>
       </c>
     </row>
-    <row r="125" spans="2:11">
-      <c r="B125" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="C125" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="D125" t="s">
-        <v>160</v>
-      </c>
-      <c r="E125" t="s">
+    <row r="127" spans="2:11">
+      <c r="B127" t="s">
+        <v>268</v>
+      </c>
+      <c r="C127" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="D127" t="s">
+        <v>158</v>
+      </c>
+      <c r="E127" t="s">
+        <v>270</v>
+      </c>
+      <c r="G127" t="str">
+        <f t="shared" si="4"/>
+        <v>Matthieu Tristram               \\</v>
+      </c>
+      <c r="I127">
+        <f t="shared" si="5"/>
+        <v>17</v>
+      </c>
+      <c r="J127">
+        <f t="shared" si="6"/>
+        <v>15</v>
+      </c>
+      <c r="K127" t="str">
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">               </v>
+      </c>
+    </row>
+    <row r="128" spans="2:11">
+      <c r="B128" s="1" t="s">
         <v>291</v>
       </c>
-      <c r="G125" t="str">
-        <f t="shared" si="4"/>
-        <v>Andrea Tartari                  \\</v>
-      </c>
-      <c r="I125">
-        <f t="shared" si="5"/>
-        <v>14</v>
-      </c>
-      <c r="J125">
-        <f t="shared" si="6"/>
-        <v>18</v>
-      </c>
-      <c r="K125" t="str">
-        <f t="shared" si="7"/>
-        <v xml:space="preserve">                  </v>
-      </c>
-    </row>
-    <row r="126" spans="2:11">
-      <c r="B126" t="s">
-        <v>268</v>
-      </c>
-      <c r="C126" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="D126" t="s">
-        <v>160</v>
-      </c>
-      <c r="E126" t="s">
-        <v>270</v>
-      </c>
-      <c r="G126" t="str">
-        <f t="shared" si="4"/>
-        <v>Grant Teply                     \\</v>
-      </c>
-      <c r="I126">
-        <f t="shared" si="5"/>
-        <v>11</v>
-      </c>
-      <c r="J126">
-        <f t="shared" si="6"/>
-        <v>21</v>
-      </c>
-      <c r="K126" t="str">
-        <f t="shared" si="7"/>
-        <v xml:space="preserve">                     </v>
-      </c>
-    </row>
-    <row r="127" spans="2:11">
-      <c r="B127" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C127" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="D127" t="s">
-        <v>160</v>
-      </c>
-      <c r="E127" t="s">
-        <v>292</v>
-      </c>
-      <c r="G127" t="str">
-        <f t="shared" si="4"/>
-        <v>Peter Timbie                    \\</v>
-      </c>
-      <c r="I127">
+      <c r="C128" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="D128" t="s">
+        <v>158</v>
+      </c>
+      <c r="E128" t="s">
+        <v>283</v>
+      </c>
+      <c r="G128" t="str">
+        <f t="shared" si="4"/>
+        <v>Benjamin Wallisch               \\</v>
+      </c>
+      <c r="I128">
+        <f t="shared" si="5"/>
+        <v>17</v>
+      </c>
+      <c r="J128">
+        <f t="shared" si="6"/>
+        <v>15</v>
+      </c>
+      <c r="K128" t="str">
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">               </v>
+      </c>
+    </row>
+    <row r="129" spans="2:11">
+      <c r="B129" t="s">
+        <v>271</v>
+      </c>
+      <c r="C129" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="D129" t="s">
+        <v>158</v>
+      </c>
+      <c r="E129" t="s">
+        <v>273</v>
+      </c>
+      <c r="G129" t="str">
+        <f t="shared" si="4"/>
+        <v>Scott Watson                    \\</v>
+      </c>
+      <c r="I129">
         <f t="shared" si="5"/>
         <v>12</v>
       </c>
-      <c r="J127">
+      <c r="J129">
         <f t="shared" si="6"/>
         <v>20</v>
       </c>
-      <c r="K127" t="str">
+      <c r="K129" t="str">
         <f t="shared" si="7"/>
         <v xml:space="preserve">                    </v>
-      </c>
-    </row>
-    <row r="128" spans="2:11">
-      <c r="B128" t="s">
-        <v>271</v>
-      </c>
-      <c r="C128" s="1" t="s">
-        <v>272</v>
-      </c>
-      <c r="D128" t="s">
-        <v>160</v>
-      </c>
-      <c r="E128" t="s">
-        <v>273</v>
-      </c>
-      <c r="G128" t="str">
-        <f t="shared" si="4"/>
-        <v>Matthieu Tristram               \\</v>
-      </c>
-      <c r="I128">
-        <f t="shared" si="5"/>
-        <v>17</v>
-      </c>
-      <c r="J128">
-        <f t="shared" si="6"/>
-        <v>15</v>
-      </c>
-      <c r="K128" t="str">
-        <f t="shared" si="7"/>
-        <v xml:space="preserve">               </v>
-      </c>
-    </row>
-    <row r="129" spans="2:11">
-      <c r="B129" s="1" t="s">
-        <v>294</v>
-      </c>
-      <c r="C129" s="1" t="s">
-        <v>298</v>
-      </c>
-      <c r="D129" t="s">
-        <v>160</v>
-      </c>
-      <c r="E129" t="s">
-        <v>286</v>
-      </c>
-      <c r="G129" t="str">
-        <f t="shared" si="4"/>
-        <v>Benjamin Wallisch               \\</v>
-      </c>
-      <c r="I129">
-        <f t="shared" si="5"/>
-        <v>17</v>
-      </c>
-      <c r="J129">
-        <f t="shared" si="6"/>
-        <v>15</v>
-      </c>
-      <c r="K129" t="str">
-        <f t="shared" si="7"/>
-        <v xml:space="preserve">               </v>
       </c>
     </row>
     <row r="130" spans="2:11">
@@ -4979,56 +4979,44 @@
         <v>275</v>
       </c>
       <c r="D130" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E130" t="s">
-        <v>276</v>
+        <v>60</v>
       </c>
       <c r="G130" t="str">
         <f t="shared" si="4"/>
-        <v>Scott Watson                    \\</v>
+        <v>Edward J. Wollack               \\</v>
       </c>
       <c r="I130">
         <f t="shared" si="5"/>
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="J130">
         <f t="shared" si="6"/>
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="K130" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">                    </v>
+        <v xml:space="preserve">               </v>
       </c>
     </row>
     <row r="131" spans="2:11">
-      <c r="B131" t="s">
-        <v>277</v>
-      </c>
-      <c r="C131" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="D131" t="s">
-        <v>160</v>
-      </c>
-      <c r="E131" t="s">
-        <v>60</v>
-      </c>
       <c r="G131" t="str">
         <f t="shared" si="4"/>
-        <v>Edward J. Wollack               \\</v>
+        <v xml:space="preserve">                                \\</v>
       </c>
       <c r="I131">
         <f t="shared" si="5"/>
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="J131">
         <f t="shared" si="6"/>
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="K131" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">               </v>
+        <v xml:space="preserve">                               </v>
       </c>
     </row>
     <row r="132" spans="2:11">
@@ -5140,48 +5128,57 @@
       </c>
     </row>
     <row r="138" spans="2:11">
+      <c r="B138" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C138" t="s">
+        <v>149</v>
+      </c>
+      <c r="D138" t="s">
+        <v>158</v>
+      </c>
       <c r="G138" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">                                \\</v>
+        <f t="shared" ref="G138:G179" si="8">CONCATENATE(B138," ",C138,K138,"\\")</f>
+        <v>Martin White                    \\</v>
       </c>
       <c r="I138">
-        <f t="shared" si="5"/>
-        <v>1</v>
+        <f t="shared" ref="I138:I179" si="9">LEN(B138) + LEN(C138) +1</f>
+        <v>12</v>
       </c>
       <c r="J138">
-        <f t="shared" si="6"/>
-        <v>31</v>
+        <f t="shared" ref="J138:J179" si="10">IF(I138&lt;30,(32-I138),3)</f>
+        <v>20</v>
       </c>
       <c r="K138" t="str">
-        <f t="shared" si="7"/>
-        <v xml:space="preserve">                               </v>
+        <f t="shared" ref="K138:K179" si="11">REPT(" ",J138)</f>
+        <v xml:space="preserve">                    </v>
       </c>
     </row>
     <row r="139" spans="2:11">
       <c r="B139" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="C139" t="s">
-        <v>151</v>
+        <v>26</v>
+      </c>
+      <c r="C139" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="D139" t="s">
-        <v>160</v>
+        <v>8</v>
       </c>
       <c r="G139" t="str">
-        <f t="shared" ref="G139:G179" si="8">CONCATENATE(B139," ",C139,K139,"\\")</f>
-        <v>Martin White                    \\</v>
+        <f>CONCATENATE(B139," ",C139,K139,"\\")</f>
+        <v>Kim Boddy                       \\</v>
       </c>
       <c r="I139">
-        <f t="shared" ref="I139:I179" si="9">LEN(B139) + LEN(C139) +1</f>
-        <v>12</v>
+        <f>LEN(B139) + LEN(C139) +1</f>
+        <v>9</v>
       </c>
       <c r="J139">
-        <f t="shared" ref="J139:J179" si="10">IF(I139&lt;30,(32-I139),3)</f>
-        <v>20</v>
+        <f>IF(I139&lt;30,(32-I139),3)</f>
+        <v>23</v>
       </c>
       <c r="K139" t="str">
-        <f t="shared" ref="K139:K179" si="11">REPT(" ",J139)</f>
-        <v xml:space="preserve">                    </v>
+        <f>REPT(" ",J139)</f>
+        <v xml:space="preserve">                       </v>
       </c>
     </row>
     <row r="140" spans="2:11">

</xml_diff>

<commit_message>
Revert "Merge branch 'master' of https://github.com/CMB-Probe/PICOReport"
This reverts commit 14accf8368aaad076e363e65dea37c7630577c6d, reversing
changes made to 2c9f1a56767c4576274eae5b75d5f6fe81326c9b.
</commit_message>
<xml_diff>
--- a/ReferenceDocuments/ReportAuthors.xlsx
+++ b/ReferenceDocuments/ReportAuthors.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="321">
   <si>
     <t>Report Authors</t>
   </si>
@@ -856,6 +856,9 @@
     <t>Please update the relevant lines above if you add/remove/change names in this list.</t>
   </si>
   <si>
+    <t>12/5/2018, 1 pm.</t>
+  </si>
+  <si>
     <t>Yale University</t>
   </si>
   <si>
@@ -974,21 +977,6 @@
   </si>
   <si>
     <t>Shirokoff</t>
-  </si>
-  <si>
-    <t>CfA/Harvard</t>
-  </si>
-  <si>
-    <t>Racine</t>
-  </si>
-  <si>
-    <t>Caterina</t>
-  </si>
-  <si>
-    <t>Umilt\`{a}</t>
-  </si>
-  <si>
-    <t>12/10/2018, 3 pm.</t>
   </si>
 </sst>
 </file>
@@ -1419,10 +1407,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:K180"/>
+  <dimension ref="A1:K179"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C4" sqref="C3:C5"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35:XFD35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -1452,7 +1440,7 @@
       </c>
       <c r="B3"/>
       <c r="C3" s="1" t="s">
-        <v>324</v>
+        <v>280</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -1461,7 +1449,7 @@
       </c>
       <c r="B4"/>
       <c r="C4" s="1" t="s">
-        <v>324</v>
+        <v>280</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -1470,7 +1458,7 @@
       </c>
       <c r="B5"/>
       <c r="C5" s="1" t="s">
-        <v>324</v>
+        <v>280</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -1502,16 +1490,16 @@
         <v>5</v>
       </c>
       <c r="G9" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="I9" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="J9" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="K9" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -1555,15 +1543,15 @@
         <v>11</v>
       </c>
       <c r="G11" t="str">
-        <f t="shared" ref="G11:G74" si="0">CONCATENATE(B11," ",C11,K11,"\\")</f>
+        <f t="shared" ref="G11:G72" si="0">CONCATENATE(B11," ",C11,K11,"\\")</f>
         <v>Peter Ashton                    \\</v>
       </c>
       <c r="I11">
-        <f t="shared" ref="I11:I74" si="1">LEN(B11) + LEN(C11) +1</f>
+        <f t="shared" ref="I11:I72" si="1">LEN(B11) + LEN(C11) +1</f>
         <v>12</v>
       </c>
       <c r="J11">
-        <f t="shared" ref="J11:J74" si="2">IF(I11&lt;30,(32-I11),3)</f>
+        <f t="shared" ref="J11:J72" si="2">IF(I11&lt;30,(32-I11),3)</f>
         <v>20</v>
       </c>
       <c r="K11" t="str">
@@ -1969,146 +1957,149 @@
     </row>
     <row r="26" spans="2:11">
       <c r="B26" t="s">
-        <v>46</v>
-      </c>
-      <c r="C26" t="s">
-        <v>47</v>
+        <v>313</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>312</v>
       </c>
       <c r="D26" t="s">
         <v>8</v>
       </c>
       <c r="E26" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="G26" t="str">
         <f t="shared" si="0"/>
-        <v>Jacques Delabrouille            \\</v>
+        <v>Gianfranco De Zotti             \\</v>
       </c>
       <c r="I26">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J26">
         <f t="shared" si="2"/>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="K26" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">            </v>
+        <v xml:space="preserve">             </v>
       </c>
     </row>
     <row r="27" spans="2:11">
       <c r="B27" t="s">
+        <v>46</v>
+      </c>
+      <c r="C27" t="s">
+        <v>47</v>
+      </c>
+      <c r="D27" t="s">
+        <v>8</v>
+      </c>
+      <c r="E27" t="s">
+        <v>48</v>
+      </c>
+      <c r="G27" t="str">
+        <f t="shared" si="0"/>
+        <v>Jacques Delabrouille            \\</v>
+      </c>
+      <c r="I27">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="J27">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="K27" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">            </v>
+      </c>
+    </row>
+    <row r="28" spans="2:11">
+      <c r="B28" t="s">
         <v>49</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C28" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D27" t="s">
-        <v>8</v>
-      </c>
-      <c r="E27" t="s">
+      <c r="D28" t="s">
+        <v>8</v>
+      </c>
+      <c r="E28" t="s">
         <v>51</v>
       </c>
-      <c r="G27" t="str">
+      <c r="G28" t="str">
         <f t="shared" si="0"/>
         <v>Eleonora Di Valentino           \\</v>
       </c>
-      <c r="I27">
+      <c r="I28">
         <f t="shared" si="1"/>
         <v>21</v>
       </c>
-      <c r="J27">
+      <c r="J28">
         <f t="shared" si="2"/>
         <v>11</v>
       </c>
-      <c r="K27" t="str">
+      <c r="K28" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve">           </v>
       </c>
     </row>
-    <row r="28" spans="2:11">
-      <c r="B28" s="1" t="s">
+    <row r="29" spans="2:11">
+      <c r="B29" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C29" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="D28" t="s">
-        <v>8</v>
-      </c>
-      <c r="G28" t="str">
+      <c r="D29" t="s">
+        <v>8</v>
+      </c>
+      <c r="G29" t="str">
         <f t="shared" si="0"/>
         <v>Joy Didier                      \\</v>
       </c>
-      <c r="I28">
+      <c r="I29">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="J28">
+      <c r="J29">
         <f t="shared" si="2"/>
         <v>22</v>
       </c>
-      <c r="K28" t="str">
+      <c r="K29" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve">                      </v>
       </c>
     </row>
-    <row r="29" spans="2:11">
-      <c r="B29" t="s">
+    <row r="30" spans="2:11">
+      <c r="B30" t="s">
         <v>54</v>
       </c>
-      <c r="C29" s="1" t="s">
-        <v>313</v>
-      </c>
-      <c r="D29" t="s">
-        <v>8</v>
-      </c>
-      <c r="E29" t="s">
+      <c r="C30" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="D30" t="s">
+        <v>8</v>
+      </c>
+      <c r="E30" t="s">
         <v>55</v>
       </c>
-      <c r="G29" t="str">
+      <c r="G30" t="str">
         <f t="shared" si="0"/>
         <v>Olivier Dor\'e                  \\</v>
       </c>
-      <c r="I29">
+      <c r="I30">
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="J29">
+      <c r="J30">
         <f t="shared" si="2"/>
         <v>18</v>
       </c>
-      <c r="K29" t="str">
+      <c r="K30" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve">                  </v>
-      </c>
-    </row>
-    <row r="30" spans="2:11">
-      <c r="B30" s="1" t="s">
-        <v>310</v>
-      </c>
-      <c r="C30" t="s">
-        <v>309</v>
-      </c>
-      <c r="D30" t="s">
-        <v>8</v>
-      </c>
-      <c r="G30" t="str">
-        <f t="shared" si="0"/>
-        <v>Alexander van Engelen           \\</v>
-      </c>
-      <c r="I30">
-        <f t="shared" si="1"/>
-        <v>21</v>
-      </c>
-      <c r="J30">
-        <f t="shared" si="2"/>
-        <v>11</v>
-      </c>
-      <c r="K30" t="str">
-        <f t="shared" si="3"/>
-        <v xml:space="preserve">           </v>
       </c>
     </row>
     <row r="31" spans="2:11">
@@ -2197,16 +2188,16 @@
     </row>
     <row r="34" spans="2:11">
       <c r="B34" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="C34" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="D34" t="s">
         <v>8</v>
       </c>
       <c r="E34" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="G34" t="str">
         <f t="shared" si="0"/>
@@ -2602,7 +2593,7 @@
     </row>
     <row r="48" spans="2:11">
       <c r="B48" s="1" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>96</v>
@@ -2655,114 +2646,114 @@
       </c>
     </row>
     <row r="50" spans="2:11">
-      <c r="B50" t="s">
-        <v>296</v>
+      <c r="B50" s="1" t="s">
+        <v>99</v>
       </c>
       <c r="C50" t="s">
-        <v>315</v>
+        <v>100</v>
       </c>
       <c r="D50" t="s">
         <v>8</v>
       </c>
-      <c r="E50" t="s">
-        <v>284</v>
-      </c>
       <c r="G50" t="str">
         <f t="shared" si="0"/>
-        <v>Marcos L\'{o}pez-Caniego        \\</v>
+        <v>Charles Lawrence                \\</v>
       </c>
       <c r="I50">
         <f t="shared" si="1"/>
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="J50">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="K50" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">        </v>
+        <v xml:space="preserve">                </v>
       </c>
     </row>
     <row r="51" spans="2:11">
       <c r="B51" s="1" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C51" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D51" t="s">
         <v>8</v>
       </c>
       <c r="G51" t="str">
         <f t="shared" si="0"/>
-        <v>Charles Lawrence                \\</v>
+        <v>Alex Lazarian                   \\</v>
       </c>
       <c r="I51">
         <f t="shared" si="1"/>
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="J51">
         <f t="shared" si="2"/>
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="K51" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">                </v>
+        <v xml:space="preserve">                   </v>
       </c>
     </row>
     <row r="52" spans="2:11">
       <c r="B52" s="1" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C52" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="D52" t="s">
         <v>8</v>
       </c>
       <c r="G52" t="str">
         <f t="shared" si="0"/>
-        <v>Alex Lazarian                   \\</v>
+        <v>Zack Li                         \\</v>
       </c>
       <c r="I52">
         <f t="shared" si="1"/>
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="J52">
         <f t="shared" si="2"/>
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="K52" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">                   </v>
+        <v xml:space="preserve">                         </v>
       </c>
     </row>
     <row r="53" spans="2:11">
-      <c r="B53" s="1" t="s">
-        <v>103</v>
+      <c r="B53" t="s">
+        <v>297</v>
       </c>
       <c r="C53" t="s">
-        <v>104</v>
+        <v>316</v>
       </c>
       <c r="D53" t="s">
         <v>8</v>
       </c>
+      <c r="E53" t="s">
+        <v>285</v>
+      </c>
       <c r="G53" t="str">
         <f t="shared" si="0"/>
-        <v>Zack Li                         \\</v>
+        <v>Marcos L\'{o}pez-Caniego        \\</v>
       </c>
       <c r="I53">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="J53">
         <f t="shared" si="2"/>
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="K53" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">                         </v>
+        <v xml:space="preserve">        </v>
       </c>
     </row>
     <row r="54" spans="2:11">
@@ -3108,144 +3099,144 @@
       </c>
     </row>
     <row r="66" spans="2:11">
-      <c r="B66" s="1" t="s">
-        <v>318</v>
+      <c r="B66" t="s">
+        <v>133</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>271</v>
+        <v>134</v>
       </c>
       <c r="D66" t="s">
         <v>8</v>
       </c>
+      <c r="E66" t="s">
+        <v>135</v>
+      </c>
       <c r="G66" t="str">
         <f t="shared" si="0"/>
-        <v>Douglas Scott                   \\</v>
+        <v>Ian Stephens                    \\</v>
       </c>
       <c r="I66">
         <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="J66">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="K66" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">                    </v>
+      </c>
+    </row>
+    <row r="67" spans="2:11">
+      <c r="B67" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C67" t="s">
+        <v>137</v>
+      </c>
+      <c r="D67" t="s">
+        <v>8</v>
+      </c>
+      <c r="G67" t="str">
+        <f t="shared" si="0"/>
+        <v>Brian Sutin                     \\</v>
+      </c>
+      <c r="I67">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="J67">
+        <f t="shared" si="2"/>
+        <v>21</v>
+      </c>
+      <c r="K67" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">                     </v>
+      </c>
+    </row>
+    <row r="68" spans="2:11">
+      <c r="B68" t="s">
+        <v>138</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="D68" t="s">
+        <v>8</v>
+      </c>
+      <c r="E68" t="s">
+        <v>140</v>
+      </c>
+      <c r="G68" t="str">
+        <f t="shared" si="0"/>
+        <v>Maurizio Tomasi                 \\</v>
+      </c>
+      <c r="I68">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="J68">
+        <f t="shared" si="2"/>
+        <v>17</v>
+      </c>
+      <c r="K68" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">                 </v>
+      </c>
+    </row>
+    <row r="69" spans="2:11">
+      <c r="B69" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C69" t="s">
+        <v>142</v>
+      </c>
+      <c r="D69" t="s">
+        <v>8</v>
+      </c>
+      <c r="G69" t="str">
+        <f t="shared" si="0"/>
+        <v>Amy Trangsrud                   \\</v>
+      </c>
+      <c r="I69">
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="J66">
+      <c r="J69">
         <f t="shared" si="2"/>
         <v>19</v>
       </c>
-      <c r="K66" t="str">
+      <c r="K69" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve">                   </v>
-      </c>
-    </row>
-    <row r="67" spans="2:11">
-      <c r="B67" t="s">
-        <v>133</v>
-      </c>
-      <c r="C67" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="D67" t="s">
-        <v>8</v>
-      </c>
-      <c r="E67" t="s">
-        <v>135</v>
-      </c>
-      <c r="G67" t="str">
-        <f t="shared" si="0"/>
-        <v>Ian Stephens                    \\</v>
-      </c>
-      <c r="I67">
-        <f t="shared" si="1"/>
-        <v>12</v>
-      </c>
-      <c r="J67">
-        <f t="shared" si="2"/>
-        <v>20</v>
-      </c>
-      <c r="K67" t="str">
-        <f t="shared" si="3"/>
-        <v xml:space="preserve">                    </v>
-      </c>
-    </row>
-    <row r="68" spans="2:11">
-      <c r="B68" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="C68" t="s">
-        <v>137</v>
-      </c>
-      <c r="D68" t="s">
-        <v>8</v>
-      </c>
-      <c r="G68" t="str">
-        <f t="shared" si="0"/>
-        <v>Brian Sutin                     \\</v>
-      </c>
-      <c r="I68">
-        <f t="shared" si="1"/>
-        <v>11</v>
-      </c>
-      <c r="J68">
-        <f t="shared" si="2"/>
-        <v>21</v>
-      </c>
-      <c r="K68" t="str">
-        <f t="shared" si="3"/>
-        <v xml:space="preserve">                     </v>
-      </c>
-    </row>
-    <row r="69" spans="2:11">
-      <c r="B69" t="s">
-        <v>138</v>
-      </c>
-      <c r="C69" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="D69" t="s">
-        <v>8</v>
-      </c>
-      <c r="E69" t="s">
-        <v>140</v>
-      </c>
-      <c r="G69" t="str">
-        <f t="shared" si="0"/>
-        <v>Maurizio Tomasi                 \\</v>
-      </c>
-      <c r="I69">
-        <f t="shared" si="1"/>
-        <v>15</v>
-      </c>
-      <c r="J69">
-        <f t="shared" si="2"/>
-        <v>17</v>
-      </c>
-      <c r="K69" t="str">
-        <f t="shared" si="3"/>
-        <v xml:space="preserve">                 </v>
       </c>
     </row>
     <row r="70" spans="2:11">
       <c r="B70" s="1" t="s">
-        <v>141</v>
+        <v>311</v>
       </c>
       <c r="C70" t="s">
-        <v>142</v>
+        <v>310</v>
       </c>
       <c r="D70" t="s">
         <v>8</v>
       </c>
       <c r="G70" t="str">
         <f t="shared" si="0"/>
-        <v>Amy Trangsrud                   \\</v>
+        <v>Alexander van Engelen           \\</v>
       </c>
       <c r="I70">
         <f t="shared" si="1"/>
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="J70">
         <f t="shared" si="2"/>
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="K70" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">                   </v>
+        <v xml:space="preserve">           </v>
       </c>
     </row>
     <row r="71" spans="2:11">
@@ -3316,19 +3307,19 @@
         <v>8</v>
       </c>
       <c r="G73" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="G73:G137" si="4">CONCATENATE(B73," ",C73,K73,"\\")</f>
         <v>Siyao Xu                        \\</v>
       </c>
       <c r="I73">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="I73:I137" si="5">LEN(B73) + LEN(C73) +1</f>
         <v>8</v>
       </c>
       <c r="J73">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="J73:J137" si="6">IF(I73&lt;30,(32-I73),3)</f>
         <v>24</v>
       </c>
       <c r="K73" t="str">
-        <f t="shared" ref="K73:K138" si="4">REPT(" ",J73)</f>
+        <f t="shared" ref="K73:K137" si="7">REPT(" ",J73)</f>
         <v xml:space="preserve">                        </v>
       </c>
     </row>
@@ -3343,19 +3334,19 @@
         <v>8</v>
       </c>
       <c r="G74" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>Karl Young                      \\</v>
       </c>
       <c r="I74">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="J74">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>22</v>
       </c>
       <c r="K74" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v xml:space="preserve">                      </v>
       </c>
     </row>
@@ -3370,1087 +3361,1107 @@
         <v>8</v>
       </c>
       <c r="G75" t="str">
-        <f t="shared" ref="G75:G76" si="5">CONCATENATE(B75," ",C75,K75,"\\")</f>
+        <f t="shared" si="4"/>
         <v>Andrea Zonca                    \\</v>
       </c>
       <c r="I75">
-        <f t="shared" ref="I75:I76" si="6">LEN(B75) + LEN(C75) +1</f>
+        <f t="shared" si="5"/>
         <v>12</v>
       </c>
       <c r="J75">
-        <f t="shared" ref="J75:J76" si="7">IF(I75&lt;30,(32-I75),3)</f>
+        <f t="shared" si="6"/>
         <v>20</v>
       </c>
       <c r="K75" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v xml:space="preserve">                    </v>
       </c>
     </row>
     <row r="76" spans="2:11">
-      <c r="B76" t="s">
-        <v>312</v>
-      </c>
-      <c r="C76" s="1" t="s">
-        <v>311</v>
-      </c>
-      <c r="D76" t="s">
-        <v>8</v>
-      </c>
-      <c r="E76" t="s">
-        <v>45</v>
-      </c>
+      <c r="B76" s="3"/>
+      <c r="C76"/>
       <c r="G76" t="str">
-        <f t="shared" si="5"/>
-        <v>Gianfranco De Zotti             \\</v>
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">                                \\</v>
       </c>
       <c r="I76">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="J76">
+        <f t="shared" si="6"/>
+        <v>31</v>
+      </c>
+      <c r="K76" t="str">
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">                               </v>
+      </c>
+    </row>
+    <row r="77" spans="2:11">
+      <c r="B77" s="3"/>
+      <c r="C77"/>
+      <c r="G77" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">                                \\</v>
+      </c>
+      <c r="I77">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="J77">
+        <f t="shared" si="6"/>
+        <v>31</v>
+      </c>
+      <c r="K77" t="str">
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">                               </v>
+      </c>
+    </row>
+    <row r="78" spans="2:11">
+      <c r="B78" t="s">
+        <v>156</v>
+      </c>
+      <c r="C78" t="s">
+        <v>157</v>
+      </c>
+      <c r="D78" t="s">
+        <v>158</v>
+      </c>
+      <c r="E78" t="s">
+        <v>159</v>
+      </c>
+      <c r="G78" t="str">
+        <f t="shared" si="4"/>
+        <v>Zeeshan Ahmed                   \\</v>
+      </c>
+      <c r="I78">
+        <f t="shared" si="5"/>
+        <v>13</v>
+      </c>
+      <c r="J78">
         <f t="shared" si="6"/>
         <v>19</v>
       </c>
-      <c r="J76">
-        <f t="shared" si="7"/>
-        <v>13</v>
-      </c>
-      <c r="K76" t="str">
-        <f>REPT(" ",J76)</f>
-        <v xml:space="preserve">             </v>
-      </c>
-    </row>
-    <row r="78" spans="2:11">
-      <c r="B78" s="3"/>
-      <c r="C78"/>
-      <c r="G78" t="str">
-        <f t="shared" ref="G73:G138" si="8">CONCATENATE(B78," ",C78,K78,"\\")</f>
-        <v xml:space="preserve">                                \\</v>
-      </c>
-      <c r="I78">
-        <f t="shared" ref="I73:I138" si="9">LEN(B78) + LEN(C78) +1</f>
-        <v>1</v>
-      </c>
-      <c r="J78">
-        <f t="shared" ref="J73:J138" si="10">IF(I78&lt;30,(32-I78),3)</f>
-        <v>31</v>
-      </c>
       <c r="K78" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">                               </v>
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">                   </v>
       </c>
     </row>
     <row r="79" spans="2:11">
       <c r="B79" t="s">
-        <v>156</v>
-      </c>
-      <c r="C79" t="s">
-        <v>157</v>
+        <v>160</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>161</v>
       </c>
       <c r="D79" t="s">
         <v>158</v>
       </c>
       <c r="E79" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="G79" t="str">
-        <f t="shared" si="8"/>
-        <v>Zeeshan Ahmed                   \\</v>
+        <f t="shared" si="4"/>
+        <v>Jason Austermann                \\</v>
       </c>
       <c r="I79">
-        <f t="shared" si="9"/>
-        <v>13</v>
+        <f t="shared" si="5"/>
+        <v>16</v>
       </c>
       <c r="J79">
-        <f t="shared" si="10"/>
-        <v>19</v>
+        <f t="shared" si="6"/>
+        <v>16</v>
       </c>
       <c r="K79" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">                   </v>
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">                </v>
       </c>
     </row>
     <row r="80" spans="2:11">
       <c r="B80" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="D80" t="s">
         <v>158</v>
       </c>
       <c r="E80" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="G80" t="str">
-        <f t="shared" ref="G80:G132" si="11">CONCATENATE(B80," ",C80,K80,"\\")</f>
-        <v>Jason Austermann                \\</v>
+        <f t="shared" si="4"/>
+        <v>Darcy Barron                    \\</v>
       </c>
       <c r="I80">
-        <f t="shared" ref="I80:I132" si="12">LEN(B80) + LEN(C80) +1</f>
-        <v>16</v>
+        <f t="shared" si="5"/>
+        <v>12</v>
       </c>
       <c r="J80">
-        <f t="shared" ref="J80:J132" si="13">IF(I80&lt;30,(32-I80),3)</f>
-        <v>16</v>
+        <f t="shared" si="6"/>
+        <v>20</v>
       </c>
       <c r="K80" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">                </v>
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">                    </v>
       </c>
     </row>
     <row r="81" spans="2:11">
       <c r="B81" t="s">
-        <v>163</v>
-      </c>
-      <c r="C81" s="1" t="s">
-        <v>164</v>
+        <v>166</v>
+      </c>
+      <c r="C81" t="s">
+        <v>167</v>
       </c>
       <c r="D81" t="s">
         <v>158</v>
       </c>
-      <c r="E81" t="s">
-        <v>165</v>
-      </c>
       <c r="G81" t="str">
-        <f t="shared" si="11"/>
-        <v>Darcy Barron                    \\</v>
+        <f t="shared" si="4"/>
+        <v>Karim Benabed                   \\</v>
       </c>
       <c r="I81">
-        <f t="shared" si="12"/>
-        <v>12</v>
+        <f t="shared" si="5"/>
+        <v>13</v>
       </c>
       <c r="J81">
-        <f t="shared" si="13"/>
-        <v>20</v>
+        <f t="shared" si="6"/>
+        <v>19</v>
       </c>
       <c r="K81" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">                    </v>
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">                   </v>
       </c>
     </row>
     <row r="82" spans="2:11">
       <c r="B82" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="C82" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="D82" t="s">
         <v>158</v>
       </c>
+      <c r="E82" t="s">
+        <v>170</v>
+      </c>
       <c r="G82" t="str">
-        <f t="shared" si="11"/>
-        <v>Karim Benabed                   \\</v>
+        <f t="shared" si="4"/>
+        <v>Federico Bianchini              \\</v>
       </c>
       <c r="I82">
-        <f t="shared" si="12"/>
-        <v>13</v>
+        <f t="shared" si="5"/>
+        <v>18</v>
       </c>
       <c r="J82">
-        <f t="shared" si="13"/>
-        <v>19</v>
+        <f t="shared" si="6"/>
+        <v>14</v>
       </c>
       <c r="K82" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">                   </v>
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">              </v>
       </c>
     </row>
     <row r="83" spans="2:11">
-      <c r="B83" t="s">
-        <v>168</v>
-      </c>
-      <c r="C83" t="s">
-        <v>169</v>
+      <c r="B83" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>296</v>
       </c>
       <c r="D83" t="s">
         <v>158</v>
       </c>
       <c r="E83" t="s">
-        <v>170</v>
+        <v>284</v>
       </c>
       <c r="G83" t="str">
-        <f t="shared" si="11"/>
-        <v>Federico Bianchini              \\</v>
+        <f t="shared" si="4"/>
+        <v>Colin Bischoff                  \\</v>
       </c>
       <c r="I83">
-        <f t="shared" si="12"/>
+        <f t="shared" si="5"/>
+        <v>14</v>
+      </c>
+      <c r="J83">
+        <f t="shared" si="6"/>
         <v>18</v>
       </c>
-      <c r="J83">
-        <f t="shared" si="13"/>
-        <v>14</v>
-      </c>
       <c r="K83" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">              </v>
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">                  </v>
       </c>
     </row>
     <row r="84" spans="2:11">
-      <c r="B84" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C84" s="1" t="s">
-        <v>295</v>
+      <c r="B84" t="s">
+        <v>174</v>
+      </c>
+      <c r="C84" t="s">
+        <v>175</v>
       </c>
       <c r="D84" t="s">
         <v>158</v>
       </c>
       <c r="E84" t="s">
-        <v>283</v>
+        <v>176</v>
       </c>
       <c r="G84" t="str">
-        <f t="shared" si="11"/>
-        <v>Colin Bischoff                  \\</v>
+        <f t="shared" si="4"/>
+        <v>J. Richard Bond                 \\</v>
       </c>
       <c r="I84">
-        <f t="shared" si="12"/>
-        <v>14</v>
+        <f t="shared" si="5"/>
+        <v>15</v>
       </c>
       <c r="J84">
-        <f t="shared" si="13"/>
-        <v>18</v>
+        <f t="shared" si="6"/>
+        <v>17</v>
       </c>
       <c r="K84" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">                  </v>
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">                 </v>
       </c>
     </row>
     <row r="85" spans="2:11">
-      <c r="B85" t="s">
-        <v>174</v>
-      </c>
-      <c r="C85" t="s">
-        <v>175</v>
+      <c r="B85" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>294</v>
       </c>
       <c r="D85" t="s">
         <v>158</v>
       </c>
       <c r="E85" t="s">
-        <v>176</v>
+        <v>282</v>
       </c>
       <c r="G85" t="str">
-        <f t="shared" si="11"/>
-        <v>J. Richard Bond                 \\</v>
+        <f t="shared" si="4"/>
+        <v>Robert Caldwell                 \\</v>
       </c>
       <c r="I85">
-        <f t="shared" si="12"/>
+        <f t="shared" si="5"/>
         <v>15</v>
       </c>
       <c r="J85">
-        <f t="shared" si="13"/>
+        <f t="shared" si="6"/>
         <v>17</v>
       </c>
       <c r="K85" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v xml:space="preserve">                 </v>
       </c>
     </row>
     <row r="86" spans="2:11">
-      <c r="B86" s="1" t="s">
-        <v>314</v>
+      <c r="B86" t="s">
+        <v>177</v>
       </c>
       <c r="C86" t="s">
-        <v>195</v>
+        <v>178</v>
       </c>
       <c r="D86" t="s">
         <v>158</v>
       </c>
       <c r="E86" t="s">
-        <v>84</v>
+        <v>135</v>
       </c>
       <c r="G86" t="str">
-        <f t="shared" si="11"/>
-        <v>Fran\c{c}ois Bouchet            \\</v>
+        <f t="shared" si="4"/>
+        <v>Xingang Chen                    \\</v>
       </c>
       <c r="I86">
-        <f t="shared" si="12"/>
+        <f t="shared" si="5"/>
+        <v>12</v>
+      </c>
+      <c r="J86">
+        <f t="shared" si="6"/>
         <v>20</v>
       </c>
-      <c r="J86">
-        <f t="shared" si="13"/>
-        <v>12</v>
-      </c>
       <c r="K86" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">            </v>
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">                    </v>
       </c>
     </row>
     <row r="87" spans="2:11">
-      <c r="B87" s="1" t="s">
-        <v>292</v>
-      </c>
-      <c r="C87" s="1" t="s">
-        <v>293</v>
+      <c r="B87" t="s">
+        <v>179</v>
+      </c>
+      <c r="C87" t="s">
+        <v>180</v>
       </c>
       <c r="D87" t="s">
         <v>158</v>
       </c>
       <c r="E87" t="s">
-        <v>281</v>
+        <v>181</v>
       </c>
       <c r="G87" t="str">
-        <f t="shared" si="11"/>
-        <v>Robert Caldwell                 \\</v>
+        <f t="shared" si="4"/>
+        <v>Jens Chluba                     \\</v>
       </c>
       <c r="I87">
-        <f t="shared" si="12"/>
-        <v>15</v>
+        <f t="shared" si="5"/>
+        <v>11</v>
       </c>
       <c r="J87">
-        <f t="shared" si="13"/>
-        <v>17</v>
+        <f t="shared" si="6"/>
+        <v>21</v>
       </c>
       <c r="K87" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">                 </v>
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">                     </v>
       </c>
     </row>
     <row r="88" spans="2:11">
       <c r="B88" t="s">
-        <v>177</v>
-      </c>
-      <c r="C88" t="s">
-        <v>178</v>
+        <v>182</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>183</v>
       </c>
       <c r="D88" t="s">
         <v>158</v>
       </c>
       <c r="E88" t="s">
-        <v>135</v>
+        <v>184</v>
       </c>
       <c r="G88" t="str">
-        <f t="shared" si="11"/>
-        <v>Xingang Chen                    \\</v>
+        <f t="shared" si="4"/>
+        <v>Francis-Yan Cyr-Racine          \\</v>
       </c>
       <c r="I88">
-        <f t="shared" si="12"/>
-        <v>12</v>
+        <f t="shared" si="5"/>
+        <v>22</v>
       </c>
       <c r="J88">
-        <f t="shared" si="13"/>
-        <v>20</v>
+        <f t="shared" si="6"/>
+        <v>10</v>
       </c>
       <c r="K88" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">                    </v>
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">          </v>
       </c>
     </row>
     <row r="89" spans="2:11">
       <c r="B89" t="s">
-        <v>179</v>
-      </c>
-      <c r="C89" t="s">
-        <v>180</v>
+        <v>185</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>186</v>
       </c>
       <c r="D89" t="s">
         <v>158</v>
       </c>
       <c r="E89" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="G89" t="str">
-        <f t="shared" si="11"/>
-        <v>Jens Chluba                     \\</v>
+        <f t="shared" si="4"/>
+        <v>Tijmen de Haan                  \\</v>
       </c>
       <c r="I89">
-        <f t="shared" si="12"/>
-        <v>11</v>
+        <f t="shared" si="5"/>
+        <v>14</v>
       </c>
       <c r="J89">
-        <f t="shared" si="13"/>
-        <v>21</v>
+        <f t="shared" si="6"/>
+        <v>18</v>
       </c>
       <c r="K89" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">                     </v>
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">                  </v>
       </c>
     </row>
     <row r="90" spans="2:11">
       <c r="B90" t="s">
-        <v>182</v>
-      </c>
-      <c r="C90" s="1" t="s">
-        <v>183</v>
+        <v>188</v>
+      </c>
+      <c r="C90" t="s">
+        <v>320</v>
       </c>
       <c r="D90" t="s">
         <v>158</v>
       </c>
       <c r="E90" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="G90" t="str">
-        <f t="shared" si="11"/>
-        <v>Francis-Yan Cyr-Racine          \\</v>
+        <f>CONCATENATE(C90," ",B90,K90,"\\")</f>
+        <v>Shirokoff Erik                  \\</v>
       </c>
       <c r="I90">
-        <f t="shared" si="12"/>
-        <v>22</v>
+        <f>LEN(C90) + LEN(B90) +1</f>
+        <v>14</v>
       </c>
       <c r="J90">
-        <f t="shared" si="13"/>
-        <v>10</v>
+        <f t="shared" si="6"/>
+        <v>18</v>
       </c>
       <c r="K90" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">          </v>
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">                  </v>
       </c>
     </row>
     <row r="91" spans="2:11">
       <c r="B91" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
       <c r="D91" t="s">
         <v>158</v>
       </c>
       <c r="E91" t="s">
-        <v>187</v>
+        <v>93</v>
       </c>
       <c r="G91" t="str">
-        <f t="shared" si="11"/>
-        <v>Tijmen de Haan                  \\</v>
+        <f t="shared" si="4"/>
+        <v>Aurelien Fraisse                \\</v>
       </c>
       <c r="I91">
-        <f t="shared" si="12"/>
-        <v>14</v>
+        <f t="shared" si="5"/>
+        <v>16</v>
       </c>
       <c r="J91">
-        <f t="shared" si="13"/>
-        <v>18</v>
+        <f t="shared" si="6"/>
+        <v>16</v>
       </c>
       <c r="K91" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">                  </v>
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">                </v>
       </c>
     </row>
     <row r="92" spans="2:11">
-      <c r="B92" t="s">
-        <v>190</v>
-      </c>
-      <c r="C92" s="1" t="s">
-        <v>191</v>
+      <c r="B92" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="C92" t="s">
+        <v>192</v>
       </c>
       <c r="D92" t="s">
         <v>158</v>
       </c>
       <c r="E92" t="s">
-        <v>93</v>
+        <v>194</v>
       </c>
       <c r="G92" t="str">
-        <f t="shared" si="11"/>
-        <v>Aurelien Fraisse                \\</v>
+        <f>CONCATENATE(C92," ",B92,K92,"\\")</f>
+        <v>Piacentini Francesco            \\</v>
       </c>
       <c r="I92">
-        <f t="shared" si="12"/>
-        <v>16</v>
+        <f>LEN(C92) + LEN(B92) +1</f>
+        <v>20</v>
       </c>
       <c r="J92">
-        <f t="shared" si="13"/>
-        <v>16</v>
+        <f t="shared" si="6"/>
+        <v>12</v>
       </c>
       <c r="K92" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">                </v>
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">            </v>
       </c>
     </row>
     <row r="93" spans="2:11">
-      <c r="B93" t="s">
-        <v>196</v>
-      </c>
-      <c r="C93" s="1" t="s">
-        <v>197</v>
+      <c r="B93" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="C93" t="s">
+        <v>195</v>
       </c>
       <c r="D93" t="s">
         <v>158</v>
       </c>
       <c r="E93" t="s">
-        <v>198</v>
+        <v>84</v>
       </c>
       <c r="G93" t="str">
-        <f t="shared" si="11"/>
-        <v>Silvia Galli                    \\</v>
+        <f>CONCATENATE(C93," ",B93,K93,"\\")</f>
+        <v>Bouchet Fran\c{c}ois            \\</v>
       </c>
       <c r="I93">
-        <f t="shared" si="12"/>
+        <f>LEN(C93) + LEN(B93) +1</f>
+        <v>20</v>
+      </c>
+      <c r="J93">
+        <f t="shared" si="6"/>
         <v>12</v>
       </c>
-      <c r="J93">
-        <f t="shared" si="13"/>
-        <v>20</v>
-      </c>
       <c r="K93" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">                    </v>
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">            </v>
       </c>
     </row>
     <row r="94" spans="2:11">
       <c r="B94" t="s">
-        <v>199</v>
-      </c>
-      <c r="C94" t="s">
-        <v>200</v>
+        <v>196</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>197</v>
       </c>
       <c r="D94" t="s">
         <v>158</v>
       </c>
       <c r="E94" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="G94" t="str">
-        <f t="shared" si="11"/>
-        <v>Ken Ganga                       \\</v>
+        <f t="shared" si="4"/>
+        <v>Silvia Galli                    \\</v>
       </c>
       <c r="I94">
-        <f t="shared" si="12"/>
-        <v>9</v>
+        <f t="shared" si="5"/>
+        <v>12</v>
       </c>
       <c r="J94">
-        <f t="shared" si="13"/>
-        <v>23</v>
+        <f t="shared" si="6"/>
+        <v>20</v>
       </c>
       <c r="K94" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">                       </v>
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">                    </v>
       </c>
     </row>
     <row r="95" spans="2:11">
       <c r="B95" t="s">
-        <v>202</v>
-      </c>
-      <c r="C95" s="1" t="s">
-        <v>203</v>
+        <v>199</v>
+      </c>
+      <c r="C95" t="s">
+        <v>200</v>
       </c>
       <c r="D95" t="s">
         <v>158</v>
       </c>
       <c r="E95" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="G95" t="str">
-        <f t="shared" si="11"/>
-        <v>Tuhin Ghosh                     \\</v>
+        <f t="shared" si="4"/>
+        <v>Ken Ganga                       \\</v>
       </c>
       <c r="I95">
-        <f t="shared" si="12"/>
-        <v>11</v>
+        <f t="shared" si="5"/>
+        <v>9</v>
       </c>
       <c r="J95">
-        <f t="shared" si="13"/>
-        <v>21</v>
+        <f t="shared" si="6"/>
+        <v>23</v>
       </c>
       <c r="K95" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">                     </v>
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">                       </v>
       </c>
     </row>
     <row r="96" spans="2:11">
       <c r="B96" t="s">
-        <v>205</v>
-      </c>
-      <c r="C96" t="s">
-        <v>206</v>
+        <v>202</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>203</v>
       </c>
       <c r="D96" t="s">
         <v>158</v>
       </c>
       <c r="E96" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="G96" t="str">
-        <f t="shared" si="11"/>
-        <v>Jon E. Gudmundsson              \\</v>
+        <f t="shared" si="4"/>
+        <v>Tuhin Ghosh                     \\</v>
       </c>
       <c r="I96">
-        <f t="shared" si="12"/>
-        <v>18</v>
+        <f t="shared" si="5"/>
+        <v>11</v>
       </c>
       <c r="J96">
-        <f t="shared" si="13"/>
-        <v>14</v>
+        <f t="shared" si="6"/>
+        <v>21</v>
       </c>
       <c r="K96" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">              </v>
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">                     </v>
       </c>
     </row>
     <row r="97" spans="2:11">
       <c r="B97" t="s">
-        <v>208</v>
-      </c>
-      <c r="C97" s="1" t="s">
-        <v>209</v>
+        <v>205</v>
+      </c>
+      <c r="C97" t="s">
+        <v>206</v>
       </c>
       <c r="D97" t="s">
         <v>158</v>
       </c>
       <c r="E97" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="G97" t="str">
-        <f t="shared" si="11"/>
-        <v>Marc Kamionkowski               \\</v>
+        <f t="shared" si="4"/>
+        <v>Jon E. Gudmundsson              \\</v>
       </c>
       <c r="I97">
-        <f t="shared" si="12"/>
-        <v>17</v>
+        <f t="shared" si="5"/>
+        <v>18</v>
       </c>
       <c r="J97">
-        <f t="shared" si="13"/>
-        <v>15</v>
+        <f t="shared" si="6"/>
+        <v>14</v>
       </c>
       <c r="K97" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">               </v>
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">              </v>
       </c>
     </row>
     <row r="98" spans="2:11">
       <c r="B98" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="D98" t="s">
         <v>158</v>
       </c>
       <c r="E98" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="G98" t="str">
-        <f t="shared" si="11"/>
-        <v>Reijo Keskitalo                 \\</v>
+        <f t="shared" si="4"/>
+        <v>Marc Kamionkowski               \\</v>
       </c>
       <c r="I98">
-        <f t="shared" si="12"/>
+        <f t="shared" si="5"/>
+        <v>17</v>
+      </c>
+      <c r="J98">
+        <f t="shared" si="6"/>
         <v>15</v>
       </c>
-      <c r="J98">
-        <f t="shared" si="13"/>
-        <v>17</v>
-      </c>
       <c r="K98" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">                 </v>
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">               </v>
       </c>
     </row>
     <row r="99" spans="2:11">
       <c r="B99" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="D99" t="s">
         <v>158</v>
       </c>
       <c r="E99" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="G99" t="str">
-        <f t="shared" si="11"/>
-        <v>Rishi Khatri                    \\</v>
+        <f t="shared" si="4"/>
+        <v>Reijo Keskitalo                 \\</v>
       </c>
       <c r="I99">
-        <f t="shared" si="12"/>
-        <v>12</v>
+        <f t="shared" si="5"/>
+        <v>15</v>
       </c>
       <c r="J99">
-        <f t="shared" si="13"/>
-        <v>20</v>
+        <f t="shared" si="6"/>
+        <v>17</v>
       </c>
       <c r="K99" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">                    </v>
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">                 </v>
       </c>
     </row>
     <row r="100" spans="2:11">
       <c r="B100" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="D100" t="s">
         <v>158</v>
       </c>
       <c r="E100" t="s">
-        <v>210</v>
+        <v>216</v>
       </c>
       <c r="G100" t="str">
-        <f t="shared" si="11"/>
-        <v>Ely Kovetz                      \\</v>
+        <f t="shared" si="4"/>
+        <v>Rishi Khatri                    \\</v>
       </c>
       <c r="I100">
-        <f t="shared" si="12"/>
-        <v>10</v>
+        <f t="shared" si="5"/>
+        <v>12</v>
       </c>
       <c r="J100">
-        <f t="shared" si="13"/>
-        <v>22</v>
+        <f t="shared" si="6"/>
+        <v>20</v>
       </c>
       <c r="K100" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">                      </v>
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">                    </v>
       </c>
     </row>
     <row r="101" spans="2:11">
       <c r="B101" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D101" t="s">
         <v>158</v>
       </c>
       <c r="E101" t="s">
-        <v>221</v>
+        <v>210</v>
       </c>
       <c r="G101" t="str">
-        <f t="shared" si="11"/>
-        <v>Daniel Lenz                     \\</v>
+        <f t="shared" si="4"/>
+        <v>Ely Kovetz                      \\</v>
       </c>
       <c r="I101">
-        <f t="shared" si="12"/>
-        <v>11</v>
+        <f t="shared" si="5"/>
+        <v>10</v>
       </c>
       <c r="J101">
-        <f t="shared" si="13"/>
-        <v>21</v>
+        <f t="shared" si="6"/>
+        <v>22</v>
       </c>
       <c r="K101" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">                     </v>
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">                      </v>
       </c>
     </row>
     <row r="102" spans="2:11">
       <c r="B102" t="s">
-        <v>222</v>
-      </c>
-      <c r="C102" t="s">
-        <v>223</v>
+        <v>219</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>220</v>
       </c>
       <c r="D102" t="s">
         <v>158</v>
       </c>
       <c r="E102" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="G102" t="str">
-        <f t="shared" si="11"/>
-        <v>Marilena Loverde                \\</v>
+        <f t="shared" si="4"/>
+        <v>Daniel Lenz                     \\</v>
       </c>
       <c r="I102">
-        <f t="shared" si="12"/>
-        <v>16</v>
+        <f t="shared" si="5"/>
+        <v>11</v>
       </c>
       <c r="J102">
-        <f t="shared" si="13"/>
-        <v>16</v>
+        <f t="shared" si="6"/>
+        <v>21</v>
       </c>
       <c r="K102" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">                </v>
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">                     </v>
       </c>
     </row>
     <row r="103" spans="2:11">
       <c r="B103" t="s">
-        <v>225</v>
-      </c>
-      <c r="C103" s="1" t="s">
-        <v>226</v>
+        <v>222</v>
+      </c>
+      <c r="C103" t="s">
+        <v>223</v>
       </c>
       <c r="D103" t="s">
         <v>158</v>
       </c>
       <c r="E103" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="G103" t="str">
-        <f t="shared" si="11"/>
-        <v>Carlos Martins                  \\</v>
+        <f t="shared" si="4"/>
+        <v>Marilena Loverde                \\</v>
       </c>
       <c r="I103">
-        <f t="shared" si="12"/>
-        <v>14</v>
+        <f t="shared" si="5"/>
+        <v>16</v>
       </c>
       <c r="J103">
-        <f t="shared" si="13"/>
-        <v>18</v>
+        <f t="shared" si="6"/>
+        <v>16</v>
       </c>
       <c r="K103" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">                  </v>
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">                </v>
       </c>
     </row>
     <row r="104" spans="2:11">
       <c r="B104" t="s">
-        <v>196</v>
-      </c>
-      <c r="C104" t="s">
-        <v>228</v>
+        <v>225</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>226</v>
       </c>
       <c r="D104" t="s">
         <v>158</v>
       </c>
       <c r="E104" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="G104" t="str">
-        <f t="shared" si="11"/>
-        <v>Silvia Masi                     \\</v>
+        <f t="shared" si="4"/>
+        <v>Carlos Martins                  \\</v>
       </c>
       <c r="I104">
-        <f t="shared" si="12"/>
-        <v>11</v>
+        <f t="shared" si="5"/>
+        <v>14</v>
       </c>
       <c r="J104">
-        <f t="shared" si="13"/>
-        <v>21</v>
+        <f t="shared" si="6"/>
+        <v>18</v>
       </c>
       <c r="K104" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">                     </v>
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">                  </v>
       </c>
     </row>
     <row r="105" spans="2:11">
-      <c r="B105" s="1" t="s">
-        <v>297</v>
-      </c>
-      <c r="C105" s="1" t="s">
-        <v>298</v>
+      <c r="B105" t="s">
+        <v>196</v>
+      </c>
+      <c r="C105" t="s">
+        <v>228</v>
       </c>
       <c r="D105" t="s">
         <v>158</v>
       </c>
       <c r="E105" t="s">
-        <v>285</v>
+        <v>229</v>
       </c>
       <c r="G105" t="str">
-        <f t="shared" si="11"/>
-        <v>Joel Meyers                     \\</v>
+        <f t="shared" si="4"/>
+        <v>Silvia Masi                     \\</v>
       </c>
       <c r="I105">
-        <f t="shared" si="12"/>
+        <f t="shared" si="5"/>
         <v>11</v>
       </c>
       <c r="J105">
-        <f t="shared" si="13"/>
+        <f t="shared" si="6"/>
         <v>21</v>
       </c>
       <c r="K105" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v xml:space="preserve">                     </v>
       </c>
     </row>
     <row r="106" spans="2:11">
-      <c r="B106" t="s">
-        <v>230</v>
+      <c r="B106" s="1" t="s">
+        <v>298</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>231</v>
+        <v>299</v>
       </c>
       <c r="D106" t="s">
         <v>158</v>
       </c>
       <c r="E106" t="s">
-        <v>232</v>
+        <v>286</v>
       </c>
       <c r="G106" t="str">
-        <f t="shared" si="11"/>
-        <v>Lorenzo Moncelsi                \\</v>
+        <f t="shared" si="4"/>
+        <v>Joel Meyers                     \\</v>
       </c>
       <c r="I106">
-        <f t="shared" si="12"/>
-        <v>16</v>
+        <f t="shared" si="5"/>
+        <v>11</v>
       </c>
       <c r="J106">
-        <f t="shared" si="13"/>
-        <v>16</v>
+        <f t="shared" si="6"/>
+        <v>21</v>
       </c>
       <c r="K106" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">                </v>
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">                     </v>
       </c>
     </row>
     <row r="107" spans="2:11">
       <c r="B107" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="D107" t="s">
         <v>158</v>
       </c>
       <c r="E107" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="G107" t="str">
-        <f t="shared" si="11"/>
-        <v>Pavel Motloch                   \\</v>
+        <f t="shared" si="4"/>
+        <v>Lorenzo Moncelsi                \\</v>
       </c>
       <c r="I107">
-        <f t="shared" si="12"/>
-        <v>13</v>
+        <f t="shared" si="5"/>
+        <v>16</v>
       </c>
       <c r="J107">
-        <f t="shared" si="13"/>
-        <v>19</v>
+        <f t="shared" si="6"/>
+        <v>16</v>
       </c>
       <c r="K107" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">                   </v>
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">                </v>
       </c>
     </row>
     <row r="108" spans="2:11">
       <c r="B108" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="D108" t="s">
         <v>158</v>
       </c>
       <c r="E108" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="G108" t="str">
-        <f t="shared" si="11"/>
-        <v>Tony Mroczkowski                \\</v>
+        <f t="shared" si="4"/>
+        <v>Pavel Motloch                   \\</v>
       </c>
       <c r="I108">
-        <f t="shared" si="12"/>
-        <v>16</v>
+        <f t="shared" si="5"/>
+        <v>13</v>
       </c>
       <c r="J108">
-        <f t="shared" si="13"/>
-        <v>16</v>
+        <f t="shared" si="6"/>
+        <v>19</v>
       </c>
       <c r="K108" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">                </v>
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">                   </v>
       </c>
     </row>
     <row r="109" spans="2:11">
       <c r="B109" t="s">
-        <v>233</v>
-      </c>
-      <c r="C109" t="s">
-        <v>239</v>
+        <v>236</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>237</v>
       </c>
       <c r="D109" t="s">
         <v>158</v>
       </c>
       <c r="E109" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="G109" t="str">
-        <f t="shared" si="11"/>
-        <v>Pavel Naselsky                  \\</v>
+        <f t="shared" si="4"/>
+        <v>Tony Mroczkowski                \\</v>
       </c>
       <c r="I109">
-        <f t="shared" si="12"/>
-        <v>14</v>
+        <f t="shared" si="5"/>
+        <v>16</v>
       </c>
       <c r="J109">
-        <f t="shared" si="13"/>
-        <v>18</v>
+        <f t="shared" si="6"/>
+        <v>16</v>
       </c>
       <c r="K109" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">                  </v>
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">                </v>
       </c>
     </row>
     <row r="110" spans="2:11">
       <c r="B110" t="s">
-        <v>168</v>
-      </c>
-      <c r="C110" s="1" t="s">
-        <v>241</v>
+        <v>233</v>
+      </c>
+      <c r="C110" t="s">
+        <v>239</v>
       </c>
       <c r="D110" t="s">
         <v>158</v>
       </c>
       <c r="E110" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="G110" t="str">
-        <f t="shared" si="11"/>
-        <v>Federico Nati                   \\</v>
+        <f t="shared" si="4"/>
+        <v>Pavel Naselsky                  \\</v>
       </c>
       <c r="I110">
-        <f t="shared" si="12"/>
-        <v>13</v>
+        <f t="shared" si="5"/>
+        <v>14</v>
       </c>
       <c r="J110">
-        <f t="shared" si="13"/>
-        <v>19</v>
+        <f t="shared" si="6"/>
+        <v>18</v>
       </c>
       <c r="K110" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">                   </v>
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">                  </v>
       </c>
     </row>
     <row r="111" spans="2:11">
       <c r="B111" t="s">
-        <v>243</v>
-      </c>
-      <c r="C111" t="s">
-        <v>244</v>
+        <v>168</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>241</v>
       </c>
       <c r="D111" t="s">
         <v>158</v>
       </c>
       <c r="E111" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="G111" t="str">
-        <f t="shared" si="11"/>
-        <v>Elena Orlando                   \\</v>
+        <f t="shared" si="4"/>
+        <v>Federico Nati                   \\</v>
       </c>
       <c r="I111">
-        <f t="shared" si="12"/>
+        <f t="shared" si="5"/>
         <v>13</v>
       </c>
       <c r="J111">
-        <f t="shared" si="13"/>
+        <f t="shared" si="6"/>
         <v>19</v>
       </c>
       <c r="K111" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v xml:space="preserve">                   </v>
       </c>
     </row>
     <row r="112" spans="2:11">
-      <c r="B112" s="1" t="s">
-        <v>193</v>
+      <c r="B112" t="s">
+        <v>243</v>
       </c>
       <c r="C112" t="s">
-        <v>192</v>
+        <v>244</v>
       </c>
       <c r="D112" t="s">
         <v>158</v>
       </c>
       <c r="E112" t="s">
-        <v>194</v>
+        <v>245</v>
       </c>
       <c r="G112" t="str">
-        <f t="shared" si="11"/>
-        <v>Francesco Piacentini            \\</v>
+        <f t="shared" si="4"/>
+        <v>Elena Orlando                   \\</v>
       </c>
       <c r="I112">
-        <f t="shared" si="12"/>
-        <v>20</v>
+        <f t="shared" si="5"/>
+        <v>13</v>
       </c>
       <c r="J112">
-        <f t="shared" si="13"/>
-        <v>12</v>
+        <f t="shared" si="6"/>
+        <v>19</v>
       </c>
       <c r="K112" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">            </v>
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">                   </v>
       </c>
     </row>
     <row r="113" spans="2:11">
@@ -4467,178 +4478,175 @@
         <v>248</v>
       </c>
       <c r="G113" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="4"/>
         <v>Giuseppe Puglisi                \\</v>
       </c>
       <c r="I113">
-        <f t="shared" si="12"/>
+        <f t="shared" si="5"/>
         <v>16</v>
       </c>
       <c r="J113">
-        <f t="shared" si="13"/>
+        <f t="shared" si="6"/>
         <v>16</v>
       </c>
       <c r="K113" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v xml:space="preserve">                </v>
       </c>
     </row>
     <row r="114" spans="2:11">
-      <c r="B114" s="1" t="s">
-        <v>290</v>
-      </c>
-      <c r="C114" s="1" t="s">
-        <v>321</v>
+      <c r="B114" t="s">
+        <v>249</v>
+      </c>
+      <c r="C114" t="s">
+        <v>250</v>
       </c>
       <c r="D114" t="s">
         <v>158</v>
       </c>
       <c r="E114" t="s">
-        <v>320</v>
+        <v>170</v>
       </c>
       <c r="G114" t="str">
-        <f t="shared" si="11"/>
-        <v>Benjamin Racine                 \\</v>
+        <f t="shared" si="4"/>
+        <v>Christian Reichardt             \\</v>
       </c>
       <c r="I114">
-        <f t="shared" si="12"/>
-        <v>15</v>
+        <f t="shared" si="5"/>
+        <v>19</v>
       </c>
       <c r="J114">
-        <f t="shared" si="13"/>
-        <v>17</v>
+        <f t="shared" si="6"/>
+        <v>13</v>
       </c>
       <c r="K114" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">                 </v>
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">             </v>
       </c>
     </row>
     <row r="115" spans="2:11">
       <c r="B115" t="s">
-        <v>249</v>
-      </c>
-      <c r="C115" t="s">
-        <v>250</v>
+        <v>251</v>
+      </c>
+      <c r="C115" s="1" t="s">
+        <v>252</v>
       </c>
       <c r="D115" t="s">
         <v>158</v>
       </c>
       <c r="E115" t="s">
-        <v>170</v>
+        <v>253</v>
       </c>
       <c r="G115" t="str">
-        <f t="shared" si="11"/>
-        <v>Christian Reichardt             \\</v>
+        <f t="shared" si="4"/>
+        <v>Anirban Roy                     \\</v>
       </c>
       <c r="I115">
-        <f t="shared" si="12"/>
-        <v>19</v>
+        <f t="shared" si="5"/>
+        <v>11</v>
       </c>
       <c r="J115">
-        <f t="shared" si="13"/>
-        <v>13</v>
+        <f t="shared" si="6"/>
+        <v>21</v>
       </c>
       <c r="K115" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">             </v>
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">                     </v>
       </c>
     </row>
     <row r="116" spans="2:11">
       <c r="B116" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="D116" t="s">
         <v>158</v>
       </c>
       <c r="E116" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="G116" t="str">
-        <f t="shared" si="11"/>
-        <v>Anirban Roy                     \\</v>
+        <f t="shared" si="4"/>
+        <v>Maria Salatino                  \\</v>
       </c>
       <c r="I116">
-        <f t="shared" si="12"/>
-        <v>11</v>
+        <f t="shared" si="5"/>
+        <v>14</v>
       </c>
       <c r="J116">
-        <f t="shared" si="13"/>
-        <v>21</v>
+        <f t="shared" si="6"/>
+        <v>18</v>
       </c>
       <c r="K116" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">                     </v>
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">                  </v>
       </c>
     </row>
     <row r="117" spans="2:11">
-      <c r="B117" t="s">
-        <v>254</v>
+      <c r="B117" s="1" t="s">
+        <v>291</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>255</v>
+        <v>292</v>
       </c>
       <c r="D117" t="s">
         <v>158</v>
       </c>
       <c r="E117" t="s">
-        <v>256</v>
+        <v>281</v>
       </c>
       <c r="G117" t="str">
-        <f t="shared" si="11"/>
-        <v>Maria Salatino                  \\</v>
+        <f t="shared" si="4"/>
+        <v>Benjamin Saliwanchik            \\</v>
       </c>
       <c r="I117">
-        <f t="shared" si="12"/>
-        <v>14</v>
+        <f t="shared" si="5"/>
+        <v>20</v>
       </c>
       <c r="J117">
-        <f t="shared" si="13"/>
-        <v>18</v>
+        <f t="shared" si="6"/>
+        <v>12</v>
       </c>
       <c r="K117" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">                  </v>
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">            </v>
       </c>
     </row>
     <row r="118" spans="2:11">
       <c r="B118" s="1" t="s">
-        <v>290</v>
+        <v>319</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>291</v>
+        <v>271</v>
       </c>
       <c r="D118" t="s">
         <v>158</v>
       </c>
-      <c r="E118" t="s">
-        <v>280</v>
-      </c>
       <c r="G118" t="str">
-        <f t="shared" si="11"/>
-        <v>Benjamin Saliwanchik            \\</v>
+        <f t="shared" si="4"/>
+        <v>Douglas Scott                   \\</v>
       </c>
       <c r="I118">
-        <f t="shared" si="12"/>
-        <v>20</v>
+        <f t="shared" si="5"/>
+        <v>13</v>
       </c>
       <c r="J118">
-        <f t="shared" si="13"/>
-        <v>12</v>
+        <f t="shared" si="6"/>
+        <v>19</v>
       </c>
       <c r="K118" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">            </v>
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">                   </v>
       </c>
     </row>
     <row r="119" spans="2:11">
       <c r="B119" s="1" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="D119" t="s">
         <v>158</v>
@@ -4647,19 +4655,19 @@
         <v>224</v>
       </c>
       <c r="G119" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="4"/>
         <v>Neelima Sehgal                  \\</v>
       </c>
       <c r="I119">
-        <f t="shared" si="12"/>
+        <f t="shared" si="5"/>
         <v>14</v>
       </c>
       <c r="J119">
-        <f t="shared" si="13"/>
+        <f t="shared" si="6"/>
         <v>18</v>
       </c>
       <c r="K119" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v xml:space="preserve">                  </v>
       </c>
     </row>
@@ -4677,1269 +4685,1225 @@
         <v>259</v>
       </c>
       <c r="G120" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="4"/>
         <v>Sarah Shandera                  \\</v>
       </c>
       <c r="I120">
-        <f t="shared" si="12"/>
+        <f t="shared" si="5"/>
         <v>14</v>
       </c>
       <c r="J120">
-        <f t="shared" si="13"/>
+        <f t="shared" si="6"/>
         <v>18</v>
       </c>
       <c r="K120" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v xml:space="preserve">                  </v>
       </c>
     </row>
     <row r="121" spans="2:11">
       <c r="B121" t="s">
-        <v>188</v>
-      </c>
-      <c r="C121" t="s">
-        <v>319</v>
+        <v>260</v>
+      </c>
+      <c r="C121" s="1" t="s">
+        <v>261</v>
       </c>
       <c r="D121" t="s">
         <v>158</v>
       </c>
       <c r="E121" t="s">
-        <v>189</v>
+        <v>262</v>
       </c>
       <c r="G121" t="str">
-        <f t="shared" si="11"/>
-        <v>Erik Shirokoff                  \\</v>
+        <f t="shared" si="4"/>
+        <v>An\v{z}e Slosar                 \\</v>
       </c>
       <c r="I121">
-        <f t="shared" si="12"/>
-        <v>14</v>
+        <f t="shared" si="5"/>
+        <v>15</v>
       </c>
       <c r="J121">
-        <f t="shared" si="13"/>
-        <v>18</v>
+        <f t="shared" si="6"/>
+        <v>17</v>
       </c>
       <c r="K121" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">                  </v>
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">                 </v>
       </c>
     </row>
     <row r="122" spans="2:11">
       <c r="B122" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="D122" t="s">
         <v>158</v>
       </c>
       <c r="E122" t="s">
-        <v>262</v>
+        <v>187</v>
       </c>
       <c r="G122" t="str">
-        <f t="shared" si="11"/>
-        <v>An\v{z}e Slosar                 \\</v>
+        <f t="shared" si="4"/>
+        <v>Aritoki Suzuki                  \\</v>
       </c>
       <c r="I122">
-        <f t="shared" si="12"/>
-        <v>15</v>
+        <f t="shared" si="5"/>
+        <v>14</v>
       </c>
       <c r="J122">
-        <f t="shared" si="13"/>
-        <v>17</v>
+        <f t="shared" si="6"/>
+        <v>18</v>
       </c>
       <c r="K122" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">                 </v>
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">                  </v>
       </c>
     </row>
     <row r="123" spans="2:11">
-      <c r="B123" t="s">
-        <v>263</v>
+      <c r="B123" s="1" t="s">
+        <v>82</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>264</v>
+        <v>300</v>
       </c>
       <c r="D123" t="s">
         <v>158</v>
       </c>
       <c r="E123" t="s">
-        <v>187</v>
+        <v>287</v>
       </c>
       <c r="G123" t="str">
-        <f t="shared" si="11"/>
-        <v>Aritoki Suzuki                  \\</v>
+        <f t="shared" si="4"/>
+        <v>Eric Switzer                    \\</v>
       </c>
       <c r="I123">
-        <f t="shared" si="12"/>
-        <v>14</v>
+        <f t="shared" si="5"/>
+        <v>12</v>
       </c>
       <c r="J123">
-        <f t="shared" si="13"/>
-        <v>18</v>
+        <f t="shared" si="6"/>
+        <v>20</v>
       </c>
       <c r="K123" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">                  </v>
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">                    </v>
       </c>
     </row>
     <row r="124" spans="2:11">
       <c r="B124" s="1" t="s">
-        <v>82</v>
+        <v>154</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="D124" t="s">
         <v>158</v>
       </c>
       <c r="E124" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="G124" t="str">
-        <f t="shared" si="11"/>
-        <v>Eric Switzer                    \\</v>
+        <f t="shared" si="4"/>
+        <v>Andrea Tartari                  \\</v>
       </c>
       <c r="I124">
-        <f t="shared" si="12"/>
-        <v>12</v>
+        <f t="shared" si="5"/>
+        <v>14</v>
       </c>
       <c r="J124">
-        <f t="shared" si="13"/>
-        <v>20</v>
+        <f t="shared" si="6"/>
+        <v>18</v>
       </c>
       <c r="K124" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">                    </v>
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">                  </v>
       </c>
     </row>
     <row r="125" spans="2:11">
-      <c r="B125" s="1" t="s">
-        <v>154</v>
+      <c r="B125" t="s">
+        <v>265</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>300</v>
+        <v>266</v>
       </c>
       <c r="D125" t="s">
         <v>158</v>
       </c>
       <c r="E125" t="s">
-        <v>287</v>
+        <v>267</v>
       </c>
       <c r="G125" t="str">
-        <f t="shared" si="11"/>
-        <v>Andrea Tartari                  \\</v>
+        <f t="shared" si="4"/>
+        <v>Grant Teply                     \\</v>
       </c>
       <c r="I125">
-        <f t="shared" si="12"/>
-        <v>14</v>
+        <f t="shared" si="5"/>
+        <v>11</v>
       </c>
       <c r="J125">
-        <f t="shared" si="13"/>
-        <v>18</v>
+        <f t="shared" si="6"/>
+        <v>21</v>
       </c>
       <c r="K125" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">                  </v>
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">                     </v>
       </c>
     </row>
     <row r="126" spans="2:11">
-      <c r="B126" t="s">
-        <v>265</v>
+      <c r="B126" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>266</v>
+        <v>304</v>
       </c>
       <c r="D126" t="s">
         <v>158</v>
       </c>
       <c r="E126" t="s">
-        <v>267</v>
+        <v>289</v>
       </c>
       <c r="G126" t="str">
-        <f t="shared" si="11"/>
-        <v>Grant Teply                     \\</v>
+        <f t="shared" si="4"/>
+        <v>Peter Timbie                    \\</v>
       </c>
       <c r="I126">
-        <f t="shared" si="12"/>
-        <v>11</v>
+        <f t="shared" si="5"/>
+        <v>12</v>
       </c>
       <c r="J126">
-        <f t="shared" si="13"/>
-        <v>21</v>
+        <f t="shared" si="6"/>
+        <v>20</v>
       </c>
       <c r="K126" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">                     </v>
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">                    </v>
       </c>
     </row>
     <row r="127" spans="2:11">
-      <c r="B127" s="1" t="s">
-        <v>9</v>
+      <c r="B127" t="s">
+        <v>268</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>303</v>
+        <v>269</v>
       </c>
       <c r="D127" t="s">
         <v>158</v>
       </c>
       <c r="E127" t="s">
-        <v>288</v>
+        <v>270</v>
       </c>
       <c r="G127" t="str">
-        <f t="shared" si="11"/>
-        <v>Peter Timbie                    \\</v>
+        <f t="shared" si="4"/>
+        <v>Matthieu Tristram               \\</v>
       </c>
       <c r="I127">
-        <f t="shared" si="12"/>
-        <v>12</v>
+        <f t="shared" si="5"/>
+        <v>17</v>
       </c>
       <c r="J127">
-        <f t="shared" si="13"/>
-        <v>20</v>
+        <f t="shared" si="6"/>
+        <v>15</v>
       </c>
       <c r="K127" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">                    </v>
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">               </v>
       </c>
     </row>
     <row r="128" spans="2:11">
-      <c r="B128" t="s">
-        <v>268</v>
+      <c r="B128" s="1" t="s">
+        <v>291</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>269</v>
+        <v>295</v>
       </c>
       <c r="D128" t="s">
         <v>158</v>
       </c>
       <c r="E128" t="s">
-        <v>270</v>
+        <v>283</v>
       </c>
       <c r="G128" t="str">
-        <f t="shared" si="11"/>
-        <v>Matthieu Tristram               \\</v>
+        <f t="shared" si="4"/>
+        <v>Benjamin Wallisch               \\</v>
       </c>
       <c r="I128">
-        <f t="shared" si="12"/>
+        <f t="shared" si="5"/>
         <v>17</v>
       </c>
       <c r="J128">
-        <f t="shared" si="13"/>
+        <f t="shared" si="6"/>
         <v>15</v>
       </c>
       <c r="K128" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v xml:space="preserve">               </v>
       </c>
     </row>
     <row r="129" spans="2:11">
-      <c r="B129" s="1" t="s">
-        <v>322</v>
+      <c r="B129" t="s">
+        <v>271</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>323</v>
+        <v>272</v>
       </c>
       <c r="D129" t="s">
         <v>158</v>
       </c>
       <c r="E129" t="s">
-        <v>283</v>
+        <v>273</v>
       </c>
       <c r="G129" t="str">
-        <f t="shared" si="11"/>
-        <v>Caterina Umilt\`{a}             \\</v>
+        <f t="shared" si="4"/>
+        <v>Scott Watson                    \\</v>
       </c>
       <c r="I129">
-        <f t="shared" si="12"/>
-        <v>19</v>
+        <f t="shared" si="5"/>
+        <v>12</v>
       </c>
       <c r="J129">
-        <f t="shared" si="13"/>
-        <v>13</v>
+        <f t="shared" si="6"/>
+        <v>20</v>
       </c>
       <c r="K129" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">             </v>
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">                    </v>
       </c>
     </row>
     <row r="130" spans="2:11">
-      <c r="B130" s="1" t="s">
-        <v>290</v>
+      <c r="B130" t="s">
+        <v>274</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>294</v>
+        <v>275</v>
       </c>
       <c r="D130" t="s">
         <v>158</v>
       </c>
       <c r="E130" t="s">
-        <v>282</v>
+        <v>60</v>
       </c>
       <c r="G130" t="str">
-        <f t="shared" si="11"/>
-        <v>Benjamin Wallisch               \\</v>
+        <f t="shared" si="4"/>
+        <v>Edward J. Wollack               \\</v>
       </c>
       <c r="I130">
-        <f t="shared" si="12"/>
+        <f t="shared" si="5"/>
         <v>17</v>
       </c>
       <c r="J130">
-        <f t="shared" si="13"/>
+        <f t="shared" si="6"/>
         <v>15</v>
       </c>
       <c r="K130" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v xml:space="preserve">               </v>
       </c>
     </row>
     <row r="131" spans="2:11">
-      <c r="B131" t="s">
-        <v>271</v>
-      </c>
-      <c r="C131" s="1" t="s">
-        <v>272</v>
-      </c>
-      <c r="D131" t="s">
+      <c r="G131" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">                                \\</v>
+      </c>
+      <c r="I131">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="J131">
+        <f t="shared" si="6"/>
+        <v>31</v>
+      </c>
+      <c r="K131" t="str">
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">                               </v>
+      </c>
+    </row>
+    <row r="132" spans="2:11">
+      <c r="G132" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">                                \\</v>
+      </c>
+      <c r="I132">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="J132">
+        <f t="shared" si="6"/>
+        <v>31</v>
+      </c>
+      <c r="K132" t="str">
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">                               </v>
+      </c>
+    </row>
+    <row r="133" spans="2:11">
+      <c r="G133" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">                                \\</v>
+      </c>
+      <c r="I133">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="J133">
+        <f t="shared" si="6"/>
+        <v>31</v>
+      </c>
+      <c r="K133" t="str">
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">                               </v>
+      </c>
+    </row>
+    <row r="134" spans="2:11">
+      <c r="G134" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">                                \\</v>
+      </c>
+      <c r="I134">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="J134">
+        <f t="shared" si="6"/>
+        <v>31</v>
+      </c>
+      <c r="K134" t="str">
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">                               </v>
+      </c>
+    </row>
+    <row r="135" spans="2:11">
+      <c r="G135" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">                                \\</v>
+      </c>
+      <c r="I135">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="J135">
+        <f t="shared" si="6"/>
+        <v>31</v>
+      </c>
+      <c r="K135" t="str">
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">                               </v>
+      </c>
+    </row>
+    <row r="136" spans="2:11">
+      <c r="G136" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">                                \\</v>
+      </c>
+      <c r="I136">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="J136">
+        <f t="shared" si="6"/>
+        <v>31</v>
+      </c>
+      <c r="K136" t="str">
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">                               </v>
+      </c>
+    </row>
+    <row r="137" spans="2:11">
+      <c r="G137" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">                                \\</v>
+      </c>
+      <c r="I137">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="J137">
+        <f t="shared" si="6"/>
+        <v>31</v>
+      </c>
+      <c r="K137" t="str">
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">                               </v>
+      </c>
+    </row>
+    <row r="138" spans="2:11">
+      <c r="B138" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C138" t="s">
+        <v>149</v>
+      </c>
+      <c r="D138" t="s">
         <v>158</v>
       </c>
-      <c r="E131" t="s">
-        <v>273</v>
-      </c>
-      <c r="G131" t="str">
-        <f t="shared" si="11"/>
-        <v>Scott Watson                    \\</v>
-      </c>
-      <c r="I131">
-        <f t="shared" si="12"/>
+      <c r="G138" t="str">
+        <f t="shared" ref="G138:G179" si="8">CONCATENATE(B138," ",C138,K138,"\\")</f>
+        <v>Martin White                    \\</v>
+      </c>
+      <c r="I138">
+        <f t="shared" ref="I138:I179" si="9">LEN(B138) + LEN(C138) +1</f>
         <v>12</v>
       </c>
-      <c r="J131">
-        <f t="shared" si="13"/>
+      <c r="J138">
+        <f t="shared" ref="J138:J179" si="10">IF(I138&lt;30,(32-I138),3)</f>
         <v>20</v>
       </c>
-      <c r="K131" t="str">
-        <f t="shared" si="4"/>
+      <c r="K138" t="str">
+        <f t="shared" ref="K138:K179" si="11">REPT(" ",J138)</f>
         <v xml:space="preserve">                    </v>
       </c>
     </row>
-    <row r="132" spans="2:11">
-      <c r="B132" t="s">
-        <v>274</v>
-      </c>
-      <c r="C132" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="D132" t="s">
-        <v>158</v>
-      </c>
-      <c r="E132" t="s">
-        <v>60</v>
-      </c>
-      <c r="G132" t="str">
-        <f t="shared" si="11"/>
-        <v>Edward J. Wollack               \\</v>
-      </c>
-      <c r="I132">
-        <f t="shared" si="12"/>
-        <v>17</v>
-      </c>
-      <c r="J132">
-        <f t="shared" si="13"/>
-        <v>15</v>
-      </c>
-      <c r="K132" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">               </v>
-      </c>
-    </row>
-    <row r="133" spans="2:11">
-      <c r="B133" s="3"/>
-      <c r="C133"/>
-      <c r="G133" t="str">
+    <row r="139" spans="2:11">
+      <c r="B139" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C139" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D139" t="s">
+        <v>8</v>
+      </c>
+      <c r="G139" t="str">
+        <f>CONCATENATE(B139," ",C139,K139,"\\")</f>
+        <v>Kim Boddy                       \\</v>
+      </c>
+      <c r="I139">
+        <f>LEN(B139) + LEN(C139) +1</f>
+        <v>9</v>
+      </c>
+      <c r="J139">
+        <f>IF(I139&lt;30,(32-I139),3)</f>
+        <v>23</v>
+      </c>
+      <c r="K139" t="str">
+        <f>REPT(" ",J139)</f>
+        <v xml:space="preserve">                       </v>
+      </c>
+    </row>
+    <row r="140" spans="2:11">
+      <c r="G140" t="str">
         <f t="shared" si="8"/>
         <v xml:space="preserve">                                \\</v>
       </c>
-      <c r="I133">
+      <c r="I140">
         <f t="shared" si="9"/>
         <v>1</v>
       </c>
-      <c r="J133">
+      <c r="J140">
         <f t="shared" si="10"/>
         <v>31</v>
       </c>
-      <c r="K133" t="str">
-        <f t="shared" si="4"/>
+      <c r="K140" t="str">
+        <f t="shared" si="11"/>
         <v xml:space="preserve">                               </v>
       </c>
     </row>
-    <row r="134" spans="2:11">
-      <c r="G134" t="str">
+    <row r="141" spans="2:11">
+      <c r="G141" t="str">
         <f t="shared" si="8"/>
         <v xml:space="preserve">                                \\</v>
       </c>
-      <c r="I134">
+      <c r="I141">
         <f t="shared" si="9"/>
         <v>1</v>
       </c>
-      <c r="J134">
+      <c r="J141">
         <f t="shared" si="10"/>
         <v>31</v>
       </c>
-      <c r="K134" t="str">
-        <f t="shared" si="4"/>
+      <c r="K141" t="str">
+        <f t="shared" si="11"/>
         <v xml:space="preserve">                               </v>
       </c>
     </row>
-    <row r="135" spans="2:11">
-      <c r="G135" t="str">
+    <row r="142" spans="2:11">
+      <c r="G142" t="str">
         <f t="shared" si="8"/>
         <v xml:space="preserve">                                \\</v>
       </c>
-      <c r="I135">
+      <c r="I142">
         <f t="shared" si="9"/>
         <v>1</v>
       </c>
-      <c r="J135">
+      <c r="J142">
         <f t="shared" si="10"/>
         <v>31</v>
       </c>
-      <c r="K135" t="str">
-        <f t="shared" si="4"/>
+      <c r="K142" t="str">
+        <f t="shared" si="11"/>
         <v xml:space="preserve">                               </v>
       </c>
     </row>
-    <row r="136" spans="2:11">
-      <c r="G136" t="str">
+    <row r="143" spans="2:11">
+      <c r="G143" t="str">
         <f t="shared" si="8"/>
         <v xml:space="preserve">                                \\</v>
       </c>
-      <c r="I136">
+      <c r="I143">
         <f t="shared" si="9"/>
         <v>1</v>
       </c>
-      <c r="J136">
+      <c r="J143">
         <f t="shared" si="10"/>
         <v>31</v>
       </c>
-      <c r="K136" t="str">
-        <f t="shared" si="4"/>
+      <c r="K143" t="str">
+        <f t="shared" si="11"/>
         <v xml:space="preserve">                               </v>
       </c>
     </row>
-    <row r="137" spans="2:11">
-      <c r="G137" t="str">
+    <row r="144" spans="2:11">
+      <c r="G144" t="str">
         <f t="shared" si="8"/>
         <v xml:space="preserve">                                \\</v>
       </c>
-      <c r="I137">
+      <c r="I144">
         <f t="shared" si="9"/>
         <v>1</v>
       </c>
-      <c r="J137">
+      <c r="J144">
         <f t="shared" si="10"/>
         <v>31</v>
       </c>
-      <c r="K137" t="str">
-        <f t="shared" si="4"/>
+      <c r="K144" t="str">
+        <f t="shared" si="11"/>
         <v xml:space="preserve">                               </v>
       </c>
     </row>
-    <row r="138" spans="2:11">
-      <c r="G138" t="str">
+    <row r="145" spans="7:11">
+      <c r="G145" t="str">
         <f t="shared" si="8"/>
         <v xml:space="preserve">                                \\</v>
       </c>
-      <c r="I138">
+      <c r="I145">
         <f t="shared" si="9"/>
         <v>1</v>
       </c>
-      <c r="J138">
+      <c r="J145">
         <f t="shared" si="10"/>
         <v>31</v>
       </c>
-      <c r="K138" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">                               </v>
-      </c>
-    </row>
-    <row r="139" spans="2:11">
-      <c r="B139" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="C139" t="s">
-        <v>149</v>
-      </c>
-      <c r="D139" t="s">
-        <v>158</v>
-      </c>
-      <c r="G139" t="str">
-        <f t="shared" ref="G139:G180" si="14">CONCATENATE(B139," ",C139,K139,"\\")</f>
-        <v>Martin White                    \\</v>
-      </c>
-      <c r="I139">
-        <f t="shared" ref="I139:I180" si="15">LEN(B139) + LEN(C139) +1</f>
-        <v>12</v>
-      </c>
-      <c r="J139">
-        <f t="shared" ref="J139:J180" si="16">IF(I139&lt;30,(32-I139),3)</f>
-        <v>20</v>
-      </c>
-      <c r="K139" t="str">
-        <f t="shared" ref="K139:K180" si="17">REPT(" ",J139)</f>
-        <v xml:space="preserve">                    </v>
-      </c>
-    </row>
-    <row r="140" spans="2:11">
-      <c r="B140" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C140" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D140" t="s">
-        <v>8</v>
-      </c>
-      <c r="G140" t="str">
-        <f>CONCATENATE(B140," ",C140,K140,"\\")</f>
-        <v>Kim Boddy                       \\</v>
-      </c>
-      <c r="I140">
-        <f>LEN(B140) + LEN(C140) +1</f>
-        <v>9</v>
-      </c>
-      <c r="J140">
-        <f>IF(I140&lt;30,(32-I140),3)</f>
-        <v>23</v>
-      </c>
-      <c r="K140" t="str">
-        <f>REPT(" ",J140)</f>
-        <v xml:space="preserve">                       </v>
-      </c>
-    </row>
-    <row r="141" spans="2:11">
-      <c r="G141" t="str">
-        <f t="shared" si="14"/>
-        <v xml:space="preserve">                                \\</v>
-      </c>
-      <c r="I141">
-        <f t="shared" si="15"/>
-        <v>1</v>
-      </c>
-      <c r="J141">
-        <f t="shared" si="16"/>
-        <v>31</v>
-      </c>
-      <c r="K141" t="str">
-        <f t="shared" si="17"/>
-        <v xml:space="preserve">                               </v>
-      </c>
-    </row>
-    <row r="142" spans="2:11">
-      <c r="G142" t="str">
-        <f t="shared" si="14"/>
-        <v xml:space="preserve">                                \\</v>
-      </c>
-      <c r="I142">
-        <f t="shared" si="15"/>
-        <v>1</v>
-      </c>
-      <c r="J142">
-        <f t="shared" si="16"/>
-        <v>31</v>
-      </c>
-      <c r="K142" t="str">
-        <f t="shared" si="17"/>
-        <v xml:space="preserve">                               </v>
-      </c>
-    </row>
-    <row r="143" spans="2:11">
-      <c r="G143" t="str">
-        <f t="shared" si="14"/>
-        <v xml:space="preserve">                                \\</v>
-      </c>
-      <c r="I143">
-        <f t="shared" si="15"/>
-        <v>1</v>
-      </c>
-      <c r="J143">
-        <f t="shared" si="16"/>
-        <v>31</v>
-      </c>
-      <c r="K143" t="str">
-        <f t="shared" si="17"/>
-        <v xml:space="preserve">                               </v>
-      </c>
-    </row>
-    <row r="144" spans="2:11">
-      <c r="G144" t="str">
-        <f t="shared" si="14"/>
-        <v xml:space="preserve">                                \\</v>
-      </c>
-      <c r="I144">
-        <f t="shared" si="15"/>
-        <v>1</v>
-      </c>
-      <c r="J144">
-        <f t="shared" si="16"/>
-        <v>31</v>
-      </c>
-      <c r="K144" t="str">
-        <f t="shared" si="17"/>
-        <v xml:space="preserve">                               </v>
-      </c>
-    </row>
-    <row r="145" spans="7:11">
-      <c r="G145" t="str">
-        <f t="shared" si="14"/>
-        <v xml:space="preserve">                                \\</v>
-      </c>
-      <c r="I145">
-        <f t="shared" si="15"/>
-        <v>1</v>
-      </c>
-      <c r="J145">
-        <f t="shared" si="16"/>
-        <v>31</v>
-      </c>
       <c r="K145" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="11"/>
         <v xml:space="preserve">                               </v>
       </c>
     </row>
     <row r="146" spans="7:11">
       <c r="G146" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="8"/>
         <v xml:space="preserve">                                \\</v>
       </c>
       <c r="I146">
-        <f t="shared" si="15"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="J146">
-        <f t="shared" si="16"/>
+        <f t="shared" si="10"/>
         <v>31</v>
       </c>
       <c r="K146" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="11"/>
         <v xml:space="preserve">                               </v>
       </c>
     </row>
     <row r="147" spans="7:11">
       <c r="G147" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="8"/>
         <v xml:space="preserve">                                \\</v>
       </c>
       <c r="I147">
-        <f t="shared" si="15"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="J147">
-        <f t="shared" si="16"/>
+        <f t="shared" si="10"/>
         <v>31</v>
       </c>
       <c r="K147" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="11"/>
         <v xml:space="preserve">                               </v>
       </c>
     </row>
     <row r="148" spans="7:11">
       <c r="G148" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="8"/>
         <v xml:space="preserve">                                \\</v>
       </c>
       <c r="I148">
-        <f t="shared" si="15"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="J148">
-        <f t="shared" si="16"/>
+        <f t="shared" si="10"/>
         <v>31</v>
       </c>
       <c r="K148" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="11"/>
         <v xml:space="preserve">                               </v>
       </c>
     </row>
     <row r="149" spans="7:11">
       <c r="G149" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="8"/>
         <v xml:space="preserve">                                \\</v>
       </c>
       <c r="I149">
-        <f t="shared" si="15"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="J149">
-        <f t="shared" si="16"/>
+        <f t="shared" si="10"/>
         <v>31</v>
       </c>
       <c r="K149" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="11"/>
         <v xml:space="preserve">                               </v>
       </c>
     </row>
     <row r="150" spans="7:11">
       <c r="G150" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="8"/>
         <v xml:space="preserve">                                \\</v>
       </c>
       <c r="I150">
-        <f t="shared" si="15"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="J150">
-        <f t="shared" si="16"/>
+        <f t="shared" si="10"/>
         <v>31</v>
       </c>
       <c r="K150" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="11"/>
         <v xml:space="preserve">                               </v>
       </c>
     </row>
     <row r="151" spans="7:11">
       <c r="G151" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="8"/>
         <v xml:space="preserve">                                \\</v>
       </c>
       <c r="I151">
-        <f t="shared" si="15"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="J151">
-        <f t="shared" si="16"/>
+        <f t="shared" si="10"/>
         <v>31</v>
       </c>
       <c r="K151" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="11"/>
         <v xml:space="preserve">                               </v>
       </c>
     </row>
     <row r="152" spans="7:11">
       <c r="G152" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="8"/>
         <v xml:space="preserve">                                \\</v>
       </c>
       <c r="I152">
-        <f t="shared" si="15"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="J152">
-        <f t="shared" si="16"/>
+        <f t="shared" si="10"/>
         <v>31</v>
       </c>
       <c r="K152" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="11"/>
         <v xml:space="preserve">                               </v>
       </c>
     </row>
     <row r="153" spans="7:11">
       <c r="G153" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="8"/>
         <v xml:space="preserve">                                \\</v>
       </c>
       <c r="I153">
-        <f t="shared" si="15"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="J153">
-        <f t="shared" si="16"/>
+        <f t="shared" si="10"/>
         <v>31</v>
       </c>
       <c r="K153" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="11"/>
         <v xml:space="preserve">                               </v>
       </c>
     </row>
     <row r="154" spans="7:11">
       <c r="G154" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="8"/>
         <v xml:space="preserve">                                \\</v>
       </c>
       <c r="I154">
-        <f t="shared" si="15"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="J154">
-        <f t="shared" si="16"/>
+        <f t="shared" si="10"/>
         <v>31</v>
       </c>
       <c r="K154" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="11"/>
         <v xml:space="preserve">                               </v>
       </c>
     </row>
     <row r="155" spans="7:11">
       <c r="G155" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="8"/>
         <v xml:space="preserve">                                \\</v>
       </c>
       <c r="I155">
-        <f t="shared" si="15"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="J155">
-        <f t="shared" si="16"/>
+        <f t="shared" si="10"/>
         <v>31</v>
       </c>
       <c r="K155" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="11"/>
         <v xml:space="preserve">                               </v>
       </c>
     </row>
     <row r="156" spans="7:11">
       <c r="G156" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="8"/>
         <v xml:space="preserve">                                \\</v>
       </c>
       <c r="I156">
-        <f t="shared" si="15"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="J156">
-        <f t="shared" si="16"/>
+        <f t="shared" si="10"/>
         <v>31</v>
       </c>
       <c r="K156" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="11"/>
         <v xml:space="preserve">                               </v>
       </c>
     </row>
     <row r="157" spans="7:11">
       <c r="G157" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="8"/>
         <v xml:space="preserve">                                \\</v>
       </c>
       <c r="I157">
-        <f t="shared" si="15"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="J157">
-        <f t="shared" si="16"/>
+        <f t="shared" si="10"/>
         <v>31</v>
       </c>
       <c r="K157" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="11"/>
         <v xml:space="preserve">                               </v>
       </c>
     </row>
     <row r="158" spans="7:11">
       <c r="G158" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="8"/>
         <v xml:space="preserve">                                \\</v>
       </c>
       <c r="I158">
-        <f t="shared" si="15"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="J158">
-        <f t="shared" si="16"/>
+        <f t="shared" si="10"/>
         <v>31</v>
       </c>
       <c r="K158" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="11"/>
         <v xml:space="preserve">                               </v>
       </c>
     </row>
     <row r="159" spans="7:11">
       <c r="G159" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="8"/>
         <v xml:space="preserve">                                \\</v>
       </c>
       <c r="I159">
-        <f t="shared" si="15"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="J159">
-        <f t="shared" si="16"/>
+        <f t="shared" si="10"/>
         <v>31</v>
       </c>
       <c r="K159" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="11"/>
         <v xml:space="preserve">                               </v>
       </c>
     </row>
     <row r="160" spans="7:11">
       <c r="G160" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="8"/>
         <v xml:space="preserve">                                \\</v>
       </c>
       <c r="I160">
-        <f t="shared" si="15"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="J160">
-        <f t="shared" si="16"/>
+        <f t="shared" si="10"/>
         <v>31</v>
       </c>
       <c r="K160" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="11"/>
         <v xml:space="preserve">                               </v>
       </c>
     </row>
     <row r="161" spans="7:11">
       <c r="G161" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="8"/>
         <v xml:space="preserve">                                \\</v>
       </c>
       <c r="I161">
-        <f t="shared" si="15"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="J161">
-        <f t="shared" si="16"/>
+        <f t="shared" si="10"/>
         <v>31</v>
       </c>
       <c r="K161" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="11"/>
         <v xml:space="preserve">                               </v>
       </c>
     </row>
     <row r="162" spans="7:11">
       <c r="G162" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="8"/>
         <v xml:space="preserve">                                \\</v>
       </c>
       <c r="I162">
-        <f t="shared" si="15"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="J162">
-        <f t="shared" si="16"/>
+        <f t="shared" si="10"/>
         <v>31</v>
       </c>
       <c r="K162" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="11"/>
         <v xml:space="preserve">                               </v>
       </c>
     </row>
     <row r="163" spans="7:11">
       <c r="G163" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="8"/>
         <v xml:space="preserve">                                \\</v>
       </c>
       <c r="I163">
-        <f t="shared" si="15"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="J163">
-        <f t="shared" si="16"/>
+        <f t="shared" si="10"/>
         <v>31</v>
       </c>
       <c r="K163" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="11"/>
         <v xml:space="preserve">                               </v>
       </c>
     </row>
     <row r="164" spans="7:11">
       <c r="G164" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="8"/>
         <v xml:space="preserve">                                \\</v>
       </c>
       <c r="I164">
-        <f t="shared" si="15"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="J164">
-        <f t="shared" si="16"/>
+        <f t="shared" si="10"/>
         <v>31</v>
       </c>
       <c r="K164" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="11"/>
         <v xml:space="preserve">                               </v>
       </c>
     </row>
     <row r="165" spans="7:11">
       <c r="G165" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="8"/>
         <v xml:space="preserve">                                \\</v>
       </c>
       <c r="I165">
-        <f t="shared" si="15"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="J165">
-        <f t="shared" si="16"/>
+        <f t="shared" si="10"/>
         <v>31</v>
       </c>
       <c r="K165" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="11"/>
         <v xml:space="preserve">                               </v>
       </c>
     </row>
     <row r="166" spans="7:11">
       <c r="G166" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="8"/>
         <v xml:space="preserve">                                \\</v>
       </c>
       <c r="I166">
-        <f t="shared" si="15"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="J166">
-        <f t="shared" si="16"/>
+        <f t="shared" si="10"/>
         <v>31</v>
       </c>
       <c r="K166" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="11"/>
         <v xml:space="preserve">                               </v>
       </c>
     </row>
     <row r="167" spans="7:11">
       <c r="G167" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="8"/>
         <v xml:space="preserve">                                \\</v>
       </c>
       <c r="I167">
-        <f t="shared" si="15"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="J167">
-        <f t="shared" si="16"/>
+        <f t="shared" si="10"/>
         <v>31</v>
       </c>
       <c r="K167" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="11"/>
         <v xml:space="preserve">                               </v>
       </c>
     </row>
     <row r="168" spans="7:11">
       <c r="G168" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="8"/>
         <v xml:space="preserve">                                \\</v>
       </c>
       <c r="I168">
-        <f t="shared" si="15"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="J168">
-        <f t="shared" si="16"/>
+        <f t="shared" si="10"/>
         <v>31</v>
       </c>
       <c r="K168" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="11"/>
         <v xml:space="preserve">                               </v>
       </c>
     </row>
     <row r="169" spans="7:11">
       <c r="G169" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="8"/>
         <v xml:space="preserve">                                \\</v>
       </c>
       <c r="I169">
-        <f t="shared" si="15"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="J169">
-        <f t="shared" si="16"/>
+        <f t="shared" si="10"/>
         <v>31</v>
       </c>
       <c r="K169" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="11"/>
         <v xml:space="preserve">                               </v>
       </c>
     </row>
     <row r="170" spans="7:11">
       <c r="G170" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="8"/>
         <v xml:space="preserve">                                \\</v>
       </c>
       <c r="I170">
-        <f t="shared" si="15"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="J170">
-        <f t="shared" si="16"/>
+        <f t="shared" si="10"/>
         <v>31</v>
       </c>
       <c r="K170" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="11"/>
         <v xml:space="preserve">                               </v>
       </c>
     </row>
     <row r="171" spans="7:11">
       <c r="G171" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="8"/>
         <v xml:space="preserve">                                \\</v>
       </c>
       <c r="I171">
-        <f t="shared" si="15"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="J171">
-        <f t="shared" si="16"/>
+        <f t="shared" si="10"/>
         <v>31</v>
       </c>
       <c r="K171" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="11"/>
         <v xml:space="preserve">                               </v>
       </c>
     </row>
     <row r="172" spans="7:11">
       <c r="G172" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="8"/>
         <v xml:space="preserve">                                \\</v>
       </c>
       <c r="I172">
-        <f t="shared" si="15"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="J172">
-        <f t="shared" si="16"/>
+        <f t="shared" si="10"/>
         <v>31</v>
       </c>
       <c r="K172" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="11"/>
         <v xml:space="preserve">                               </v>
       </c>
     </row>
     <row r="173" spans="7:11">
       <c r="G173" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="8"/>
         <v xml:space="preserve">                                \\</v>
       </c>
       <c r="I173">
-        <f t="shared" si="15"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="J173">
-        <f t="shared" si="16"/>
+        <f t="shared" si="10"/>
         <v>31</v>
       </c>
       <c r="K173" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="11"/>
         <v xml:space="preserve">                               </v>
       </c>
     </row>
     <row r="174" spans="7:11">
       <c r="G174" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="8"/>
         <v xml:space="preserve">                                \\</v>
       </c>
       <c r="I174">
-        <f t="shared" si="15"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="J174">
-        <f t="shared" si="16"/>
+        <f t="shared" si="10"/>
         <v>31</v>
       </c>
       <c r="K174" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="11"/>
         <v xml:space="preserve">                               </v>
       </c>
     </row>
     <row r="175" spans="7:11">
       <c r="G175" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="8"/>
         <v xml:space="preserve">                                \\</v>
       </c>
       <c r="I175">
-        <f t="shared" si="15"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="J175">
-        <f t="shared" si="16"/>
+        <f t="shared" si="10"/>
         <v>31</v>
       </c>
       <c r="K175" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="11"/>
         <v xml:space="preserve">                               </v>
       </c>
     </row>
     <row r="176" spans="7:11">
       <c r="G176" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="8"/>
         <v xml:space="preserve">                                \\</v>
       </c>
       <c r="I176">
-        <f t="shared" si="15"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="J176">
-        <f t="shared" si="16"/>
+        <f t="shared" si="10"/>
         <v>31</v>
       </c>
       <c r="K176" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="11"/>
         <v xml:space="preserve">                               </v>
       </c>
     </row>
     <row r="177" spans="7:11">
       <c r="G177" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="8"/>
         <v xml:space="preserve">                                \\</v>
       </c>
       <c r="I177">
-        <f t="shared" si="15"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="J177">
-        <f t="shared" si="16"/>
+        <f t="shared" si="10"/>
         <v>31</v>
       </c>
       <c r="K177" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="11"/>
         <v xml:space="preserve">                               </v>
       </c>
     </row>
     <row r="178" spans="7:11">
       <c r="G178" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="8"/>
         <v xml:space="preserve">                                \\</v>
       </c>
       <c r="I178">
-        <f t="shared" si="15"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="J178">
-        <f t="shared" si="16"/>
+        <f t="shared" si="10"/>
         <v>31</v>
       </c>
       <c r="K178" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="11"/>
         <v xml:space="preserve">                               </v>
       </c>
     </row>
     <row r="179" spans="7:11">
       <c r="G179" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="8"/>
         <v xml:space="preserve">                                \\</v>
       </c>
       <c r="I179">
-        <f t="shared" si="15"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="J179">
-        <f t="shared" si="16"/>
+        <f t="shared" si="10"/>
         <v>31</v>
       </c>
       <c r="K179" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="11"/>
         <v xml:space="preserve">                               </v>
       </c>
     </row>
-    <row r="180" spans="7:11">
-      <c r="G180" t="str">
-        <f t="shared" si="14"/>
-        <v xml:space="preserve">                                \\</v>
-      </c>
-      <c r="I180">
-        <f t="shared" si="15"/>
-        <v>1</v>
-      </c>
-      <c r="J180">
-        <f t="shared" si="16"/>
-        <v>31</v>
-      </c>
-      <c r="K180" t="str">
-        <f t="shared" si="17"/>
-        <v xml:space="preserve">                               </v>
-      </c>
-    </row>
   </sheetData>
-  <sortState ref="B10:E76">
-    <sortCondition ref="C10:C76"/>
+  <sortState ref="B10:E77">
+    <sortCondition ref="C10:C77"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
Revert "Revert "Merge branch 'master' of https://github.com/CMB-Probe/PICOReport""
This reverts commit 4fd85bb4e5d4f2c5f0519f8db77bc5da0c96ff54.
</commit_message>
<xml_diff>
--- a/ReferenceDocuments/ReportAuthors.xlsx
+++ b/ReferenceDocuments/ReportAuthors.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="325">
   <si>
     <t>Report Authors</t>
   </si>
@@ -856,9 +856,6 @@
     <t>Please update the relevant lines above if you add/remove/change names in this list.</t>
   </si>
   <si>
-    <t>12/5/2018, 1 pm.</t>
-  </si>
-  <si>
     <t>Yale University</t>
   </si>
   <si>
@@ -977,6 +974,21 @@
   </si>
   <si>
     <t>Shirokoff</t>
+  </si>
+  <si>
+    <t>CfA/Harvard</t>
+  </si>
+  <si>
+    <t>Racine</t>
+  </si>
+  <si>
+    <t>Caterina</t>
+  </si>
+  <si>
+    <t>Umilt\`{a}</t>
+  </si>
+  <si>
+    <t>12/10/2018, 3 pm.</t>
   </si>
 </sst>
 </file>
@@ -1407,10 +1419,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:K179"/>
+  <dimension ref="A1:K180"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35:XFD35"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C4" sqref="C3:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -1440,7 +1452,7 @@
       </c>
       <c r="B3"/>
       <c r="C3" s="1" t="s">
-        <v>280</v>
+        <v>324</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -1449,7 +1461,7 @@
       </c>
       <c r="B4"/>
       <c r="C4" s="1" t="s">
-        <v>280</v>
+        <v>324</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -1458,7 +1470,7 @@
       </c>
       <c r="B5"/>
       <c r="C5" s="1" t="s">
-        <v>280</v>
+        <v>324</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -1490,16 +1502,16 @@
         <v>5</v>
       </c>
       <c r="G9" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="I9" t="s">
+        <v>306</v>
+      </c>
+      <c r="J9" t="s">
         <v>307</v>
       </c>
-      <c r="J9" t="s">
+      <c r="K9" t="s">
         <v>308</v>
-      </c>
-      <c r="K9" t="s">
-        <v>309</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -1543,15 +1555,15 @@
         <v>11</v>
       </c>
       <c r="G11" t="str">
-        <f t="shared" ref="G11:G72" si="0">CONCATENATE(B11," ",C11,K11,"\\")</f>
+        <f t="shared" ref="G11:G74" si="0">CONCATENATE(B11," ",C11,K11,"\\")</f>
         <v>Peter Ashton                    \\</v>
       </c>
       <c r="I11">
-        <f t="shared" ref="I11:I72" si="1">LEN(B11) + LEN(C11) +1</f>
+        <f t="shared" ref="I11:I74" si="1">LEN(B11) + LEN(C11) +1</f>
         <v>12</v>
       </c>
       <c r="J11">
-        <f t="shared" ref="J11:J72" si="2">IF(I11&lt;30,(32-I11),3)</f>
+        <f t="shared" ref="J11:J74" si="2">IF(I11&lt;30,(32-I11),3)</f>
         <v>20</v>
       </c>
       <c r="K11" t="str">
@@ -1957,149 +1969,146 @@
     </row>
     <row r="26" spans="2:11">
       <c r="B26" t="s">
-        <v>313</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>312</v>
+        <v>46</v>
+      </c>
+      <c r="C26" t="s">
+        <v>47</v>
       </c>
       <c r="D26" t="s">
         <v>8</v>
       </c>
       <c r="E26" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="G26" t="str">
         <f t="shared" si="0"/>
-        <v>Gianfranco De Zotti             \\</v>
+        <v>Jacques Delabrouille            \\</v>
       </c>
       <c r="I26">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J26">
         <f t="shared" si="2"/>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K26" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">             </v>
+        <v xml:space="preserve">            </v>
       </c>
     </row>
     <row r="27" spans="2:11">
       <c r="B27" t="s">
-        <v>46</v>
-      </c>
-      <c r="C27" t="s">
-        <v>47</v>
+        <v>49</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>50</v>
       </c>
       <c r="D27" t="s">
         <v>8</v>
       </c>
       <c r="E27" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="G27" t="str">
         <f t="shared" si="0"/>
-        <v>Jacques Delabrouille            \\</v>
+        <v>Eleonora Di Valentino           \\</v>
       </c>
       <c r="I27">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="J27">
         <f t="shared" si="2"/>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K27" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">            </v>
+        <v xml:space="preserve">           </v>
       </c>
     </row>
     <row r="28" spans="2:11">
-      <c r="B28" t="s">
-        <v>49</v>
+      <c r="B28" s="1" t="s">
+        <v>52</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D28" t="s">
         <v>8</v>
       </c>
-      <c r="E28" t="s">
-        <v>51</v>
-      </c>
       <c r="G28" t="str">
         <f t="shared" si="0"/>
-        <v>Eleonora Di Valentino           \\</v>
+        <v>Joy Didier                      \\</v>
       </c>
       <c r="I28">
         <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="J28">
+        <f t="shared" si="2"/>
+        <v>22</v>
+      </c>
+      <c r="K28" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">                      </v>
+      </c>
+    </row>
+    <row r="29" spans="2:11">
+      <c r="B29" t="s">
+        <v>54</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="D29" t="s">
+        <v>8</v>
+      </c>
+      <c r="E29" t="s">
+        <v>55</v>
+      </c>
+      <c r="G29" t="str">
+        <f t="shared" si="0"/>
+        <v>Olivier Dor\'e                  \\</v>
+      </c>
+      <c r="I29">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="J29">
+        <f t="shared" si="2"/>
+        <v>18</v>
+      </c>
+      <c r="K29" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">                  </v>
+      </c>
+    </row>
+    <row r="30" spans="2:11">
+      <c r="B30" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="C30" t="s">
+        <v>309</v>
+      </c>
+      <c r="D30" t="s">
+        <v>8</v>
+      </c>
+      <c r="G30" t="str">
+        <f t="shared" si="0"/>
+        <v>Alexander van Engelen           \\</v>
+      </c>
+      <c r="I30">
+        <f t="shared" si="1"/>
         <v>21</v>
       </c>
-      <c r="J28">
+      <c r="J30">
         <f t="shared" si="2"/>
         <v>11</v>
       </c>
-      <c r="K28" t="str">
+      <c r="K30" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve">           </v>
-      </c>
-    </row>
-    <row r="29" spans="2:11">
-      <c r="B29" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D29" t="s">
-        <v>8</v>
-      </c>
-      <c r="G29" t="str">
-        <f t="shared" si="0"/>
-        <v>Joy Didier                      \\</v>
-      </c>
-      <c r="I29">
-        <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
-      <c r="J29">
-        <f t="shared" si="2"/>
-        <v>22</v>
-      </c>
-      <c r="K29" t="str">
-        <f t="shared" si="3"/>
-        <v xml:space="preserve">                      </v>
-      </c>
-    </row>
-    <row r="30" spans="2:11">
-      <c r="B30" t="s">
-        <v>54</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>314</v>
-      </c>
-      <c r="D30" t="s">
-        <v>8</v>
-      </c>
-      <c r="E30" t="s">
-        <v>55</v>
-      </c>
-      <c r="G30" t="str">
-        <f t="shared" si="0"/>
-        <v>Olivier Dor\'e                  \\</v>
-      </c>
-      <c r="I30">
-        <f t="shared" si="1"/>
-        <v>14</v>
-      </c>
-      <c r="J30">
-        <f t="shared" si="2"/>
-        <v>18</v>
-      </c>
-      <c r="K30" t="str">
-        <f t="shared" si="3"/>
-        <v xml:space="preserve">                  </v>
       </c>
     </row>
     <row r="31" spans="2:11">
@@ -2188,16 +2197,16 @@
     </row>
     <row r="34" spans="2:11">
       <c r="B34" t="s">
+        <v>304</v>
+      </c>
+      <c r="C34" t="s">
         <v>305</v>
       </c>
-      <c r="C34" t="s">
-        <v>306</v>
-      </c>
       <c r="D34" t="s">
         <v>8</v>
       </c>
       <c r="E34" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="G34" t="str">
         <f t="shared" si="0"/>
@@ -2593,7 +2602,7 @@
     </row>
     <row r="48" spans="2:11">
       <c r="B48" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>96</v>
@@ -2646,114 +2655,114 @@
       </c>
     </row>
     <row r="50" spans="2:11">
-      <c r="B50" s="1" t="s">
-        <v>99</v>
+      <c r="B50" t="s">
+        <v>296</v>
       </c>
       <c r="C50" t="s">
-        <v>100</v>
+        <v>315</v>
       </c>
       <c r="D50" t="s">
         <v>8</v>
       </c>
+      <c r="E50" t="s">
+        <v>284</v>
+      </c>
       <c r="G50" t="str">
         <f t="shared" si="0"/>
-        <v>Charles Lawrence                \\</v>
+        <v>Marcos L\'{o}pez-Caniego        \\</v>
       </c>
       <c r="I50">
         <f t="shared" si="1"/>
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="J50">
         <f t="shared" si="2"/>
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="K50" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">                </v>
+        <v xml:space="preserve">        </v>
       </c>
     </row>
     <row r="51" spans="2:11">
       <c r="B51" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C51" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D51" t="s">
         <v>8</v>
       </c>
       <c r="G51" t="str">
         <f t="shared" si="0"/>
-        <v>Alex Lazarian                   \\</v>
+        <v>Charles Lawrence                \\</v>
       </c>
       <c r="I51">
         <f t="shared" si="1"/>
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="J51">
         <f t="shared" si="2"/>
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="K51" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">                   </v>
+        <v xml:space="preserve">                </v>
       </c>
     </row>
     <row r="52" spans="2:11">
       <c r="B52" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C52" t="s">
+        <v>102</v>
+      </c>
+      <c r="D52" t="s">
+        <v>8</v>
+      </c>
+      <c r="G52" t="str">
+        <f t="shared" si="0"/>
+        <v>Alex Lazarian                   \\</v>
+      </c>
+      <c r="I52">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="J52">
+        <f t="shared" si="2"/>
+        <v>19</v>
+      </c>
+      <c r="K52" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">                   </v>
+      </c>
+    </row>
+    <row r="53" spans="2:11">
+      <c r="B53" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C53" t="s">
         <v>104</v>
       </c>
-      <c r="D52" t="s">
-        <v>8</v>
-      </c>
-      <c r="G52" t="str">
+      <c r="D53" t="s">
+        <v>8</v>
+      </c>
+      <c r="G53" t="str">
         <f t="shared" si="0"/>
         <v>Zack Li                         \\</v>
       </c>
-      <c r="I52">
+      <c r="I53">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="J52">
+      <c r="J53">
         <f t="shared" si="2"/>
         <v>25</v>
       </c>
-      <c r="K52" t="str">
+      <c r="K53" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve">                         </v>
-      </c>
-    </row>
-    <row r="53" spans="2:11">
-      <c r="B53" t="s">
-        <v>297</v>
-      </c>
-      <c r="C53" t="s">
-        <v>316</v>
-      </c>
-      <c r="D53" t="s">
-        <v>8</v>
-      </c>
-      <c r="E53" t="s">
-        <v>285</v>
-      </c>
-      <c r="G53" t="str">
-        <f t="shared" si="0"/>
-        <v>Marcos L\'{o}pez-Caniego        \\</v>
-      </c>
-      <c r="I53">
-        <f t="shared" si="1"/>
-        <v>24</v>
-      </c>
-      <c r="J53">
-        <f t="shared" si="2"/>
-        <v>8</v>
-      </c>
-      <c r="K53" t="str">
-        <f t="shared" si="3"/>
-        <v xml:space="preserve">        </v>
       </c>
     </row>
     <row r="54" spans="2:11">
@@ -3099,144 +3108,144 @@
       </c>
     </row>
     <row r="66" spans="2:11">
-      <c r="B66" t="s">
+      <c r="B66" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="D66" t="s">
+        <v>8</v>
+      </c>
+      <c r="G66" t="str">
+        <f t="shared" si="0"/>
+        <v>Douglas Scott                   \\</v>
+      </c>
+      <c r="I66">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="J66">
+        <f t="shared" si="2"/>
+        <v>19</v>
+      </c>
+      <c r="K66" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">                   </v>
+      </c>
+    </row>
+    <row r="67" spans="2:11">
+      <c r="B67" t="s">
         <v>133</v>
       </c>
-      <c r="C66" s="1" t="s">
+      <c r="C67" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="D66" t="s">
-        <v>8</v>
-      </c>
-      <c r="E66" t="s">
+      <c r="D67" t="s">
+        <v>8</v>
+      </c>
+      <c r="E67" t="s">
         <v>135</v>
       </c>
-      <c r="G66" t="str">
+      <c r="G67" t="str">
         <f t="shared" si="0"/>
         <v>Ian Stephens                    \\</v>
       </c>
-      <c r="I66">
+      <c r="I67">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="J66">
+      <c r="J67">
         <f t="shared" si="2"/>
         <v>20</v>
       </c>
-      <c r="K66" t="str">
+      <c r="K67" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve">                    </v>
       </c>
     </row>
-    <row r="67" spans="2:11">
-      <c r="B67" s="1" t="s">
+    <row r="68" spans="2:11">
+      <c r="B68" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="C67" t="s">
+      <c r="C68" t="s">
         <v>137</v>
       </c>
-      <c r="D67" t="s">
-        <v>8</v>
-      </c>
-      <c r="G67" t="str">
+      <c r="D68" t="s">
+        <v>8</v>
+      </c>
+      <c r="G68" t="str">
         <f t="shared" si="0"/>
         <v>Brian Sutin                     \\</v>
       </c>
-      <c r="I67">
+      <c r="I68">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="J67">
+      <c r="J68">
         <f t="shared" si="2"/>
         <v>21</v>
       </c>
-      <c r="K67" t="str">
+      <c r="K68" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve">                     </v>
       </c>
     </row>
-    <row r="68" spans="2:11">
-      <c r="B68" t="s">
+    <row r="69" spans="2:11">
+      <c r="B69" t="s">
         <v>138</v>
       </c>
-      <c r="C68" s="1" t="s">
+      <c r="C69" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="D68" t="s">
-        <v>8</v>
-      </c>
-      <c r="E68" t="s">
+      <c r="D69" t="s">
+        <v>8</v>
+      </c>
+      <c r="E69" t="s">
         <v>140</v>
       </c>
-      <c r="G68" t="str">
+      <c r="G69" t="str">
         <f t="shared" si="0"/>
         <v>Maurizio Tomasi                 \\</v>
       </c>
-      <c r="I68">
+      <c r="I69">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="J68">
+      <c r="J69">
         <f t="shared" si="2"/>
         <v>17</v>
       </c>
-      <c r="K68" t="str">
+      <c r="K69" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve">                 </v>
-      </c>
-    </row>
-    <row r="69" spans="2:11">
-      <c r="B69" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="C69" t="s">
-        <v>142</v>
-      </c>
-      <c r="D69" t="s">
-        <v>8</v>
-      </c>
-      <c r="G69" t="str">
-        <f t="shared" si="0"/>
-        <v>Amy Trangsrud                   \\</v>
-      </c>
-      <c r="I69">
-        <f t="shared" si="1"/>
-        <v>13</v>
-      </c>
-      <c r="J69">
-        <f t="shared" si="2"/>
-        <v>19</v>
-      </c>
-      <c r="K69" t="str">
-        <f t="shared" si="3"/>
-        <v xml:space="preserve">                   </v>
       </c>
     </row>
     <row r="70" spans="2:11">
       <c r="B70" s="1" t="s">
-        <v>311</v>
+        <v>141</v>
       </c>
       <c r="C70" t="s">
-        <v>310</v>
+        <v>142</v>
       </c>
       <c r="D70" t="s">
         <v>8</v>
       </c>
       <c r="G70" t="str">
         <f t="shared" si="0"/>
-        <v>Alexander van Engelen           \\</v>
+        <v>Amy Trangsrud                   \\</v>
       </c>
       <c r="I70">
         <f t="shared" si="1"/>
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="J70">
         <f t="shared" si="2"/>
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="K70" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">           </v>
+        <v xml:space="preserve">                   </v>
       </c>
     </row>
     <row r="71" spans="2:11">
@@ -3307,19 +3316,19 @@
         <v>8</v>
       </c>
       <c r="G73" t="str">
-        <f t="shared" ref="G73:G137" si="4">CONCATENATE(B73," ",C73,K73,"\\")</f>
+        <f t="shared" si="0"/>
         <v>Siyao Xu                        \\</v>
       </c>
       <c r="I73">
-        <f t="shared" ref="I73:I137" si="5">LEN(B73) + LEN(C73) +1</f>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="J73">
-        <f t="shared" ref="J73:J137" si="6">IF(I73&lt;30,(32-I73),3)</f>
+        <f t="shared" si="2"/>
         <v>24</v>
       </c>
       <c r="K73" t="str">
-        <f t="shared" ref="K73:K137" si="7">REPT(" ",J73)</f>
+        <f t="shared" ref="K73:K138" si="4">REPT(" ",J73)</f>
         <v xml:space="preserve">                        </v>
       </c>
     </row>
@@ -3334,19 +3343,19 @@
         <v>8</v>
       </c>
       <c r="G74" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="0"/>
         <v>Karl Young                      \\</v>
       </c>
       <c r="I74">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="J74">
-        <f t="shared" si="6"/>
+        <f t="shared" si="2"/>
         <v>22</v>
       </c>
       <c r="K74" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">                      </v>
       </c>
     </row>
@@ -3361,1107 +3370,1087 @@
         <v>8</v>
       </c>
       <c r="G75" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="G75:G76" si="5">CONCATENATE(B75," ",C75,K75,"\\")</f>
         <v>Andrea Zonca                    \\</v>
       </c>
       <c r="I75">
+        <f t="shared" ref="I75:I76" si="6">LEN(B75) + LEN(C75) +1</f>
+        <v>12</v>
+      </c>
+      <c r="J75">
+        <f t="shared" ref="J75:J76" si="7">IF(I75&lt;30,(32-I75),3)</f>
+        <v>20</v>
+      </c>
+      <c r="K75" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">                    </v>
+      </c>
+    </row>
+    <row r="76" spans="2:11">
+      <c r="B76" t="s">
+        <v>312</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="D76" t="s">
+        <v>8</v>
+      </c>
+      <c r="E76" t="s">
+        <v>45</v>
+      </c>
+      <c r="G76" t="str">
         <f t="shared" si="5"/>
-        <v>12</v>
-      </c>
-      <c r="J75">
-        <f t="shared" si="6"/>
-        <v>20</v>
-      </c>
-      <c r="K75" t="str">
-        <f t="shared" si="7"/>
-        <v xml:space="preserve">                    </v>
-      </c>
-    </row>
-    <row r="76" spans="2:11">
-      <c r="B76" s="3"/>
-      <c r="C76"/>
-      <c r="G76" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">                                \\</v>
+        <v>Gianfranco De Zotti             \\</v>
       </c>
       <c r="I76">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="J76">
-        <f t="shared" si="6"/>
-        <v>31</v>
-      </c>
-      <c r="K76" t="str">
-        <f t="shared" si="7"/>
-        <v xml:space="preserve">                               </v>
-      </c>
-    </row>
-    <row r="77" spans="2:11">
-      <c r="B77" s="3"/>
-      <c r="C77"/>
-      <c r="G77" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">                                \\</v>
-      </c>
-      <c r="I77">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="J77">
-        <f t="shared" si="6"/>
-        <v>31</v>
-      </c>
-      <c r="K77" t="str">
-        <f t="shared" si="7"/>
-        <v xml:space="preserve">                               </v>
-      </c>
-    </row>
-    <row r="78" spans="2:11">
-      <c r="B78" t="s">
-        <v>156</v>
-      </c>
-      <c r="C78" t="s">
-        <v>157</v>
-      </c>
-      <c r="D78" t="s">
-        <v>158</v>
-      </c>
-      <c r="E78" t="s">
-        <v>159</v>
-      </c>
-      <c r="G78" t="str">
-        <f t="shared" si="4"/>
-        <v>Zeeshan Ahmed                   \\</v>
-      </c>
-      <c r="I78">
-        <f t="shared" si="5"/>
-        <v>13</v>
-      </c>
-      <c r="J78">
         <f t="shared" si="6"/>
         <v>19</v>
       </c>
+      <c r="J76">
+        <f t="shared" si="7"/>
+        <v>13</v>
+      </c>
+      <c r="K76" t="str">
+        <f>REPT(" ",J76)</f>
+        <v xml:space="preserve">             </v>
+      </c>
+    </row>
+    <row r="78" spans="2:11">
+      <c r="B78" s="3"/>
+      <c r="C78"/>
+      <c r="G78" t="str">
+        <f t="shared" ref="G73:G138" si="8">CONCATENATE(B78," ",C78,K78,"\\")</f>
+        <v xml:space="preserve">                                \\</v>
+      </c>
+      <c r="I78">
+        <f t="shared" ref="I73:I138" si="9">LEN(B78) + LEN(C78) +1</f>
+        <v>1</v>
+      </c>
+      <c r="J78">
+        <f t="shared" ref="J73:J138" si="10">IF(I78&lt;30,(32-I78),3)</f>
+        <v>31</v>
+      </c>
       <c r="K78" t="str">
-        <f t="shared" si="7"/>
-        <v xml:space="preserve">                   </v>
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">                               </v>
       </c>
     </row>
     <row r="79" spans="2:11">
       <c r="B79" t="s">
-        <v>160</v>
-      </c>
-      <c r="C79" s="1" t="s">
-        <v>161</v>
+        <v>156</v>
+      </c>
+      <c r="C79" t="s">
+        <v>157</v>
       </c>
       <c r="D79" t="s">
         <v>158</v>
       </c>
       <c r="E79" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="G79" t="str">
-        <f t="shared" si="4"/>
-        <v>Jason Austermann                \\</v>
+        <f t="shared" si="8"/>
+        <v>Zeeshan Ahmed                   \\</v>
       </c>
       <c r="I79">
-        <f t="shared" si="5"/>
-        <v>16</v>
+        <f t="shared" si="9"/>
+        <v>13</v>
       </c>
       <c r="J79">
-        <f t="shared" si="6"/>
-        <v>16</v>
+        <f t="shared" si="10"/>
+        <v>19</v>
       </c>
       <c r="K79" t="str">
-        <f t="shared" si="7"/>
-        <v xml:space="preserve">                </v>
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">                   </v>
       </c>
     </row>
     <row r="80" spans="2:11">
       <c r="B80" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="D80" t="s">
         <v>158</v>
       </c>
       <c r="E80" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="G80" t="str">
-        <f t="shared" si="4"/>
-        <v>Darcy Barron                    \\</v>
+        <f t="shared" ref="G80:G132" si="11">CONCATENATE(B80," ",C80,K80,"\\")</f>
+        <v>Jason Austermann                \\</v>
       </c>
       <c r="I80">
-        <f t="shared" si="5"/>
-        <v>12</v>
+        <f t="shared" ref="I80:I132" si="12">LEN(B80) + LEN(C80) +1</f>
+        <v>16</v>
       </c>
       <c r="J80">
-        <f t="shared" si="6"/>
-        <v>20</v>
+        <f t="shared" ref="J80:J132" si="13">IF(I80&lt;30,(32-I80),3)</f>
+        <v>16</v>
       </c>
       <c r="K80" t="str">
-        <f t="shared" si="7"/>
-        <v xml:space="preserve">                    </v>
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">                </v>
       </c>
     </row>
     <row r="81" spans="2:11">
       <c r="B81" t="s">
-        <v>166</v>
-      </c>
-      <c r="C81" t="s">
-        <v>167</v>
+        <v>163</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>164</v>
       </c>
       <c r="D81" t="s">
         <v>158</v>
       </c>
+      <c r="E81" t="s">
+        <v>165</v>
+      </c>
       <c r="G81" t="str">
-        <f t="shared" si="4"/>
-        <v>Karim Benabed                   \\</v>
+        <f t="shared" si="11"/>
+        <v>Darcy Barron                    \\</v>
       </c>
       <c r="I81">
-        <f t="shared" si="5"/>
-        <v>13</v>
+        <f t="shared" si="12"/>
+        <v>12</v>
       </c>
       <c r="J81">
-        <f t="shared" si="6"/>
-        <v>19</v>
+        <f t="shared" si="13"/>
+        <v>20</v>
       </c>
       <c r="K81" t="str">
-        <f t="shared" si="7"/>
-        <v xml:space="preserve">                   </v>
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">                    </v>
       </c>
     </row>
     <row r="82" spans="2:11">
       <c r="B82" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C82" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D82" t="s">
         <v>158</v>
       </c>
-      <c r="E82" t="s">
-        <v>170</v>
-      </c>
       <c r="G82" t="str">
-        <f t="shared" si="4"/>
-        <v>Federico Bianchini              \\</v>
+        <f t="shared" si="11"/>
+        <v>Karim Benabed                   \\</v>
       </c>
       <c r="I82">
-        <f t="shared" si="5"/>
-        <v>18</v>
+        <f t="shared" si="12"/>
+        <v>13</v>
       </c>
       <c r="J82">
-        <f t="shared" si="6"/>
-        <v>14</v>
+        <f t="shared" si="13"/>
+        <v>19</v>
       </c>
       <c r="K82" t="str">
-        <f t="shared" si="7"/>
-        <v xml:space="preserve">              </v>
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">                   </v>
       </c>
     </row>
     <row r="83" spans="2:11">
-      <c r="B83" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C83" s="1" t="s">
-        <v>296</v>
+      <c r="B83" t="s">
+        <v>168</v>
+      </c>
+      <c r="C83" t="s">
+        <v>169</v>
       </c>
       <c r="D83" t="s">
         <v>158</v>
       </c>
       <c r="E83" t="s">
-        <v>284</v>
+        <v>170</v>
       </c>
       <c r="G83" t="str">
-        <f t="shared" si="4"/>
-        <v>Colin Bischoff                  \\</v>
+        <f t="shared" si="11"/>
+        <v>Federico Bianchini              \\</v>
       </c>
       <c r="I83">
-        <f t="shared" si="5"/>
+        <f t="shared" si="12"/>
+        <v>18</v>
+      </c>
+      <c r="J83">
+        <f t="shared" si="13"/>
         <v>14</v>
       </c>
-      <c r="J83">
-        <f t="shared" si="6"/>
-        <v>18</v>
-      </c>
       <c r="K83" t="str">
-        <f t="shared" si="7"/>
-        <v xml:space="preserve">                  </v>
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">              </v>
       </c>
     </row>
     <row r="84" spans="2:11">
-      <c r="B84" t="s">
-        <v>174</v>
-      </c>
-      <c r="C84" t="s">
-        <v>175</v>
+      <c r="B84" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>295</v>
       </c>
       <c r="D84" t="s">
         <v>158</v>
       </c>
       <c r="E84" t="s">
-        <v>176</v>
+        <v>283</v>
       </c>
       <c r="G84" t="str">
-        <f t="shared" si="4"/>
-        <v>J. Richard Bond                 \\</v>
+        <f t="shared" si="11"/>
+        <v>Colin Bischoff                  \\</v>
       </c>
       <c r="I84">
-        <f t="shared" si="5"/>
-        <v>15</v>
+        <f t="shared" si="12"/>
+        <v>14</v>
       </c>
       <c r="J84">
-        <f t="shared" si="6"/>
-        <v>17</v>
+        <f t="shared" si="13"/>
+        <v>18</v>
       </c>
       <c r="K84" t="str">
-        <f t="shared" si="7"/>
-        <v xml:space="preserve">                 </v>
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">                  </v>
       </c>
     </row>
     <row r="85" spans="2:11">
-      <c r="B85" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="C85" s="1" t="s">
-        <v>294</v>
+      <c r="B85" t="s">
+        <v>174</v>
+      </c>
+      <c r="C85" t="s">
+        <v>175</v>
       </c>
       <c r="D85" t="s">
         <v>158</v>
       </c>
       <c r="E85" t="s">
-        <v>282</v>
+        <v>176</v>
       </c>
       <c r="G85" t="str">
-        <f t="shared" si="4"/>
-        <v>Robert Caldwell                 \\</v>
+        <f t="shared" si="11"/>
+        <v>J. Richard Bond                 \\</v>
       </c>
       <c r="I85">
-        <f t="shared" si="5"/>
+        <f t="shared" si="12"/>
         <v>15</v>
       </c>
       <c r="J85">
-        <f t="shared" si="6"/>
+        <f t="shared" si="13"/>
         <v>17</v>
       </c>
       <c r="K85" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">                 </v>
       </c>
     </row>
     <row r="86" spans="2:11">
-      <c r="B86" t="s">
-        <v>177</v>
+      <c r="B86" s="1" t="s">
+        <v>314</v>
       </c>
       <c r="C86" t="s">
-        <v>178</v>
+        <v>195</v>
       </c>
       <c r="D86" t="s">
         <v>158</v>
       </c>
       <c r="E86" t="s">
-        <v>135</v>
+        <v>84</v>
       </c>
       <c r="G86" t="str">
-        <f t="shared" si="4"/>
-        <v>Xingang Chen                    \\</v>
+        <f t="shared" si="11"/>
+        <v>Fran\c{c}ois Bouchet            \\</v>
       </c>
       <c r="I86">
-        <f t="shared" si="5"/>
+        <f t="shared" si="12"/>
+        <v>20</v>
+      </c>
+      <c r="J86">
+        <f t="shared" si="13"/>
         <v>12</v>
       </c>
-      <c r="J86">
-        <f t="shared" si="6"/>
-        <v>20</v>
-      </c>
       <c r="K86" t="str">
-        <f t="shared" si="7"/>
-        <v xml:space="preserve">                    </v>
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">            </v>
       </c>
     </row>
     <row r="87" spans="2:11">
-      <c r="B87" t="s">
-        <v>179</v>
-      </c>
-      <c r="C87" t="s">
-        <v>180</v>
+      <c r="B87" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>293</v>
       </c>
       <c r="D87" t="s">
         <v>158</v>
       </c>
       <c r="E87" t="s">
-        <v>181</v>
+        <v>281</v>
       </c>
       <c r="G87" t="str">
-        <f t="shared" si="4"/>
-        <v>Jens Chluba                     \\</v>
+        <f t="shared" si="11"/>
+        <v>Robert Caldwell                 \\</v>
       </c>
       <c r="I87">
-        <f t="shared" si="5"/>
-        <v>11</v>
+        <f t="shared" si="12"/>
+        <v>15</v>
       </c>
       <c r="J87">
-        <f t="shared" si="6"/>
-        <v>21</v>
+        <f t="shared" si="13"/>
+        <v>17</v>
       </c>
       <c r="K87" t="str">
-        <f t="shared" si="7"/>
-        <v xml:space="preserve">                     </v>
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">                 </v>
       </c>
     </row>
     <row r="88" spans="2:11">
       <c r="B88" t="s">
-        <v>182</v>
-      </c>
-      <c r="C88" s="1" t="s">
-        <v>183</v>
+        <v>177</v>
+      </c>
+      <c r="C88" t="s">
+        <v>178</v>
       </c>
       <c r="D88" t="s">
         <v>158</v>
       </c>
       <c r="E88" t="s">
-        <v>184</v>
+        <v>135</v>
       </c>
       <c r="G88" t="str">
-        <f t="shared" si="4"/>
-        <v>Francis-Yan Cyr-Racine          \\</v>
+        <f t="shared" si="11"/>
+        <v>Xingang Chen                    \\</v>
       </c>
       <c r="I88">
-        <f t="shared" si="5"/>
-        <v>22</v>
+        <f t="shared" si="12"/>
+        <v>12</v>
       </c>
       <c r="J88">
-        <f t="shared" si="6"/>
-        <v>10</v>
+        <f t="shared" si="13"/>
+        <v>20</v>
       </c>
       <c r="K88" t="str">
-        <f t="shared" si="7"/>
-        <v xml:space="preserve">          </v>
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">                    </v>
       </c>
     </row>
     <row r="89" spans="2:11">
       <c r="B89" t="s">
-        <v>185</v>
-      </c>
-      <c r="C89" s="1" t="s">
-        <v>186</v>
+        <v>179</v>
+      </c>
+      <c r="C89" t="s">
+        <v>180</v>
       </c>
       <c r="D89" t="s">
         <v>158</v>
       </c>
       <c r="E89" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="G89" t="str">
-        <f t="shared" si="4"/>
-        <v>Tijmen de Haan                  \\</v>
+        <f t="shared" si="11"/>
+        <v>Jens Chluba                     \\</v>
       </c>
       <c r="I89">
-        <f t="shared" si="5"/>
-        <v>14</v>
+        <f t="shared" si="12"/>
+        <v>11</v>
       </c>
       <c r="J89">
-        <f t="shared" si="6"/>
-        <v>18</v>
+        <f t="shared" si="13"/>
+        <v>21</v>
       </c>
       <c r="K89" t="str">
-        <f t="shared" si="7"/>
-        <v xml:space="preserve">                  </v>
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">                     </v>
       </c>
     </row>
     <row r="90" spans="2:11">
       <c r="B90" t="s">
-        <v>188</v>
-      </c>
-      <c r="C90" t="s">
-        <v>320</v>
+        <v>182</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>183</v>
       </c>
       <c r="D90" t="s">
         <v>158</v>
       </c>
       <c r="E90" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="G90" t="str">
-        <f>CONCATENATE(C90," ",B90,K90,"\\")</f>
-        <v>Shirokoff Erik                  \\</v>
+        <f t="shared" si="11"/>
+        <v>Francis-Yan Cyr-Racine          \\</v>
       </c>
       <c r="I90">
-        <f>LEN(C90) + LEN(B90) +1</f>
-        <v>14</v>
+        <f t="shared" si="12"/>
+        <v>22</v>
       </c>
       <c r="J90">
-        <f t="shared" si="6"/>
-        <v>18</v>
+        <f t="shared" si="13"/>
+        <v>10</v>
       </c>
       <c r="K90" t="str">
-        <f t="shared" si="7"/>
-        <v xml:space="preserve">                  </v>
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">          </v>
       </c>
     </row>
     <row r="91" spans="2:11">
       <c r="B91" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="D91" t="s">
         <v>158</v>
       </c>
       <c r="E91" t="s">
-        <v>93</v>
+        <v>187</v>
       </c>
       <c r="G91" t="str">
-        <f t="shared" si="4"/>
-        <v>Aurelien Fraisse                \\</v>
+        <f t="shared" si="11"/>
+        <v>Tijmen de Haan                  \\</v>
       </c>
       <c r="I91">
-        <f t="shared" si="5"/>
-        <v>16</v>
+        <f t="shared" si="12"/>
+        <v>14</v>
       </c>
       <c r="J91">
-        <f t="shared" si="6"/>
-        <v>16</v>
+        <f t="shared" si="13"/>
+        <v>18</v>
       </c>
       <c r="K91" t="str">
-        <f t="shared" si="7"/>
-        <v xml:space="preserve">                </v>
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">                  </v>
       </c>
     </row>
     <row r="92" spans="2:11">
-      <c r="B92" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="C92" t="s">
-        <v>192</v>
+      <c r="B92" t="s">
+        <v>190</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>191</v>
       </c>
       <c r="D92" t="s">
         <v>158</v>
       </c>
       <c r="E92" t="s">
-        <v>194</v>
+        <v>93</v>
       </c>
       <c r="G92" t="str">
-        <f>CONCATENATE(C92," ",B92,K92,"\\")</f>
-        <v>Piacentini Francesco            \\</v>
+        <f t="shared" si="11"/>
+        <v>Aurelien Fraisse                \\</v>
       </c>
       <c r="I92">
-        <f>LEN(C92) + LEN(B92) +1</f>
-        <v>20</v>
+        <f t="shared" si="12"/>
+        <v>16</v>
       </c>
       <c r="J92">
-        <f t="shared" si="6"/>
-        <v>12</v>
+        <f t="shared" si="13"/>
+        <v>16</v>
       </c>
       <c r="K92" t="str">
-        <f t="shared" si="7"/>
-        <v xml:space="preserve">            </v>
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">                </v>
       </c>
     </row>
     <row r="93" spans="2:11">
-      <c r="B93" s="1" t="s">
-        <v>315</v>
-      </c>
-      <c r="C93" t="s">
-        <v>195</v>
+      <c r="B93" t="s">
+        <v>196</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>197</v>
       </c>
       <c r="D93" t="s">
         <v>158</v>
       </c>
       <c r="E93" t="s">
-        <v>84</v>
+        <v>198</v>
       </c>
       <c r="G93" t="str">
-        <f>CONCATENATE(C93," ",B93,K93,"\\")</f>
-        <v>Bouchet Fran\c{c}ois            \\</v>
+        <f t="shared" si="11"/>
+        <v>Silvia Galli                    \\</v>
       </c>
       <c r="I93">
-        <f>LEN(C93) + LEN(B93) +1</f>
+        <f t="shared" si="12"/>
+        <v>12</v>
+      </c>
+      <c r="J93">
+        <f t="shared" si="13"/>
         <v>20</v>
       </c>
-      <c r="J93">
-        <f t="shared" si="6"/>
-        <v>12</v>
-      </c>
       <c r="K93" t="str">
-        <f t="shared" si="7"/>
-        <v xml:space="preserve">            </v>
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">                    </v>
       </c>
     </row>
     <row r="94" spans="2:11">
       <c r="B94" t="s">
-        <v>196</v>
-      </c>
-      <c r="C94" s="1" t="s">
-        <v>197</v>
+        <v>199</v>
+      </c>
+      <c r="C94" t="s">
+        <v>200</v>
       </c>
       <c r="D94" t="s">
         <v>158</v>
       </c>
       <c r="E94" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="G94" t="str">
-        <f t="shared" si="4"/>
-        <v>Silvia Galli                    \\</v>
+        <f t="shared" si="11"/>
+        <v>Ken Ganga                       \\</v>
       </c>
       <c r="I94">
-        <f t="shared" si="5"/>
-        <v>12</v>
+        <f t="shared" si="12"/>
+        <v>9</v>
       </c>
       <c r="J94">
-        <f t="shared" si="6"/>
-        <v>20</v>
+        <f t="shared" si="13"/>
+        <v>23</v>
       </c>
       <c r="K94" t="str">
-        <f t="shared" si="7"/>
-        <v xml:space="preserve">                    </v>
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">                       </v>
       </c>
     </row>
     <row r="95" spans="2:11">
       <c r="B95" t="s">
-        <v>199</v>
-      </c>
-      <c r="C95" t="s">
-        <v>200</v>
+        <v>202</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>203</v>
       </c>
       <c r="D95" t="s">
         <v>158</v>
       </c>
       <c r="E95" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="G95" t="str">
-        <f t="shared" si="4"/>
-        <v>Ken Ganga                       \\</v>
+        <f t="shared" si="11"/>
+        <v>Tuhin Ghosh                     \\</v>
       </c>
       <c r="I95">
-        <f t="shared" si="5"/>
-        <v>9</v>
+        <f t="shared" si="12"/>
+        <v>11</v>
       </c>
       <c r="J95">
-        <f t="shared" si="6"/>
-        <v>23</v>
+        <f t="shared" si="13"/>
+        <v>21</v>
       </c>
       <c r="K95" t="str">
-        <f t="shared" si="7"/>
-        <v xml:space="preserve">                       </v>
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">                     </v>
       </c>
     </row>
     <row r="96" spans="2:11">
       <c r="B96" t="s">
-        <v>202</v>
-      </c>
-      <c r="C96" s="1" t="s">
-        <v>203</v>
+        <v>205</v>
+      </c>
+      <c r="C96" t="s">
+        <v>206</v>
       </c>
       <c r="D96" t="s">
         <v>158</v>
       </c>
       <c r="E96" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="G96" t="str">
-        <f t="shared" si="4"/>
-        <v>Tuhin Ghosh                     \\</v>
+        <f t="shared" si="11"/>
+        <v>Jon E. Gudmundsson              \\</v>
       </c>
       <c r="I96">
-        <f t="shared" si="5"/>
-        <v>11</v>
+        <f t="shared" si="12"/>
+        <v>18</v>
       </c>
       <c r="J96">
-        <f t="shared" si="6"/>
-        <v>21</v>
+        <f t="shared" si="13"/>
+        <v>14</v>
       </c>
       <c r="K96" t="str">
-        <f t="shared" si="7"/>
-        <v xml:space="preserve">                     </v>
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">              </v>
       </c>
     </row>
     <row r="97" spans="2:11">
       <c r="B97" t="s">
-        <v>205</v>
-      </c>
-      <c r="C97" t="s">
-        <v>206</v>
+        <v>208</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>209</v>
       </c>
       <c r="D97" t="s">
         <v>158</v>
       </c>
       <c r="E97" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="G97" t="str">
-        <f t="shared" si="4"/>
-        <v>Jon E. Gudmundsson              \\</v>
+        <f t="shared" si="11"/>
+        <v>Marc Kamionkowski               \\</v>
       </c>
       <c r="I97">
-        <f t="shared" si="5"/>
-        <v>18</v>
+        <f t="shared" si="12"/>
+        <v>17</v>
       </c>
       <c r="J97">
-        <f t="shared" si="6"/>
-        <v>14</v>
+        <f t="shared" si="13"/>
+        <v>15</v>
       </c>
       <c r="K97" t="str">
-        <f t="shared" si="7"/>
-        <v xml:space="preserve">              </v>
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">               </v>
       </c>
     </row>
     <row r="98" spans="2:11">
       <c r="B98" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="D98" t="s">
         <v>158</v>
       </c>
       <c r="E98" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="G98" t="str">
-        <f t="shared" si="4"/>
-        <v>Marc Kamionkowski               \\</v>
+        <f t="shared" si="11"/>
+        <v>Reijo Keskitalo                 \\</v>
       </c>
       <c r="I98">
-        <f t="shared" si="5"/>
+        <f t="shared" si="12"/>
+        <v>15</v>
+      </c>
+      <c r="J98">
+        <f t="shared" si="13"/>
         <v>17</v>
       </c>
-      <c r="J98">
-        <f t="shared" si="6"/>
-        <v>15</v>
-      </c>
       <c r="K98" t="str">
-        <f t="shared" si="7"/>
-        <v xml:space="preserve">               </v>
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">                 </v>
       </c>
     </row>
     <row r="99" spans="2:11">
       <c r="B99" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="D99" t="s">
         <v>158</v>
       </c>
       <c r="E99" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="G99" t="str">
-        <f t="shared" si="4"/>
-        <v>Reijo Keskitalo                 \\</v>
+        <f t="shared" si="11"/>
+        <v>Rishi Khatri                    \\</v>
       </c>
       <c r="I99">
-        <f t="shared" si="5"/>
-        <v>15</v>
+        <f t="shared" si="12"/>
+        <v>12</v>
       </c>
       <c r="J99">
-        <f t="shared" si="6"/>
-        <v>17</v>
+        <f t="shared" si="13"/>
+        <v>20</v>
       </c>
       <c r="K99" t="str">
-        <f t="shared" si="7"/>
-        <v xml:space="preserve">                 </v>
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">                    </v>
       </c>
     </row>
     <row r="100" spans="2:11">
       <c r="B100" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="D100" t="s">
         <v>158</v>
       </c>
       <c r="E100" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="G100" t="str">
-        <f t="shared" si="4"/>
-        <v>Rishi Khatri                    \\</v>
+        <f t="shared" si="11"/>
+        <v>Ely Kovetz                      \\</v>
       </c>
       <c r="I100">
-        <f t="shared" si="5"/>
-        <v>12</v>
+        <f t="shared" si="12"/>
+        <v>10</v>
       </c>
       <c r="J100">
-        <f t="shared" si="6"/>
-        <v>20</v>
+        <f t="shared" si="13"/>
+        <v>22</v>
       </c>
       <c r="K100" t="str">
-        <f t="shared" si="7"/>
-        <v xml:space="preserve">                    </v>
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">                      </v>
       </c>
     </row>
     <row r="101" spans="2:11">
       <c r="B101" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="D101" t="s">
         <v>158</v>
       </c>
       <c r="E101" t="s">
-        <v>210</v>
+        <v>221</v>
       </c>
       <c r="G101" t="str">
-        <f t="shared" si="4"/>
-        <v>Ely Kovetz                      \\</v>
+        <f t="shared" si="11"/>
+        <v>Daniel Lenz                     \\</v>
       </c>
       <c r="I101">
-        <f t="shared" si="5"/>
-        <v>10</v>
+        <f t="shared" si="12"/>
+        <v>11</v>
       </c>
       <c r="J101">
-        <f t="shared" si="6"/>
-        <v>22</v>
+        <f t="shared" si="13"/>
+        <v>21</v>
       </c>
       <c r="K101" t="str">
-        <f t="shared" si="7"/>
-        <v xml:space="preserve">                      </v>
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">                     </v>
       </c>
     </row>
     <row r="102" spans="2:11">
       <c r="B102" t="s">
-        <v>219</v>
-      </c>
-      <c r="C102" s="1" t="s">
-        <v>220</v>
+        <v>222</v>
+      </c>
+      <c r="C102" t="s">
+        <v>223</v>
       </c>
       <c r="D102" t="s">
         <v>158</v>
       </c>
       <c r="E102" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="G102" t="str">
-        <f t="shared" si="4"/>
-        <v>Daniel Lenz                     \\</v>
+        <f t="shared" si="11"/>
+        <v>Marilena Loverde                \\</v>
       </c>
       <c r="I102">
-        <f t="shared" si="5"/>
-        <v>11</v>
+        <f t="shared" si="12"/>
+        <v>16</v>
       </c>
       <c r="J102">
-        <f t="shared" si="6"/>
-        <v>21</v>
+        <f t="shared" si="13"/>
+        <v>16</v>
       </c>
       <c r="K102" t="str">
-        <f t="shared" si="7"/>
-        <v xml:space="preserve">                     </v>
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">                </v>
       </c>
     </row>
     <row r="103" spans="2:11">
       <c r="B103" t="s">
-        <v>222</v>
-      </c>
-      <c r="C103" t="s">
-        <v>223</v>
+        <v>225</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>226</v>
       </c>
       <c r="D103" t="s">
         <v>158</v>
       </c>
       <c r="E103" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="G103" t="str">
-        <f t="shared" si="4"/>
-        <v>Marilena Loverde                \\</v>
+        <f t="shared" si="11"/>
+        <v>Carlos Martins                  \\</v>
       </c>
       <c r="I103">
-        <f t="shared" si="5"/>
-        <v>16</v>
+        <f t="shared" si="12"/>
+        <v>14</v>
       </c>
       <c r="J103">
-        <f t="shared" si="6"/>
-        <v>16</v>
+        <f t="shared" si="13"/>
+        <v>18</v>
       </c>
       <c r="K103" t="str">
-        <f t="shared" si="7"/>
-        <v xml:space="preserve">                </v>
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">                  </v>
       </c>
     </row>
     <row r="104" spans="2:11">
       <c r="B104" t="s">
-        <v>225</v>
-      </c>
-      <c r="C104" s="1" t="s">
-        <v>226</v>
+        <v>196</v>
+      </c>
+      <c r="C104" t="s">
+        <v>228</v>
       </c>
       <c r="D104" t="s">
         <v>158</v>
       </c>
       <c r="E104" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="G104" t="str">
-        <f t="shared" si="4"/>
-        <v>Carlos Martins                  \\</v>
+        <f t="shared" si="11"/>
+        <v>Silvia Masi                     \\</v>
       </c>
       <c r="I104">
-        <f t="shared" si="5"/>
-        <v>14</v>
+        <f t="shared" si="12"/>
+        <v>11</v>
       </c>
       <c r="J104">
-        <f t="shared" si="6"/>
-        <v>18</v>
+        <f t="shared" si="13"/>
+        <v>21</v>
       </c>
       <c r="K104" t="str">
-        <f t="shared" si="7"/>
-        <v xml:space="preserve">                  </v>
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">                     </v>
       </c>
     </row>
     <row r="105" spans="2:11">
-      <c r="B105" t="s">
-        <v>196</v>
-      </c>
-      <c r="C105" t="s">
-        <v>228</v>
+      <c r="B105" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>298</v>
       </c>
       <c r="D105" t="s">
         <v>158</v>
       </c>
       <c r="E105" t="s">
-        <v>229</v>
+        <v>285</v>
       </c>
       <c r="G105" t="str">
-        <f t="shared" si="4"/>
-        <v>Silvia Masi                     \\</v>
+        <f t="shared" si="11"/>
+        <v>Joel Meyers                     \\</v>
       </c>
       <c r="I105">
-        <f t="shared" si="5"/>
+        <f t="shared" si="12"/>
         <v>11</v>
       </c>
       <c r="J105">
-        <f t="shared" si="6"/>
+        <f t="shared" si="13"/>
         <v>21</v>
       </c>
       <c r="K105" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">                     </v>
       </c>
     </row>
     <row r="106" spans="2:11">
-      <c r="B106" s="1" t="s">
-        <v>298</v>
+      <c r="B106" t="s">
+        <v>230</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>299</v>
+        <v>231</v>
       </c>
       <c r="D106" t="s">
         <v>158</v>
       </c>
       <c r="E106" t="s">
-        <v>286</v>
+        <v>232</v>
       </c>
       <c r="G106" t="str">
-        <f t="shared" si="4"/>
-        <v>Joel Meyers                     \\</v>
+        <f t="shared" si="11"/>
+        <v>Lorenzo Moncelsi                \\</v>
       </c>
       <c r="I106">
-        <f t="shared" si="5"/>
-        <v>11</v>
+        <f t="shared" si="12"/>
+        <v>16</v>
       </c>
       <c r="J106">
-        <f t="shared" si="6"/>
-        <v>21</v>
+        <f t="shared" si="13"/>
+        <v>16</v>
       </c>
       <c r="K106" t="str">
-        <f t="shared" si="7"/>
-        <v xml:space="preserve">                     </v>
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">                </v>
       </c>
     </row>
     <row r="107" spans="2:11">
       <c r="B107" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="D107" t="s">
         <v>158</v>
       </c>
       <c r="E107" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="G107" t="str">
-        <f t="shared" si="4"/>
-        <v>Lorenzo Moncelsi                \\</v>
+        <f t="shared" si="11"/>
+        <v>Pavel Motloch                   \\</v>
       </c>
       <c r="I107">
-        <f t="shared" si="5"/>
-        <v>16</v>
+        <f t="shared" si="12"/>
+        <v>13</v>
       </c>
       <c r="J107">
-        <f t="shared" si="6"/>
-        <v>16</v>
+        <f t="shared" si="13"/>
+        <v>19</v>
       </c>
       <c r="K107" t="str">
-        <f t="shared" si="7"/>
-        <v xml:space="preserve">                </v>
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">                   </v>
       </c>
     </row>
     <row r="108" spans="2:11">
       <c r="B108" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="D108" t="s">
         <v>158</v>
       </c>
       <c r="E108" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="G108" t="str">
-        <f t="shared" si="4"/>
-        <v>Pavel Motloch                   \\</v>
+        <f t="shared" si="11"/>
+        <v>Tony Mroczkowski                \\</v>
       </c>
       <c r="I108">
-        <f t="shared" si="5"/>
-        <v>13</v>
+        <f t="shared" si="12"/>
+        <v>16</v>
       </c>
       <c r="J108">
-        <f t="shared" si="6"/>
-        <v>19</v>
+        <f t="shared" si="13"/>
+        <v>16</v>
       </c>
       <c r="K108" t="str">
-        <f t="shared" si="7"/>
-        <v xml:space="preserve">                   </v>
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">                </v>
       </c>
     </row>
     <row r="109" spans="2:11">
       <c r="B109" t="s">
-        <v>236</v>
-      </c>
-      <c r="C109" s="1" t="s">
-        <v>237</v>
+        <v>233</v>
+      </c>
+      <c r="C109" t="s">
+        <v>239</v>
       </c>
       <c r="D109" t="s">
         <v>158</v>
       </c>
       <c r="E109" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="G109" t="str">
-        <f t="shared" si="4"/>
-        <v>Tony Mroczkowski                \\</v>
+        <f t="shared" si="11"/>
+        <v>Pavel Naselsky                  \\</v>
       </c>
       <c r="I109">
-        <f t="shared" si="5"/>
-        <v>16</v>
+        <f t="shared" si="12"/>
+        <v>14</v>
       </c>
       <c r="J109">
-        <f t="shared" si="6"/>
-        <v>16</v>
+        <f t="shared" si="13"/>
+        <v>18</v>
       </c>
       <c r="K109" t="str">
-        <f t="shared" si="7"/>
-        <v xml:space="preserve">                </v>
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">                  </v>
       </c>
     </row>
     <row r="110" spans="2:11">
       <c r="B110" t="s">
-        <v>233</v>
-      </c>
-      <c r="C110" t="s">
-        <v>239</v>
+        <v>168</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>241</v>
       </c>
       <c r="D110" t="s">
         <v>158</v>
       </c>
       <c r="E110" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="G110" t="str">
-        <f t="shared" si="4"/>
-        <v>Pavel Naselsky                  \\</v>
+        <f t="shared" si="11"/>
+        <v>Federico Nati                   \\</v>
       </c>
       <c r="I110">
-        <f t="shared" si="5"/>
-        <v>14</v>
+        <f t="shared" si="12"/>
+        <v>13</v>
       </c>
       <c r="J110">
-        <f t="shared" si="6"/>
-        <v>18</v>
+        <f t="shared" si="13"/>
+        <v>19</v>
       </c>
       <c r="K110" t="str">
-        <f t="shared" si="7"/>
-        <v xml:space="preserve">                  </v>
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">                   </v>
       </c>
     </row>
     <row r="111" spans="2:11">
       <c r="B111" t="s">
-        <v>168</v>
-      </c>
-      <c r="C111" s="1" t="s">
-        <v>241</v>
+        <v>243</v>
+      </c>
+      <c r="C111" t="s">
+        <v>244</v>
       </c>
       <c r="D111" t="s">
         <v>158</v>
       </c>
       <c r="E111" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="G111" t="str">
-        <f t="shared" si="4"/>
-        <v>Federico Nati                   \\</v>
+        <f t="shared" si="11"/>
+        <v>Elena Orlando                   \\</v>
       </c>
       <c r="I111">
-        <f t="shared" si="5"/>
+        <f t="shared" si="12"/>
         <v>13</v>
       </c>
       <c r="J111">
-        <f t="shared" si="6"/>
+        <f t="shared" si="13"/>
         <v>19</v>
       </c>
       <c r="K111" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">                   </v>
       </c>
     </row>
     <row r="112" spans="2:11">
-      <c r="B112" t="s">
-        <v>243</v>
+      <c r="B112" s="1" t="s">
+        <v>193</v>
       </c>
       <c r="C112" t="s">
-        <v>244</v>
+        <v>192</v>
       </c>
       <c r="D112" t="s">
         <v>158</v>
       </c>
       <c r="E112" t="s">
-        <v>245</v>
+        <v>194</v>
       </c>
       <c r="G112" t="str">
-        <f t="shared" si="4"/>
-        <v>Elena Orlando                   \\</v>
+        <f t="shared" si="11"/>
+        <v>Francesco Piacentini            \\</v>
       </c>
       <c r="I112">
-        <f t="shared" si="5"/>
-        <v>13</v>
+        <f t="shared" si="12"/>
+        <v>20</v>
       </c>
       <c r="J112">
-        <f t="shared" si="6"/>
-        <v>19</v>
+        <f t="shared" si="13"/>
+        <v>12</v>
       </c>
       <c r="K112" t="str">
-        <f t="shared" si="7"/>
-        <v xml:space="preserve">                   </v>
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">            </v>
       </c>
     </row>
     <row r="113" spans="2:11">
@@ -4478,175 +4467,178 @@
         <v>248</v>
       </c>
       <c r="G113" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="11"/>
         <v>Giuseppe Puglisi                \\</v>
       </c>
       <c r="I113">
-        <f t="shared" si="5"/>
+        <f t="shared" si="12"/>
         <v>16</v>
       </c>
       <c r="J113">
-        <f t="shared" si="6"/>
+        <f t="shared" si="13"/>
         <v>16</v>
       </c>
       <c r="K113" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">                </v>
       </c>
     </row>
     <row r="114" spans="2:11">
-      <c r="B114" t="s">
-        <v>249</v>
-      </c>
-      <c r="C114" t="s">
-        <v>250</v>
+      <c r="B114" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>321</v>
       </c>
       <c r="D114" t="s">
         <v>158</v>
       </c>
       <c r="E114" t="s">
-        <v>170</v>
+        <v>320</v>
       </c>
       <c r="G114" t="str">
-        <f t="shared" si="4"/>
-        <v>Christian Reichardt             \\</v>
+        <f t="shared" si="11"/>
+        <v>Benjamin Racine                 \\</v>
       </c>
       <c r="I114">
-        <f t="shared" si="5"/>
-        <v>19</v>
+        <f t="shared" si="12"/>
+        <v>15</v>
       </c>
       <c r="J114">
-        <f t="shared" si="6"/>
-        <v>13</v>
+        <f t="shared" si="13"/>
+        <v>17</v>
       </c>
       <c r="K114" t="str">
-        <f t="shared" si="7"/>
-        <v xml:space="preserve">             </v>
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">                 </v>
       </c>
     </row>
     <row r="115" spans="2:11">
       <c r="B115" t="s">
-        <v>251</v>
-      </c>
-      <c r="C115" s="1" t="s">
-        <v>252</v>
+        <v>249</v>
+      </c>
+      <c r="C115" t="s">
+        <v>250</v>
       </c>
       <c r="D115" t="s">
         <v>158</v>
       </c>
       <c r="E115" t="s">
-        <v>253</v>
+        <v>170</v>
       </c>
       <c r="G115" t="str">
-        <f t="shared" si="4"/>
-        <v>Anirban Roy                     \\</v>
+        <f t="shared" si="11"/>
+        <v>Christian Reichardt             \\</v>
       </c>
       <c r="I115">
-        <f t="shared" si="5"/>
-        <v>11</v>
+        <f t="shared" si="12"/>
+        <v>19</v>
       </c>
       <c r="J115">
-        <f t="shared" si="6"/>
-        <v>21</v>
+        <f t="shared" si="13"/>
+        <v>13</v>
       </c>
       <c r="K115" t="str">
-        <f t="shared" si="7"/>
-        <v xml:space="preserve">                     </v>
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">             </v>
       </c>
     </row>
     <row r="116" spans="2:11">
       <c r="B116" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="D116" t="s">
         <v>158</v>
       </c>
       <c r="E116" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="G116" t="str">
-        <f t="shared" si="4"/>
-        <v>Maria Salatino                  \\</v>
+        <f t="shared" si="11"/>
+        <v>Anirban Roy                     \\</v>
       </c>
       <c r="I116">
-        <f t="shared" si="5"/>
-        <v>14</v>
+        <f t="shared" si="12"/>
+        <v>11</v>
       </c>
       <c r="J116">
-        <f t="shared" si="6"/>
-        <v>18</v>
+        <f t="shared" si="13"/>
+        <v>21</v>
       </c>
       <c r="K116" t="str">
-        <f t="shared" si="7"/>
-        <v xml:space="preserve">                  </v>
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">                     </v>
       </c>
     </row>
     <row r="117" spans="2:11">
-      <c r="B117" s="1" t="s">
-        <v>291</v>
+      <c r="B117" t="s">
+        <v>254</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>292</v>
+        <v>255</v>
       </c>
       <c r="D117" t="s">
         <v>158</v>
       </c>
       <c r="E117" t="s">
-        <v>281</v>
+        <v>256</v>
       </c>
       <c r="G117" t="str">
-        <f t="shared" si="4"/>
-        <v>Benjamin Saliwanchik            \\</v>
+        <f t="shared" si="11"/>
+        <v>Maria Salatino                  \\</v>
       </c>
       <c r="I117">
-        <f t="shared" si="5"/>
-        <v>20</v>
+        <f t="shared" si="12"/>
+        <v>14</v>
       </c>
       <c r="J117">
-        <f t="shared" si="6"/>
-        <v>12</v>
+        <f t="shared" si="13"/>
+        <v>18</v>
       </c>
       <c r="K117" t="str">
-        <f t="shared" si="7"/>
-        <v xml:space="preserve">            </v>
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">                  </v>
       </c>
     </row>
     <row r="118" spans="2:11">
       <c r="B118" s="1" t="s">
-        <v>319</v>
+        <v>290</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>271</v>
+        <v>291</v>
       </c>
       <c r="D118" t="s">
         <v>158</v>
       </c>
+      <c r="E118" t="s">
+        <v>280</v>
+      </c>
       <c r="G118" t="str">
-        <f t="shared" si="4"/>
-        <v>Douglas Scott                   \\</v>
+        <f t="shared" si="11"/>
+        <v>Benjamin Saliwanchik            \\</v>
       </c>
       <c r="I118">
-        <f t="shared" si="5"/>
-        <v>13</v>
+        <f t="shared" si="12"/>
+        <v>20</v>
       </c>
       <c r="J118">
-        <f t="shared" si="6"/>
-        <v>19</v>
+        <f t="shared" si="13"/>
+        <v>12</v>
       </c>
       <c r="K118" t="str">
-        <f t="shared" si="7"/>
-        <v xml:space="preserve">                   </v>
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">            </v>
       </c>
     </row>
     <row r="119" spans="2:11">
       <c r="B119" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="C119" s="1" t="s">
         <v>302</v>
-      </c>
-      <c r="C119" s="1" t="s">
-        <v>303</v>
       </c>
       <c r="D119" t="s">
         <v>158</v>
@@ -4655,19 +4647,19 @@
         <v>224</v>
       </c>
       <c r="G119" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="11"/>
         <v>Neelima Sehgal                  \\</v>
       </c>
       <c r="I119">
-        <f t="shared" si="5"/>
+        <f t="shared" si="12"/>
         <v>14</v>
       </c>
       <c r="J119">
-        <f t="shared" si="6"/>
+        <f t="shared" si="13"/>
         <v>18</v>
       </c>
       <c r="K119" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">                  </v>
       </c>
     </row>
@@ -4685,1225 +4677,1269 @@
         <v>259</v>
       </c>
       <c r="G120" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="11"/>
         <v>Sarah Shandera                  \\</v>
       </c>
       <c r="I120">
-        <f t="shared" si="5"/>
+        <f t="shared" si="12"/>
         <v>14</v>
       </c>
       <c r="J120">
-        <f t="shared" si="6"/>
+        <f t="shared" si="13"/>
         <v>18</v>
       </c>
       <c r="K120" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">                  </v>
       </c>
     </row>
     <row r="121" spans="2:11">
       <c r="B121" t="s">
-        <v>260</v>
-      </c>
-      <c r="C121" s="1" t="s">
-        <v>261</v>
+        <v>188</v>
+      </c>
+      <c r="C121" t="s">
+        <v>319</v>
       </c>
       <c r="D121" t="s">
         <v>158</v>
       </c>
       <c r="E121" t="s">
-        <v>262</v>
+        <v>189</v>
       </c>
       <c r="G121" t="str">
-        <f t="shared" si="4"/>
-        <v>An\v{z}e Slosar                 \\</v>
+        <f t="shared" si="11"/>
+        <v>Erik Shirokoff                  \\</v>
       </c>
       <c r="I121">
-        <f t="shared" si="5"/>
-        <v>15</v>
+        <f t="shared" si="12"/>
+        <v>14</v>
       </c>
       <c r="J121">
-        <f t="shared" si="6"/>
-        <v>17</v>
+        <f t="shared" si="13"/>
+        <v>18</v>
       </c>
       <c r="K121" t="str">
-        <f t="shared" si="7"/>
-        <v xml:space="preserve">                 </v>
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">                  </v>
       </c>
     </row>
     <row r="122" spans="2:11">
       <c r="B122" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D122" t="s">
         <v>158</v>
       </c>
       <c r="E122" t="s">
-        <v>187</v>
+        <v>262</v>
       </c>
       <c r="G122" t="str">
-        <f t="shared" si="4"/>
-        <v>Aritoki Suzuki                  \\</v>
+        <f t="shared" si="11"/>
+        <v>An\v{z}e Slosar                 \\</v>
       </c>
       <c r="I122">
-        <f t="shared" si="5"/>
-        <v>14</v>
+        <f t="shared" si="12"/>
+        <v>15</v>
       </c>
       <c r="J122">
-        <f t="shared" si="6"/>
-        <v>18</v>
+        <f t="shared" si="13"/>
+        <v>17</v>
       </c>
       <c r="K122" t="str">
-        <f t="shared" si="7"/>
-        <v xml:space="preserve">                  </v>
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">                 </v>
       </c>
     </row>
     <row r="123" spans="2:11">
-      <c r="B123" s="1" t="s">
-        <v>82</v>
+      <c r="B123" t="s">
+        <v>263</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>300</v>
+        <v>264</v>
       </c>
       <c r="D123" t="s">
         <v>158</v>
       </c>
       <c r="E123" t="s">
-        <v>287</v>
+        <v>187</v>
       </c>
       <c r="G123" t="str">
-        <f t="shared" si="4"/>
-        <v>Eric Switzer                    \\</v>
+        <f t="shared" si="11"/>
+        <v>Aritoki Suzuki                  \\</v>
       </c>
       <c r="I123">
-        <f t="shared" si="5"/>
-        <v>12</v>
+        <f t="shared" si="12"/>
+        <v>14</v>
       </c>
       <c r="J123">
-        <f t="shared" si="6"/>
-        <v>20</v>
+        <f t="shared" si="13"/>
+        <v>18</v>
       </c>
       <c r="K123" t="str">
-        <f t="shared" si="7"/>
-        <v xml:space="preserve">                    </v>
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">                  </v>
       </c>
     </row>
     <row r="124" spans="2:11">
       <c r="B124" s="1" t="s">
-        <v>154</v>
+        <v>82</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="D124" t="s">
         <v>158</v>
       </c>
       <c r="E124" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="G124" t="str">
-        <f t="shared" si="4"/>
-        <v>Andrea Tartari                  \\</v>
+        <f t="shared" si="11"/>
+        <v>Eric Switzer                    \\</v>
       </c>
       <c r="I124">
-        <f t="shared" si="5"/>
-        <v>14</v>
+        <f t="shared" si="12"/>
+        <v>12</v>
       </c>
       <c r="J124">
-        <f t="shared" si="6"/>
-        <v>18</v>
+        <f t="shared" si="13"/>
+        <v>20</v>
       </c>
       <c r="K124" t="str">
-        <f t="shared" si="7"/>
-        <v xml:space="preserve">                  </v>
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">                    </v>
       </c>
     </row>
     <row r="125" spans="2:11">
-      <c r="B125" t="s">
-        <v>265</v>
+      <c r="B125" s="1" t="s">
+        <v>154</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>266</v>
+        <v>300</v>
       </c>
       <c r="D125" t="s">
         <v>158</v>
       </c>
       <c r="E125" t="s">
-        <v>267</v>
+        <v>287</v>
       </c>
       <c r="G125" t="str">
-        <f t="shared" si="4"/>
-        <v>Grant Teply                     \\</v>
+        <f t="shared" si="11"/>
+        <v>Andrea Tartari                  \\</v>
       </c>
       <c r="I125">
-        <f t="shared" si="5"/>
-        <v>11</v>
+        <f t="shared" si="12"/>
+        <v>14</v>
       </c>
       <c r="J125">
-        <f t="shared" si="6"/>
-        <v>21</v>
+        <f t="shared" si="13"/>
+        <v>18</v>
       </c>
       <c r="K125" t="str">
-        <f t="shared" si="7"/>
-        <v xml:space="preserve">                     </v>
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">                  </v>
       </c>
     </row>
     <row r="126" spans="2:11">
-      <c r="B126" s="1" t="s">
-        <v>9</v>
+      <c r="B126" t="s">
+        <v>265</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>304</v>
+        <v>266</v>
       </c>
       <c r="D126" t="s">
         <v>158</v>
       </c>
       <c r="E126" t="s">
-        <v>289</v>
+        <v>267</v>
       </c>
       <c r="G126" t="str">
-        <f t="shared" si="4"/>
-        <v>Peter Timbie                    \\</v>
+        <f t="shared" si="11"/>
+        <v>Grant Teply                     \\</v>
       </c>
       <c r="I126">
-        <f t="shared" si="5"/>
-        <v>12</v>
+        <f t="shared" si="12"/>
+        <v>11</v>
       </c>
       <c r="J126">
-        <f t="shared" si="6"/>
-        <v>20</v>
+        <f t="shared" si="13"/>
+        <v>21</v>
       </c>
       <c r="K126" t="str">
-        <f t="shared" si="7"/>
-        <v xml:space="preserve">                    </v>
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">                     </v>
       </c>
     </row>
     <row r="127" spans="2:11">
-      <c r="B127" t="s">
-        <v>268</v>
+      <c r="B127" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>269</v>
+        <v>303</v>
       </c>
       <c r="D127" t="s">
         <v>158</v>
       </c>
       <c r="E127" t="s">
-        <v>270</v>
+        <v>288</v>
       </c>
       <c r="G127" t="str">
-        <f t="shared" si="4"/>
-        <v>Matthieu Tristram               \\</v>
+        <f t="shared" si="11"/>
+        <v>Peter Timbie                    \\</v>
       </c>
       <c r="I127">
-        <f t="shared" si="5"/>
-        <v>17</v>
+        <f t="shared" si="12"/>
+        <v>12</v>
       </c>
       <c r="J127">
-        <f t="shared" si="6"/>
-        <v>15</v>
+        <f t="shared" si="13"/>
+        <v>20</v>
       </c>
       <c r="K127" t="str">
-        <f t="shared" si="7"/>
-        <v xml:space="preserve">               </v>
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">                    </v>
       </c>
     </row>
     <row r="128" spans="2:11">
-      <c r="B128" s="1" t="s">
-        <v>291</v>
+      <c r="B128" t="s">
+        <v>268</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>295</v>
+        <v>269</v>
       </c>
       <c r="D128" t="s">
         <v>158</v>
       </c>
       <c r="E128" t="s">
-        <v>283</v>
+        <v>270</v>
       </c>
       <c r="G128" t="str">
-        <f t="shared" si="4"/>
-        <v>Benjamin Wallisch               \\</v>
+        <f t="shared" si="11"/>
+        <v>Matthieu Tristram               \\</v>
       </c>
       <c r="I128">
-        <f t="shared" si="5"/>
+        <f t="shared" si="12"/>
         <v>17</v>
       </c>
       <c r="J128">
-        <f t="shared" si="6"/>
+        <f t="shared" si="13"/>
         <v>15</v>
       </c>
       <c r="K128" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">               </v>
       </c>
     </row>
     <row r="129" spans="2:11">
-      <c r="B129" t="s">
-        <v>271</v>
+      <c r="B129" s="1" t="s">
+        <v>322</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>272</v>
+        <v>323</v>
       </c>
       <c r="D129" t="s">
         <v>158</v>
       </c>
       <c r="E129" t="s">
-        <v>273</v>
+        <v>283</v>
       </c>
       <c r="G129" t="str">
-        <f t="shared" si="4"/>
-        <v>Scott Watson                    \\</v>
+        <f t="shared" si="11"/>
+        <v>Caterina Umilt\`{a}             \\</v>
       </c>
       <c r="I129">
-        <f t="shared" si="5"/>
-        <v>12</v>
+        <f t="shared" si="12"/>
+        <v>19</v>
       </c>
       <c r="J129">
-        <f t="shared" si="6"/>
-        <v>20</v>
+        <f t="shared" si="13"/>
+        <v>13</v>
       </c>
       <c r="K129" t="str">
-        <f t="shared" si="7"/>
-        <v xml:space="preserve">                    </v>
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">             </v>
       </c>
     </row>
     <row r="130" spans="2:11">
-      <c r="B130" t="s">
-        <v>274</v>
+      <c r="B130" s="1" t="s">
+        <v>290</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>275</v>
+        <v>294</v>
       </c>
       <c r="D130" t="s">
         <v>158</v>
       </c>
       <c r="E130" t="s">
+        <v>282</v>
+      </c>
+      <c r="G130" t="str">
+        <f t="shared" si="11"/>
+        <v>Benjamin Wallisch               \\</v>
+      </c>
+      <c r="I130">
+        <f t="shared" si="12"/>
+        <v>17</v>
+      </c>
+      <c r="J130">
+        <f t="shared" si="13"/>
+        <v>15</v>
+      </c>
+      <c r="K130" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">               </v>
+      </c>
+    </row>
+    <row r="131" spans="2:11">
+      <c r="B131" t="s">
+        <v>271</v>
+      </c>
+      <c r="C131" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="D131" t="s">
+        <v>158</v>
+      </c>
+      <c r="E131" t="s">
+        <v>273</v>
+      </c>
+      <c r="G131" t="str">
+        <f t="shared" si="11"/>
+        <v>Scott Watson                    \\</v>
+      </c>
+      <c r="I131">
+        <f t="shared" si="12"/>
+        <v>12</v>
+      </c>
+      <c r="J131">
+        <f t="shared" si="13"/>
+        <v>20</v>
+      </c>
+      <c r="K131" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">                    </v>
+      </c>
+    </row>
+    <row r="132" spans="2:11">
+      <c r="B132" t="s">
+        <v>274</v>
+      </c>
+      <c r="C132" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="D132" t="s">
+        <v>158</v>
+      </c>
+      <c r="E132" t="s">
         <v>60</v>
       </c>
-      <c r="G130" t="str">
-        <f t="shared" si="4"/>
+      <c r="G132" t="str">
+        <f t="shared" si="11"/>
         <v>Edward J. Wollack               \\</v>
       </c>
-      <c r="I130">
-        <f t="shared" si="5"/>
+      <c r="I132">
+        <f t="shared" si="12"/>
         <v>17</v>
       </c>
-      <c r="J130">
-        <f t="shared" si="6"/>
+      <c r="J132">
+        <f t="shared" si="13"/>
         <v>15</v>
       </c>
-      <c r="K130" t="str">
-        <f t="shared" si="7"/>
+      <c r="K132" t="str">
+        <f t="shared" si="4"/>
         <v xml:space="preserve">               </v>
       </c>
     </row>
-    <row r="131" spans="2:11">
-      <c r="G131" t="str">
-        <f t="shared" si="4"/>
+    <row r="133" spans="2:11">
+      <c r="B133" s="3"/>
+      <c r="C133"/>
+      <c r="G133" t="str">
+        <f t="shared" si="8"/>
         <v xml:space="preserve">                                \\</v>
       </c>
-      <c r="I131">
-        <f t="shared" si="5"/>
+      <c r="I133">
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
-      <c r="J131">
-        <f t="shared" si="6"/>
+      <c r="J133">
+        <f t="shared" si="10"/>
         <v>31</v>
       </c>
-      <c r="K131" t="str">
-        <f t="shared" si="7"/>
-        <v xml:space="preserve">                               </v>
-      </c>
-    </row>
-    <row r="132" spans="2:11">
-      <c r="G132" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">                                \\</v>
-      </c>
-      <c r="I132">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="J132">
-        <f t="shared" si="6"/>
-        <v>31</v>
-      </c>
-      <c r="K132" t="str">
-        <f t="shared" si="7"/>
-        <v xml:space="preserve">                               </v>
-      </c>
-    </row>
-    <row r="133" spans="2:11">
-      <c r="G133" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">                                \\</v>
-      </c>
-      <c r="I133">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="J133">
-        <f t="shared" si="6"/>
-        <v>31</v>
-      </c>
       <c r="K133" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">                               </v>
       </c>
     </row>
     <row r="134" spans="2:11">
       <c r="G134" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v xml:space="preserve">                                \\</v>
       </c>
       <c r="I134">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="J134">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>31</v>
       </c>
       <c r="K134" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">                               </v>
       </c>
     </row>
     <row r="135" spans="2:11">
       <c r="G135" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v xml:space="preserve">                                \\</v>
       </c>
       <c r="I135">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="J135">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>31</v>
       </c>
       <c r="K135" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">                               </v>
       </c>
     </row>
     <row r="136" spans="2:11">
       <c r="G136" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v xml:space="preserve">                                \\</v>
       </c>
       <c r="I136">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="J136">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>31</v>
       </c>
       <c r="K136" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">                               </v>
       </c>
     </row>
     <row r="137" spans="2:11">
       <c r="G137" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v xml:space="preserve">                                \\</v>
       </c>
       <c r="I137">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="J137">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>31</v>
       </c>
       <c r="K137" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">                               </v>
       </c>
     </row>
     <row r="138" spans="2:11">
-      <c r="B138" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="C138" t="s">
-        <v>149</v>
-      </c>
-      <c r="D138" t="s">
-        <v>158</v>
-      </c>
       <c r="G138" t="str">
-        <f t="shared" ref="G138:G179" si="8">CONCATENATE(B138," ",C138,K138,"\\")</f>
-        <v>Martin White                    \\</v>
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">                                \\</v>
       </c>
       <c r="I138">
-        <f t="shared" ref="I138:I179" si="9">LEN(B138) + LEN(C138) +1</f>
-        <v>12</v>
+        <f t="shared" si="9"/>
+        <v>1</v>
       </c>
       <c r="J138">
-        <f t="shared" ref="J138:J179" si="10">IF(I138&lt;30,(32-I138),3)</f>
-        <v>20</v>
+        <f t="shared" si="10"/>
+        <v>31</v>
       </c>
       <c r="K138" t="str">
-        <f t="shared" ref="K138:K179" si="11">REPT(" ",J138)</f>
-        <v xml:space="preserve">                    </v>
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">                               </v>
       </c>
     </row>
     <row r="139" spans="2:11">
       <c r="B139" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C139" t="s">
+        <v>149</v>
+      </c>
+      <c r="D139" t="s">
+        <v>158</v>
+      </c>
+      <c r="G139" t="str">
+        <f t="shared" ref="G139:G180" si="14">CONCATENATE(B139," ",C139,K139,"\\")</f>
+        <v>Martin White                    \\</v>
+      </c>
+      <c r="I139">
+        <f t="shared" ref="I139:I180" si="15">LEN(B139) + LEN(C139) +1</f>
+        <v>12</v>
+      </c>
+      <c r="J139">
+        <f t="shared" ref="J139:J180" si="16">IF(I139&lt;30,(32-I139),3)</f>
+        <v>20</v>
+      </c>
+      <c r="K139" t="str">
+        <f t="shared" ref="K139:K180" si="17">REPT(" ",J139)</f>
+        <v xml:space="preserve">                    </v>
+      </c>
+    </row>
+    <row r="140" spans="2:11">
+      <c r="B140" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C139" s="1" t="s">
+      <c r="C140" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D139" t="s">
-        <v>8</v>
-      </c>
-      <c r="G139" t="str">
-        <f>CONCATENATE(B139," ",C139,K139,"\\")</f>
+      <c r="D140" t="s">
+        <v>8</v>
+      </c>
+      <c r="G140" t="str">
+        <f>CONCATENATE(B140," ",C140,K140,"\\")</f>
         <v>Kim Boddy                       \\</v>
       </c>
-      <c r="I139">
-        <f>LEN(B139) + LEN(C139) +1</f>
+      <c r="I140">
+        <f>LEN(B140) + LEN(C140) +1</f>
         <v>9</v>
       </c>
-      <c r="J139">
-        <f>IF(I139&lt;30,(32-I139),3)</f>
+      <c r="J140">
+        <f>IF(I140&lt;30,(32-I140),3)</f>
         <v>23</v>
       </c>
-      <c r="K139" t="str">
-        <f>REPT(" ",J139)</f>
+      <c r="K140" t="str">
+        <f>REPT(" ",J140)</f>
         <v xml:space="preserve">                       </v>
-      </c>
-    </row>
-    <row r="140" spans="2:11">
-      <c r="G140" t="str">
-        <f t="shared" si="8"/>
-        <v xml:space="preserve">                                \\</v>
-      </c>
-      <c r="I140">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="J140">
-        <f t="shared" si="10"/>
-        <v>31</v>
-      </c>
-      <c r="K140" t="str">
-        <f t="shared" si="11"/>
-        <v xml:space="preserve">                               </v>
       </c>
     </row>
     <row r="141" spans="2:11">
       <c r="G141" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v xml:space="preserve">                                \\</v>
       </c>
       <c r="I141">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="J141">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>31</v>
       </c>
       <c r="K141" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v xml:space="preserve">                               </v>
       </c>
     </row>
     <row r="142" spans="2:11">
       <c r="G142" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v xml:space="preserve">                                \\</v>
       </c>
       <c r="I142">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="J142">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>31</v>
       </c>
       <c r="K142" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v xml:space="preserve">                               </v>
       </c>
     </row>
     <row r="143" spans="2:11">
       <c r="G143" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v xml:space="preserve">                                \\</v>
       </c>
       <c r="I143">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="J143">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>31</v>
       </c>
       <c r="K143" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v xml:space="preserve">                               </v>
       </c>
     </row>
     <row r="144" spans="2:11">
       <c r="G144" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v xml:space="preserve">                                \\</v>
       </c>
       <c r="I144">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="J144">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>31</v>
       </c>
       <c r="K144" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v xml:space="preserve">                               </v>
       </c>
     </row>
     <row r="145" spans="7:11">
       <c r="G145" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v xml:space="preserve">                                \\</v>
       </c>
       <c r="I145">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="J145">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>31</v>
       </c>
       <c r="K145" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v xml:space="preserve">                               </v>
       </c>
     </row>
     <row r="146" spans="7:11">
       <c r="G146" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v xml:space="preserve">                                \\</v>
       </c>
       <c r="I146">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="J146">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>31</v>
       </c>
       <c r="K146" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v xml:space="preserve">                               </v>
       </c>
     </row>
     <row r="147" spans="7:11">
       <c r="G147" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v xml:space="preserve">                                \\</v>
       </c>
       <c r="I147">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="J147">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>31</v>
       </c>
       <c r="K147" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v xml:space="preserve">                               </v>
       </c>
     </row>
     <row r="148" spans="7:11">
       <c r="G148" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v xml:space="preserve">                                \\</v>
       </c>
       <c r="I148">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="J148">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>31</v>
       </c>
       <c r="K148" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v xml:space="preserve">                               </v>
       </c>
     </row>
     <row r="149" spans="7:11">
       <c r="G149" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v xml:space="preserve">                                \\</v>
       </c>
       <c r="I149">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="J149">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>31</v>
       </c>
       <c r="K149" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v xml:space="preserve">                               </v>
       </c>
     </row>
     <row r="150" spans="7:11">
       <c r="G150" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v xml:space="preserve">                                \\</v>
       </c>
       <c r="I150">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="J150">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>31</v>
       </c>
       <c r="K150" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v xml:space="preserve">                               </v>
       </c>
     </row>
     <row r="151" spans="7:11">
       <c r="G151" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v xml:space="preserve">                                \\</v>
       </c>
       <c r="I151">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="J151">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>31</v>
       </c>
       <c r="K151" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v xml:space="preserve">                               </v>
       </c>
     </row>
     <row r="152" spans="7:11">
       <c r="G152" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v xml:space="preserve">                                \\</v>
       </c>
       <c r="I152">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="J152">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>31</v>
       </c>
       <c r="K152" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v xml:space="preserve">                               </v>
       </c>
     </row>
     <row r="153" spans="7:11">
       <c r="G153" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v xml:space="preserve">                                \\</v>
       </c>
       <c r="I153">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="J153">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>31</v>
       </c>
       <c r="K153" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v xml:space="preserve">                               </v>
       </c>
     </row>
     <row r="154" spans="7:11">
       <c r="G154" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v xml:space="preserve">                                \\</v>
       </c>
       <c r="I154">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="J154">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>31</v>
       </c>
       <c r="K154" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v xml:space="preserve">                               </v>
       </c>
     </row>
     <row r="155" spans="7:11">
       <c r="G155" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v xml:space="preserve">                                \\</v>
       </c>
       <c r="I155">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="J155">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>31</v>
       </c>
       <c r="K155" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v xml:space="preserve">                               </v>
       </c>
     </row>
     <row r="156" spans="7:11">
       <c r="G156" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v xml:space="preserve">                                \\</v>
       </c>
       <c r="I156">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="J156">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>31</v>
       </c>
       <c r="K156" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v xml:space="preserve">                               </v>
       </c>
     </row>
     <row r="157" spans="7:11">
       <c r="G157" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v xml:space="preserve">                                \\</v>
       </c>
       <c r="I157">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="J157">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>31</v>
       </c>
       <c r="K157" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v xml:space="preserve">                               </v>
       </c>
     </row>
     <row r="158" spans="7:11">
       <c r="G158" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v xml:space="preserve">                                \\</v>
       </c>
       <c r="I158">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="J158">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>31</v>
       </c>
       <c r="K158" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v xml:space="preserve">                               </v>
       </c>
     </row>
     <row r="159" spans="7:11">
       <c r="G159" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v xml:space="preserve">                                \\</v>
       </c>
       <c r="I159">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="J159">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>31</v>
       </c>
       <c r="K159" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v xml:space="preserve">                               </v>
       </c>
     </row>
     <row r="160" spans="7:11">
       <c r="G160" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v xml:space="preserve">                                \\</v>
       </c>
       <c r="I160">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="J160">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>31</v>
       </c>
       <c r="K160" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v xml:space="preserve">                               </v>
       </c>
     </row>
     <row r="161" spans="7:11">
       <c r="G161" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v xml:space="preserve">                                \\</v>
       </c>
       <c r="I161">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="J161">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>31</v>
       </c>
       <c r="K161" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v xml:space="preserve">                               </v>
       </c>
     </row>
     <row r="162" spans="7:11">
       <c r="G162" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v xml:space="preserve">                                \\</v>
       </c>
       <c r="I162">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="J162">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>31</v>
       </c>
       <c r="K162" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v xml:space="preserve">                               </v>
       </c>
     </row>
     <row r="163" spans="7:11">
       <c r="G163" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v xml:space="preserve">                                \\</v>
       </c>
       <c r="I163">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="J163">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>31</v>
       </c>
       <c r="K163" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v xml:space="preserve">                               </v>
       </c>
     </row>
     <row r="164" spans="7:11">
       <c r="G164" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v xml:space="preserve">                                \\</v>
       </c>
       <c r="I164">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="J164">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>31</v>
       </c>
       <c r="K164" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v xml:space="preserve">                               </v>
       </c>
     </row>
     <row r="165" spans="7:11">
       <c r="G165" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v xml:space="preserve">                                \\</v>
       </c>
       <c r="I165">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="J165">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>31</v>
       </c>
       <c r="K165" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v xml:space="preserve">                               </v>
       </c>
     </row>
     <row r="166" spans="7:11">
       <c r="G166" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v xml:space="preserve">                                \\</v>
       </c>
       <c r="I166">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="J166">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>31</v>
       </c>
       <c r="K166" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v xml:space="preserve">                               </v>
       </c>
     </row>
     <row r="167" spans="7:11">
       <c r="G167" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v xml:space="preserve">                                \\</v>
       </c>
       <c r="I167">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="J167">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>31</v>
       </c>
       <c r="K167" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v xml:space="preserve">                               </v>
       </c>
     </row>
     <row r="168" spans="7:11">
       <c r="G168" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v xml:space="preserve">                                \\</v>
       </c>
       <c r="I168">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="J168">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>31</v>
       </c>
       <c r="K168" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v xml:space="preserve">                               </v>
       </c>
     </row>
     <row r="169" spans="7:11">
       <c r="G169" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v xml:space="preserve">                                \\</v>
       </c>
       <c r="I169">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="J169">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>31</v>
       </c>
       <c r="K169" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v xml:space="preserve">                               </v>
       </c>
     </row>
     <row r="170" spans="7:11">
       <c r="G170" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v xml:space="preserve">                                \\</v>
       </c>
       <c r="I170">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="J170">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>31</v>
       </c>
       <c r="K170" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v xml:space="preserve">                               </v>
       </c>
     </row>
     <row r="171" spans="7:11">
       <c r="G171" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v xml:space="preserve">                                \\</v>
       </c>
       <c r="I171">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="J171">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>31</v>
       </c>
       <c r="K171" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v xml:space="preserve">                               </v>
       </c>
     </row>
     <row r="172" spans="7:11">
       <c r="G172" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v xml:space="preserve">                                \\</v>
       </c>
       <c r="I172">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="J172">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>31</v>
       </c>
       <c r="K172" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v xml:space="preserve">                               </v>
       </c>
     </row>
     <row r="173" spans="7:11">
       <c r="G173" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v xml:space="preserve">                                \\</v>
       </c>
       <c r="I173">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="J173">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>31</v>
       </c>
       <c r="K173" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v xml:space="preserve">                               </v>
       </c>
     </row>
     <row r="174" spans="7:11">
       <c r="G174" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v xml:space="preserve">                                \\</v>
       </c>
       <c r="I174">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="J174">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>31</v>
       </c>
       <c r="K174" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v xml:space="preserve">                               </v>
       </c>
     </row>
     <row r="175" spans="7:11">
       <c r="G175" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v xml:space="preserve">                                \\</v>
       </c>
       <c r="I175">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="J175">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>31</v>
       </c>
       <c r="K175" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v xml:space="preserve">                               </v>
       </c>
     </row>
     <row r="176" spans="7:11">
       <c r="G176" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v xml:space="preserve">                                \\</v>
       </c>
       <c r="I176">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="J176">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>31</v>
       </c>
       <c r="K176" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v xml:space="preserve">                               </v>
       </c>
     </row>
     <row r="177" spans="7:11">
       <c r="G177" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v xml:space="preserve">                                \\</v>
       </c>
       <c r="I177">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="J177">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>31</v>
       </c>
       <c r="K177" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v xml:space="preserve">                               </v>
       </c>
     </row>
     <row r="178" spans="7:11">
       <c r="G178" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v xml:space="preserve">                                \\</v>
       </c>
       <c r="I178">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="J178">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>31</v>
       </c>
       <c r="K178" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v xml:space="preserve">                               </v>
       </c>
     </row>
     <row r="179" spans="7:11">
       <c r="G179" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v xml:space="preserve">                                \\</v>
       </c>
       <c r="I179">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="J179">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>31</v>
       </c>
       <c r="K179" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v xml:space="preserve">                               </v>
       </c>
     </row>
+    <row r="180" spans="7:11">
+      <c r="G180" t="str">
+        <f t="shared" si="14"/>
+        <v xml:space="preserve">                                \\</v>
+      </c>
+      <c r="I180">
+        <f t="shared" si="15"/>
+        <v>1</v>
+      </c>
+      <c r="J180">
+        <f t="shared" si="16"/>
+        <v>31</v>
+      </c>
+      <c r="K180" t="str">
+        <f t="shared" si="17"/>
+        <v xml:space="preserve">                               </v>
+      </c>
+    </row>
   </sheetData>
-  <sortState ref="B10:E77">
-    <sortCondition ref="C10:C77"/>
+  <sortState ref="B10:E76">
+    <sortCondition ref="C10:C76"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
adding author affiliations to xls doc
</commit_message>
<xml_diff>
--- a/ReferenceDocuments/ReportAuthors.xlsx
+++ b/ReferenceDocuments/ReportAuthors.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="343">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="360">
   <si>
     <t>Report Authors</t>
   </si>
@@ -112,9 +112,6 @@
     <t>Borrill</t>
   </si>
   <si>
-    <t>Francois</t>
-  </si>
-  <si>
     <t>Boulanger</t>
   </si>
   <si>
@@ -452,9 +449,6 @@
   </si>
   <si>
     <t>Wen</t>
-  </si>
-  <si>
-    <t>UMN</t>
   </si>
   <si>
     <t>Martin</t>
@@ -1057,22 +1051,79 @@
     <t>Hlo\v{z}ek</t>
   </si>
   <si>
-    <t>Valentino</t>
-  </si>
-  <si>
     <t>Department of Astronomy \&amp; Astrophysics and Dunlap Institute, University of Toronto</t>
   </si>
   <si>
-    <t>12/18/2018, 3 pm.</t>
-  </si>
-  <si>
     <t>UC Berkeley / LBNL</t>
   </si>
   <si>
     <t>University of Oslo</t>
   </si>
   <si>
-    <t>Eleonora Di</t>
+    <t> Instituto de Física de Cantabria (CSIC-Universidad de Cantabria), Avda. de los Castros s/n, Santander, Spain </t>
+  </si>
+  <si>
+    <t>School of Physics, Indian Institute of Science Education and Research Thiruvananthapuram, Maruthamala PO, Vithura, Thiruvananthapuram, 695551 Kerala, India</t>
+  </si>
+  <si>
+    <t>Lawrence Berkeley National Laboratory, Berkeley, CA, USA , Space Sciences Laboratory, University of California, Berkeley, CA, USA</t>
+  </si>
+  <si>
+    <t>Institut d’Astrophysique Spatiale, Orsay, France</t>
+  </si>
+  <si>
+    <t>Villanova University</t>
+  </si>
+  <si>
+    <t>University of Southern California</t>
+  </si>
+  <si>
+    <t>Canadian Institute for Theoretical Astrophysics, University of Toronto, 60 St. George Street, Toronto, Canada</t>
+  </si>
+  <si>
+    <t>Institut Lagrange, LPNHE, place Jussieu 4, 75005 Paris, France</t>
+  </si>
+  <si>
+    <t>Flatiron Institute</t>
+  </si>
+  <si>
+    <t>JPL</t>
+  </si>
+  <si>
+    <t>University of California, Berkeley</t>
+  </si>
+  <si>
+    <t>Institute for Advanced Study, Flatiron Institute</t>
+  </si>
+  <si>
+    <t>UC Davis</t>
+  </si>
+  <si>
+    <t>University of Wisconsin - Madison</t>
+  </si>
+  <si>
+    <t>Department of Astrophysical Sciences, Princeton University</t>
+  </si>
+  <si>
+    <t>CEA Saclay, DRF/Irfu/SPP, 91191 Gif-sur-Yvette Cedex, France</t>
+  </si>
+  <si>
+    <t>??</t>
+  </si>
+  <si>
+    <t>Institute for Advanced Study, Princeton</t>
+  </si>
+  <si>
+    <t>University of British Columbia, Canada</t>
+  </si>
+  <si>
+    <t>Institut d’Astrophysique Spatiale, CNRS, Univ. Paris-Sud, Universite´ Paris-Saclay, Bat. 121, 91405 Orsay cedex, France</t>
+  </si>
+  <si>
+    <t>San Diego Supercomputer Center, UC San Diego</t>
+  </si>
+  <si>
+    <t>12/18/2018, 5 pm.</t>
   </si>
 </sst>
 </file>
@@ -1524,8 +1575,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:K188"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B79" sqref="B79"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -1555,25 +1606,25 @@
       </c>
       <c r="B3"/>
       <c r="C3" s="1" t="s">
-        <v>339</v>
+        <v>359</v>
       </c>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="2" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B4"/>
       <c r="C4" s="1" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="2" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B5"/>
       <c r="C5" s="1" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -1581,10 +1632,10 @@
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="4" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B7" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -1605,16 +1656,16 @@
         <v>5</v>
       </c>
       <c r="G9" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="I9" t="s">
+        <v>303</v>
+      </c>
+      <c r="J9" t="s">
+        <v>304</v>
+      </c>
+      <c r="K9" t="s">
         <v>305</v>
-      </c>
-      <c r="J9" t="s">
-        <v>306</v>
-      </c>
-      <c r="K9" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -1628,7 +1679,7 @@
         <v>8</v>
       </c>
       <c r="E10" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="G10" t="str">
         <f>CONCATENATE(B10," ",C10,K10,"\\")</f>
@@ -1718,7 +1769,7 @@
         <v>8</v>
       </c>
       <c r="E13" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="G13" t="str">
         <f t="shared" si="0"/>
@@ -1747,6 +1798,9 @@
       <c r="D14" t="s">
         <v>8</v>
       </c>
+      <c r="E14" t="s">
+        <v>338</v>
+      </c>
       <c r="G14" t="str">
         <f t="shared" si="0"/>
         <v>Belen Barreiro                  \\</v>
@@ -1804,6 +1858,9 @@
       <c r="D16" t="s">
         <v>8</v>
       </c>
+      <c r="E16" t="s">
+        <v>339</v>
+      </c>
       <c r="G16" t="str">
         <f t="shared" si="0"/>
         <v>Soumen Basak                    \\</v>
@@ -1831,6 +1888,9 @@
       <c r="D17" t="s">
         <v>8</v>
       </c>
+      <c r="E17" t="s">
+        <v>91</v>
+      </c>
       <c r="G17" t="str">
         <f t="shared" si="0"/>
         <v>Nicholas Battaglia              \\</v>
@@ -1850,16 +1910,16 @@
     </row>
     <row r="18" spans="2:11">
       <c r="B18" t="s">
+        <v>168</v>
+      </c>
+      <c r="C18" t="s">
+        <v>169</v>
+      </c>
+      <c r="D18" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" t="s">
         <v>170</v>
-      </c>
-      <c r="C18" t="s">
-        <v>171</v>
-      </c>
-      <c r="D18" t="s">
-        <v>8</v>
-      </c>
-      <c r="E18" t="s">
-        <v>172</v>
       </c>
       <c r="G18" t="str">
         <f t="shared" si="0"/>
@@ -1880,7 +1940,7 @@
     </row>
     <row r="19" spans="2:11">
       <c r="B19" s="1" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>26</v>
@@ -1889,7 +1949,7 @@
         <v>8</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="G19" t="str">
         <f t="shared" si="0"/>
@@ -1948,6 +2008,9 @@
       <c r="D21" t="s">
         <v>8</v>
       </c>
+      <c r="E21" t="s">
+        <v>340</v>
+      </c>
       <c r="G21" t="str">
         <f t="shared" si="0"/>
         <v>Julian Borrill                  \\</v>
@@ -1967,43 +2030,46 @@
     </row>
     <row r="22" spans="2:11">
       <c r="B22" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="D22" t="s">
         <v>8</v>
+      </c>
+      <c r="E22" t="s">
+        <v>341</v>
       </c>
       <c r="G22" t="str">
         <f t="shared" si="0"/>
-        <v>Francois Boulanger              \\</v>
+        <v>Fran\c{c}ois Boulanger          \\</v>
       </c>
       <c r="I22">
         <f t="shared" si="1"/>
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="J22">
         <f t="shared" si="2"/>
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="K22" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">              </v>
+        <v xml:space="preserve">          </v>
       </c>
     </row>
     <row r="23" spans="2:11">
       <c r="B23" t="s">
+        <v>33</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="D23" t="s">
+        <v>8</v>
+      </c>
+      <c r="E23" t="s">
         <v>35</v>
-      </c>
-      <c r="D23" t="s">
-        <v>8</v>
-      </c>
-      <c r="E23" t="s">
-        <v>36</v>
       </c>
       <c r="G23" t="str">
         <f t="shared" si="0"/>
@@ -2024,13 +2090,16 @@
     </row>
     <row r="24" spans="2:11">
       <c r="B24" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C24" s="1" t="s">
-        <v>38</v>
-      </c>
       <c r="D24" t="s">
         <v>8</v>
+      </c>
+      <c r="E24" t="s">
+        <v>342</v>
       </c>
       <c r="G24" t="str">
         <f t="shared" si="0"/>
@@ -2051,16 +2120,16 @@
     </row>
     <row r="25" spans="2:11">
       <c r="B25" t="s">
+        <v>38</v>
+      </c>
+      <c r="C25" t="s">
         <v>39</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D25" t="s">
+        <v>8</v>
+      </c>
+      <c r="E25" t="s">
         <v>40</v>
-      </c>
-      <c r="D25" t="s">
-        <v>8</v>
-      </c>
-      <c r="E25" t="s">
-        <v>41</v>
       </c>
       <c r="G25" t="str">
         <f t="shared" si="0"/>
@@ -2081,13 +2150,16 @@
     </row>
     <row r="26" spans="2:11">
       <c r="B26" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C26" s="1" t="s">
-        <v>43</v>
-      </c>
       <c r="D26" t="s">
         <v>8</v>
+      </c>
+      <c r="E26" t="s">
+        <v>53</v>
       </c>
       <c r="G26" t="str">
         <f t="shared" si="0"/>
@@ -2108,16 +2180,16 @@
     </row>
     <row r="27" spans="2:11">
       <c r="B27" t="s">
+        <v>44</v>
+      </c>
+      <c r="C27" t="s">
         <v>45</v>
       </c>
-      <c r="C27" t="s">
+      <c r="D27" t="s">
+        <v>8</v>
+      </c>
+      <c r="E27" t="s">
         <v>46</v>
-      </c>
-      <c r="D27" t="s">
-        <v>8</v>
-      </c>
-      <c r="E27" t="s">
-        <v>47</v>
       </c>
       <c r="G27" t="str">
         <f t="shared" si="0"/>
@@ -2138,16 +2210,16 @@
     </row>
     <row r="28" spans="2:11">
       <c r="B28" t="s">
+        <v>47</v>
+      </c>
+      <c r="C28" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="D28" t="s">
+        <v>8</v>
+      </c>
+      <c r="E28" t="s">
         <v>49</v>
-      </c>
-      <c r="D28" t="s">
-        <v>8</v>
-      </c>
-      <c r="E28" t="s">
-        <v>50</v>
       </c>
       <c r="G28" t="str">
         <f t="shared" si="0"/>
@@ -2168,13 +2240,16 @@
     </row>
     <row r="29" spans="2:11">
       <c r="B29" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C29" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C29" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="D29" t="s">
         <v>8</v>
+      </c>
+      <c r="E29" t="s">
+        <v>343</v>
       </c>
       <c r="G29" t="str">
         <f t="shared" si="0"/>
@@ -2195,16 +2270,16 @@
     </row>
     <row r="30" spans="2:11">
       <c r="B30" t="s">
+        <v>52</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="D30" t="s">
+        <v>8</v>
+      </c>
+      <c r="E30" t="s">
         <v>53</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>312</v>
-      </c>
-      <c r="D30" t="s">
-        <v>8</v>
-      </c>
-      <c r="E30" t="s">
-        <v>54</v>
       </c>
       <c r="G30" t="str">
         <f t="shared" si="0"/>
@@ -2225,13 +2300,16 @@
     </row>
     <row r="31" spans="2:11">
       <c r="B31" s="1" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C31" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="D31" t="s">
         <v>8</v>
+      </c>
+      <c r="E31" t="s">
+        <v>344</v>
       </c>
       <c r="G31" t="str">
         <f t="shared" si="0"/>
@@ -2252,13 +2330,16 @@
     </row>
     <row r="32" spans="2:11">
       <c r="B32" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C32" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C32" s="1" t="s">
-        <v>56</v>
-      </c>
       <c r="D32" t="s">
         <v>8</v>
+      </c>
+      <c r="E32" t="s">
+        <v>345</v>
       </c>
       <c r="G32" t="str">
         <f t="shared" si="0"/>
@@ -2279,16 +2360,16 @@
     </row>
     <row r="33" spans="2:11">
       <c r="B33" t="s">
+        <v>56</v>
+      </c>
+      <c r="C33" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="D33" t="s">
+        <v>8</v>
+      </c>
+      <c r="E33" t="s">
         <v>58</v>
-      </c>
-      <c r="D33" t="s">
-        <v>8</v>
-      </c>
-      <c r="E33" t="s">
-        <v>59</v>
       </c>
       <c r="G33" t="str">
         <f t="shared" si="0"/>
@@ -2309,13 +2390,16 @@
     </row>
     <row r="34" spans="2:11">
       <c r="B34" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C34" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C34" s="1" t="s">
-        <v>61</v>
-      </c>
       <c r="D34" t="s">
         <v>8</v>
+      </c>
+      <c r="E34" t="s">
+        <v>346</v>
       </c>
       <c r="G34" t="str">
         <f t="shared" si="0"/>
@@ -2336,16 +2420,16 @@
     </row>
     <row r="35" spans="2:11">
       <c r="B35" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C35" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="D35" t="s">
         <v>8</v>
       </c>
       <c r="E35" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="G35" t="str">
         <f t="shared" si="0"/>
@@ -2366,16 +2450,16 @@
     </row>
     <row r="36" spans="2:11">
       <c r="B36" t="s">
+        <v>61</v>
+      </c>
+      <c r="C36" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="D36" t="s">
+        <v>8</v>
+      </c>
+      <c r="E36" t="s">
         <v>63</v>
-      </c>
-      <c r="D36" t="s">
-        <v>8</v>
-      </c>
-      <c r="E36" t="s">
-        <v>64</v>
       </c>
       <c r="G36" t="str">
         <f t="shared" si="0"/>
@@ -2396,16 +2480,16 @@
     </row>
     <row r="37" spans="2:11">
       <c r="B37" t="s">
+        <v>64</v>
+      </c>
+      <c r="C37" t="s">
         <v>65</v>
       </c>
-      <c r="C37" t="s">
+      <c r="D37" t="s">
+        <v>8</v>
+      </c>
+      <c r="E37" t="s">
         <v>66</v>
-      </c>
-      <c r="D37" t="s">
-        <v>8</v>
-      </c>
-      <c r="E37" t="s">
-        <v>67</v>
       </c>
       <c r="G37" t="str">
         <f t="shared" si="0"/>
@@ -2426,13 +2510,16 @@
     </row>
     <row r="38" spans="2:11">
       <c r="B38" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C38" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C38" s="1" t="s">
-        <v>69</v>
-      </c>
       <c r="D38" t="s">
         <v>8</v>
+      </c>
+      <c r="E38" t="s">
+        <v>40</v>
       </c>
       <c r="G38" t="str">
         <f t="shared" si="0"/>
@@ -2453,13 +2540,16 @@
     </row>
     <row r="39" spans="2:11">
       <c r="B39" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C39" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C39" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="D39" t="s">
         <v>8</v>
+      </c>
+      <c r="E39" t="s">
+        <v>347</v>
       </c>
       <c r="G39" t="str">
         <f t="shared" si="0"/>
@@ -2480,13 +2570,16 @@
     </row>
     <row r="40" spans="2:11">
       <c r="B40" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C40" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C40" s="1" t="s">
-        <v>73</v>
-      </c>
       <c r="D40" t="s">
         <v>8</v>
+      </c>
+      <c r="E40" t="s">
+        <v>348</v>
       </c>
       <c r="G40" t="str">
         <f t="shared" si="0"/>
@@ -2507,13 +2600,16 @@
     </row>
     <row r="41" spans="2:11">
       <c r="B41" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C41" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C41" s="1" t="s">
-        <v>75</v>
-      </c>
       <c r="D41" t="s">
         <v>8</v>
+      </c>
+      <c r="E41" t="s">
+        <v>91</v>
       </c>
       <c r="G41" t="str">
         <f t="shared" si="0"/>
@@ -2534,16 +2630,16 @@
     </row>
     <row r="42" spans="2:11">
       <c r="B42" t="s">
+        <v>75</v>
+      </c>
+      <c r="C42" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C42" s="1" t="s">
+      <c r="D42" t="s">
+        <v>8</v>
+      </c>
+      <c r="E42" t="s">
         <v>77</v>
-      </c>
-      <c r="D42" t="s">
-        <v>8</v>
-      </c>
-      <c r="E42" t="s">
-        <v>78</v>
       </c>
       <c r="G42" t="str">
         <f t="shared" si="0"/>
@@ -2564,13 +2660,16 @@
     </row>
     <row r="43" spans="2:11">
       <c r="B43" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C43" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C43" s="1" t="s">
-        <v>80</v>
-      </c>
       <c r="D43" t="s">
         <v>8</v>
+      </c>
+      <c r="E43" t="s">
+        <v>349</v>
       </c>
       <c r="G43" t="str">
         <f t="shared" si="0"/>
@@ -2591,16 +2690,16 @@
     </row>
     <row r="44" spans="2:11">
       <c r="B44" t="s">
+        <v>80</v>
+      </c>
+      <c r="C44" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C44" s="1" t="s">
+      <c r="D44" t="s">
+        <v>8</v>
+      </c>
+      <c r="E44" t="s">
         <v>82</v>
-      </c>
-      <c r="D44" t="s">
-        <v>8</v>
-      </c>
-      <c r="E44" t="s">
-        <v>83</v>
       </c>
       <c r="G44" t="str">
         <f t="shared" si="0"/>
@@ -2621,16 +2720,16 @@
     </row>
     <row r="45" spans="2:11">
       <c r="B45" t="s">
+        <v>83</v>
+      </c>
+      <c r="C45" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C45" s="1" t="s">
+      <c r="D45" t="s">
+        <v>8</v>
+      </c>
+      <c r="E45" t="s">
         <v>85</v>
-      </c>
-      <c r="D45" t="s">
-        <v>8</v>
-      </c>
-      <c r="E45" t="s">
-        <v>86</v>
       </c>
       <c r="G45" t="str">
         <f t="shared" si="0"/>
@@ -2651,16 +2750,16 @@
     </row>
     <row r="46" spans="2:11">
       <c r="B46" t="s">
+        <v>86</v>
+      </c>
+      <c r="C46" t="s">
         <v>87</v>
       </c>
-      <c r="C46" t="s">
+      <c r="D46" t="s">
+        <v>8</v>
+      </c>
+      <c r="E46" t="s">
         <v>88</v>
-      </c>
-      <c r="D46" t="s">
-        <v>8</v>
-      </c>
-      <c r="E46" t="s">
-        <v>89</v>
       </c>
       <c r="G46" t="str">
         <f t="shared" si="0"/>
@@ -2681,16 +2780,16 @@
     </row>
     <row r="47" spans="2:11">
       <c r="B47" t="s">
+        <v>89</v>
+      </c>
+      <c r="C47" t="s">
         <v>90</v>
       </c>
-      <c r="C47" t="s">
+      <c r="D47" t="s">
+        <v>8</v>
+      </c>
+      <c r="E47" t="s">
         <v>91</v>
-      </c>
-      <c r="D47" t="s">
-        <v>8</v>
-      </c>
-      <c r="E47" t="s">
-        <v>92</v>
       </c>
       <c r="G47" t="str">
         <f t="shared" si="0"/>
@@ -2711,16 +2810,16 @@
     </row>
     <row r="48" spans="2:11">
       <c r="B48" t="s">
+        <v>92</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D48" t="s">
+        <v>8</v>
+      </c>
+      <c r="E48" t="s">
         <v>93</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="D48" t="s">
-        <v>8</v>
-      </c>
-      <c r="E48" t="s">
-        <v>94</v>
       </c>
       <c r="G48" t="str">
         <f t="shared" si="0"/>
@@ -2741,13 +2840,16 @@
     </row>
     <row r="49" spans="2:11">
       <c r="B49" s="1" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D49" t="s">
         <v>8</v>
+      </c>
+      <c r="E49" t="s">
+        <v>350</v>
       </c>
       <c r="G49" t="str">
         <f t="shared" si="0"/>
@@ -2768,13 +2870,16 @@
     </row>
     <row r="50" spans="2:11">
       <c r="B50" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C50" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="C50" s="1" t="s">
-        <v>97</v>
-      </c>
       <c r="D50" t="s">
         <v>8</v>
+      </c>
+      <c r="E50" t="s">
+        <v>58</v>
       </c>
       <c r="G50" t="str">
         <f t="shared" si="0"/>
@@ -2795,16 +2900,16 @@
     </row>
     <row r="51" spans="2:11">
       <c r="B51" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C51" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D51" t="s">
         <v>8</v>
       </c>
       <c r="E51" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="G51" t="str">
         <f t="shared" si="0"/>
@@ -2825,13 +2930,16 @@
     </row>
     <row r="52" spans="2:11">
       <c r="B52" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C52" t="s">
         <v>98</v>
       </c>
-      <c r="C52" t="s">
-        <v>99</v>
-      </c>
       <c r="D52" t="s">
         <v>8</v>
+      </c>
+      <c r="E52" t="s">
+        <v>347</v>
       </c>
       <c r="G52" t="str">
         <f t="shared" si="0"/>
@@ -2852,13 +2960,16 @@
     </row>
     <row r="53" spans="2:11">
       <c r="B53" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C53" t="s">
         <v>100</v>
       </c>
-      <c r="C53" t="s">
-        <v>101</v>
-      </c>
       <c r="D53" t="s">
         <v>8</v>
+      </c>
+      <c r="E53" t="s">
+        <v>351</v>
       </c>
       <c r="G53" t="str">
         <f t="shared" si="0"/>
@@ -2879,13 +2990,16 @@
     </row>
     <row r="54" spans="2:11">
       <c r="B54" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C54" t="s">
         <v>102</v>
       </c>
-      <c r="C54" t="s">
-        <v>103</v>
-      </c>
       <c r="D54" t="s">
         <v>8</v>
+      </c>
+      <c r="E54" t="s">
+        <v>352</v>
       </c>
       <c r="G54" t="str">
         <f t="shared" si="0"/>
@@ -2906,13 +3020,16 @@
     </row>
     <row r="55" spans="2:11">
       <c r="B55" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C55" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="C55" s="1" t="s">
-        <v>105</v>
-      </c>
       <c r="D55" t="s">
         <v>8</v>
+      </c>
+      <c r="E55" t="s">
+        <v>352</v>
       </c>
       <c r="G55" t="str">
         <f t="shared" si="0"/>
@@ -2933,13 +3050,16 @@
     </row>
     <row r="56" spans="2:11">
       <c r="B56" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C56" t="s">
         <v>106</v>
       </c>
-      <c r="C56" t="s">
-        <v>107</v>
-      </c>
       <c r="D56" t="s">
         <v>8</v>
+      </c>
+      <c r="E56" t="s">
+        <v>353</v>
       </c>
       <c r="G56" t="str">
         <f t="shared" si="0"/>
@@ -2960,16 +3080,16 @@
     </row>
     <row r="57" spans="2:11">
       <c r="B57" t="s">
+        <v>107</v>
+      </c>
+      <c r="C57" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="C57" s="1" t="s">
+      <c r="D57" t="s">
+        <v>8</v>
+      </c>
+      <c r="E57" t="s">
         <v>109</v>
-      </c>
-      <c r="D57" t="s">
-        <v>8</v>
-      </c>
-      <c r="E57" t="s">
-        <v>110</v>
       </c>
       <c r="G57" t="str">
         <f t="shared" si="0"/>
@@ -2990,16 +3110,16 @@
     </row>
     <row r="58" spans="2:11">
       <c r="B58" t="s">
+        <v>110</v>
+      </c>
+      <c r="C58" t="s">
         <v>111</v>
       </c>
-      <c r="C58" t="s">
+      <c r="D58" t="s">
+        <v>8</v>
+      </c>
+      <c r="E58" t="s">
         <v>112</v>
-      </c>
-      <c r="D58" t="s">
-        <v>8</v>
-      </c>
-      <c r="E58" t="s">
-        <v>113</v>
       </c>
       <c r="G58" t="str">
         <f t="shared" si="0"/>
@@ -3020,16 +3140,16 @@
     </row>
     <row r="59" spans="2:11">
       <c r="B59" t="s">
+        <v>113</v>
+      </c>
+      <c r="C59" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="C59" s="1" t="s">
+      <c r="D59" t="s">
+        <v>8</v>
+      </c>
+      <c r="E59" t="s">
         <v>115</v>
-      </c>
-      <c r="D59" t="s">
-        <v>8</v>
-      </c>
-      <c r="E59" t="s">
-        <v>116</v>
       </c>
       <c r="G59" t="str">
         <f t="shared" si="0"/>
@@ -3050,13 +3170,16 @@
     </row>
     <row r="60" spans="2:11">
       <c r="B60" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C60" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="C60" s="1" t="s">
-        <v>118</v>
-      </c>
       <c r="D60" t="s">
         <v>8</v>
+      </c>
+      <c r="E60" t="s">
+        <v>354</v>
       </c>
       <c r="G60" t="str">
         <f t="shared" si="0"/>
@@ -3077,13 +3200,16 @@
     </row>
     <row r="61" spans="2:11">
       <c r="B61" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C61" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="C61" s="1" t="s">
-        <v>120</v>
-      </c>
       <c r="D61" t="s">
         <v>8</v>
+      </c>
+      <c r="E61" t="s">
+        <v>53</v>
       </c>
       <c r="G61" t="str">
         <f t="shared" si="0"/>
@@ -3104,16 +3230,16 @@
     </row>
     <row r="62" spans="2:11">
       <c r="B62" t="s">
+        <v>120</v>
+      </c>
+      <c r="C62" t="s">
         <v>121</v>
       </c>
-      <c r="C62" t="s">
+      <c r="D62" t="s">
+        <v>8</v>
+      </c>
+      <c r="E62" t="s">
         <v>122</v>
-      </c>
-      <c r="D62" t="s">
-        <v>8</v>
-      </c>
-      <c r="E62" t="s">
-        <v>123</v>
       </c>
       <c r="G62" t="str">
         <f t="shared" si="0"/>
@@ -3134,13 +3260,16 @@
     </row>
     <row r="63" spans="2:11">
       <c r="B63" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C63" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="C63" s="1" t="s">
-        <v>125</v>
-      </c>
       <c r="D63" t="s">
         <v>8</v>
+      </c>
+      <c r="E63" t="s">
+        <v>93</v>
       </c>
       <c r="G63" t="str">
         <f t="shared" si="0"/>
@@ -3161,16 +3290,16 @@
     </row>
     <row r="64" spans="2:11">
       <c r="B64" t="s">
+        <v>125</v>
+      </c>
+      <c r="C64" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="C64" s="1" t="s">
-        <v>127</v>
-      </c>
       <c r="D64" t="s">
         <v>8</v>
       </c>
       <c r="E64" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G64" t="str">
         <f t="shared" si="0"/>
@@ -3191,16 +3320,16 @@
     </row>
     <row r="65" spans="2:11">
       <c r="B65" t="s">
+        <v>127</v>
+      </c>
+      <c r="C65" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="C65" s="1" t="s">
-        <v>129</v>
-      </c>
       <c r="D65" t="s">
         <v>8</v>
       </c>
       <c r="E65" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G65" t="str">
         <f t="shared" si="0"/>
@@ -3221,13 +3350,16 @@
     </row>
     <row r="66" spans="2:11">
       <c r="B66" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C66" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="C66" s="1" t="s">
-        <v>131</v>
-      </c>
       <c r="D66" t="s">
         <v>8</v>
+      </c>
+      <c r="E66" t="s">
+        <v>355</v>
       </c>
       <c r="G66" t="str">
         <f t="shared" si="0"/>
@@ -3248,13 +3380,16 @@
     </row>
     <row r="67" spans="2:11">
       <c r="B67" s="1" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="D67" t="s">
         <v>8</v>
+      </c>
+      <c r="E67" t="s">
+        <v>356</v>
       </c>
       <c r="G67" t="str">
         <f t="shared" si="0"/>
@@ -3275,16 +3410,16 @@
     </row>
     <row r="68" spans="2:11">
       <c r="B68" t="s">
+        <v>131</v>
+      </c>
+      <c r="C68" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="C68" s="1" t="s">
+      <c r="D68" t="s">
+        <v>8</v>
+      </c>
+      <c r="E68" t="s">
         <v>133</v>
-      </c>
-      <c r="D68" t="s">
-        <v>8</v>
-      </c>
-      <c r="E68" t="s">
-        <v>134</v>
       </c>
       <c r="G68" t="str">
         <f t="shared" si="0"/>
@@ -3305,13 +3440,16 @@
     </row>
     <row r="69" spans="2:11">
       <c r="B69" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C69" t="s">
         <v>135</v>
       </c>
-      <c r="C69" t="s">
-        <v>136</v>
-      </c>
       <c r="D69" t="s">
         <v>8</v>
+      </c>
+      <c r="E69" t="s">
+        <v>347</v>
       </c>
       <c r="G69" t="str">
         <f t="shared" si="0"/>
@@ -3332,16 +3470,16 @@
     </row>
     <row r="70" spans="2:11">
       <c r="B70" t="s">
+        <v>136</v>
+      </c>
+      <c r="C70" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="C70" s="1" t="s">
+      <c r="D70" t="s">
+        <v>8</v>
+      </c>
+      <c r="E70" t="s">
         <v>138</v>
-      </c>
-      <c r="D70" t="s">
-        <v>8</v>
-      </c>
-      <c r="E70" t="s">
-        <v>139</v>
       </c>
       <c r="G70" t="str">
         <f t="shared" si="0"/>
@@ -3362,13 +3500,16 @@
     </row>
     <row r="71" spans="2:11">
       <c r="B71" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C71" t="s">
         <v>140</v>
       </c>
-      <c r="C71" t="s">
-        <v>141</v>
-      </c>
       <c r="D71" t="s">
         <v>8</v>
+      </c>
+      <c r="E71" t="s">
+        <v>347</v>
       </c>
       <c r="G71" t="str">
         <f t="shared" si="0"/>
@@ -3389,13 +3530,16 @@
     </row>
     <row r="72" spans="2:11">
       <c r="B72" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C72" t="s">
         <v>142</v>
       </c>
-      <c r="C72" t="s">
-        <v>143</v>
-      </c>
       <c r="D72" t="s">
         <v>8</v>
+      </c>
+      <c r="E72" t="s">
+        <v>357</v>
       </c>
       <c r="G72" t="str">
         <f t="shared" si="0"/>
@@ -3416,16 +3560,16 @@
     </row>
     <row r="73" spans="2:11">
       <c r="B73" t="s">
+        <v>143</v>
+      </c>
+      <c r="C73" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="C73" s="1" t="s">
-        <v>145</v>
-      </c>
       <c r="D73" t="s">
         <v>8</v>
       </c>
       <c r="E73" t="s">
-        <v>146</v>
+        <v>93</v>
       </c>
       <c r="G73" t="str">
         <f t="shared" si="0"/>
@@ -3446,13 +3590,16 @@
     </row>
     <row r="74" spans="2:11">
       <c r="B74" s="3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C74" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D74" t="s">
         <v>8</v>
+      </c>
+      <c r="E74" t="s">
+        <v>351</v>
       </c>
       <c r="G74" t="str">
         <f t="shared" si="0"/>
@@ -3473,13 +3620,16 @@
     </row>
     <row r="75" spans="2:11">
       <c r="B75" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C75" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D75" t="s">
         <v>8</v>
+      </c>
+      <c r="E75" t="s">
+        <v>93</v>
       </c>
       <c r="G75" t="str">
         <f t="shared" ref="G75:G76" si="5">CONCATENATE(B75," ",C75,K75,"\\")</f>
@@ -3500,13 +3650,16 @@
     </row>
     <row r="76" spans="2:11">
       <c r="B76" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C76" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D76" t="s">
         <v>8</v>
+      </c>
+      <c r="E76" t="s">
+        <v>358</v>
       </c>
       <c r="G76" t="str">
         <f t="shared" si="5"/>
@@ -3527,16 +3680,16 @@
     </row>
     <row r="77" spans="2:11">
       <c r="B77" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="D77" t="s">
         <v>8</v>
       </c>
       <c r="E77" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G77" t="str">
         <f t="shared" ref="G77" si="8">CONCATENATE(B77," ",C77,K77,"\\")</f>
@@ -3557,16 +3710,16 @@
     </row>
     <row r="78" spans="2:11">
       <c r="B78" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="D78" t="s">
+        <v>8</v>
+      </c>
+      <c r="E78" t="s">
         <v>335</v>
-      </c>
-      <c r="C78" s="1" t="s">
-        <v>336</v>
-      </c>
-      <c r="D78" t="s">
-        <v>8</v>
-      </c>
-      <c r="E78" t="s">
-        <v>338</v>
       </c>
       <c r="G78" t="str">
         <f t="shared" ref="G78:G80" si="12">CONCATENATE(B78," ",C78,K78,"\\")</f>
@@ -3587,16 +3740,16 @@
     </row>
     <row r="79" spans="2:11">
       <c r="B79" t="s">
-        <v>342</v>
+        <v>47</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>337</v>
+        <v>48</v>
       </c>
       <c r="D79" t="s">
         <v>8</v>
       </c>
       <c r="E79" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G79" t="str">
         <f t="shared" si="12"/>
@@ -3656,16 +3809,16 @@
     </row>
     <row r="87" spans="2:11">
       <c r="B87" t="s">
+        <v>153</v>
+      </c>
+      <c r="C87" t="s">
+        <v>154</v>
+      </c>
+      <c r="D87" t="s">
         <v>155</v>
       </c>
-      <c r="C87" t="s">
+      <c r="E87" t="s">
         <v>156</v>
-      </c>
-      <c r="D87" t="s">
-        <v>157</v>
-      </c>
-      <c r="E87" t="s">
-        <v>158</v>
       </c>
       <c r="G87" t="str">
         <f t="shared" si="15"/>
@@ -3686,16 +3839,16 @@
     </row>
     <row r="88" spans="2:11">
       <c r="B88" t="s">
+        <v>157</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D88" t="s">
+        <v>155</v>
+      </c>
+      <c r="E88" t="s">
         <v>159</v>
-      </c>
-      <c r="C88" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="D88" t="s">
-        <v>157</v>
-      </c>
-      <c r="E88" t="s">
-        <v>161</v>
       </c>
       <c r="G88" t="str">
         <f t="shared" ref="G88:G140" si="18">CONCATENATE(B88," ",C88,K88,"\\")</f>
@@ -3716,16 +3869,16 @@
     </row>
     <row r="89" spans="2:11">
       <c r="B89" t="s">
+        <v>160</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="D89" t="s">
+        <v>155</v>
+      </c>
+      <c r="E89" t="s">
         <v>162</v>
-      </c>
-      <c r="C89" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="D89" t="s">
-        <v>157</v>
-      </c>
-      <c r="E89" t="s">
-        <v>164</v>
       </c>
       <c r="G89" t="str">
         <f t="shared" si="18"/>
@@ -3746,13 +3899,13 @@
     </row>
     <row r="90" spans="2:11">
       <c r="B90" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C90" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D90" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G90" t="str">
         <f t="shared" si="18"/>
@@ -3773,16 +3926,16 @@
     </row>
     <row r="91" spans="2:11">
       <c r="B91" t="s">
+        <v>165</v>
+      </c>
+      <c r="C91" t="s">
+        <v>166</v>
+      </c>
+      <c r="D91" t="s">
+        <v>155</v>
+      </c>
+      <c r="E91" t="s">
         <v>167</v>
-      </c>
-      <c r="C91" t="s">
-        <v>168</v>
-      </c>
-      <c r="D91" t="s">
-        <v>157</v>
-      </c>
-      <c r="E91" t="s">
-        <v>169</v>
       </c>
       <c r="G91" t="str">
         <f t="shared" si="18"/>
@@ -3803,16 +3956,16 @@
     </row>
     <row r="92" spans="2:11">
       <c r="B92" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D92" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E92" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="G92" t="str">
         <f t="shared" si="18"/>
@@ -3833,16 +3986,16 @@
     </row>
     <row r="93" spans="2:11">
       <c r="B93" t="s">
+        <v>171</v>
+      </c>
+      <c r="C93" t="s">
+        <v>172</v>
+      </c>
+      <c r="D93" t="s">
+        <v>155</v>
+      </c>
+      <c r="E93" t="s">
         <v>173</v>
-      </c>
-      <c r="C93" t="s">
-        <v>174</v>
-      </c>
-      <c r="D93" t="s">
-        <v>157</v>
-      </c>
-      <c r="E93" t="s">
-        <v>175</v>
       </c>
       <c r="G93" t="str">
         <f t="shared" si="18"/>
@@ -3863,16 +4016,16 @@
     </row>
     <row r="94" spans="2:11">
       <c r="B94" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C94" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D94" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E94" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G94" t="str">
         <f t="shared" si="18"/>
@@ -3893,16 +4046,16 @@
     </row>
     <row r="95" spans="2:11">
       <c r="B95" s="1" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="D95" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E95" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="G95" t="str">
         <f t="shared" si="18"/>
@@ -3923,16 +4076,16 @@
     </row>
     <row r="96" spans="2:11">
       <c r="B96" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C96" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D96" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E96" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G96" t="str">
         <f t="shared" si="18"/>
@@ -3953,16 +4106,16 @@
     </row>
     <row r="97" spans="2:11">
       <c r="B97" t="s">
+        <v>176</v>
+      </c>
+      <c r="C97" t="s">
+        <v>177</v>
+      </c>
+      <c r="D97" t="s">
+        <v>155</v>
+      </c>
+      <c r="E97" t="s">
         <v>178</v>
-      </c>
-      <c r="C97" t="s">
-        <v>179</v>
-      </c>
-      <c r="D97" t="s">
-        <v>157</v>
-      </c>
-      <c r="E97" t="s">
-        <v>180</v>
       </c>
       <c r="G97" t="str">
         <f t="shared" si="18"/>
@@ -3983,16 +4136,16 @@
     </row>
     <row r="98" spans="2:11">
       <c r="B98" t="s">
+        <v>179</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="D98" t="s">
+        <v>155</v>
+      </c>
+      <c r="E98" t="s">
         <v>181</v>
-      </c>
-      <c r="C98" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="D98" t="s">
-        <v>157</v>
-      </c>
-      <c r="E98" t="s">
-        <v>183</v>
       </c>
       <c r="G98" t="str">
         <f t="shared" si="18"/>
@@ -4013,16 +4166,16 @@
     </row>
     <row r="99" spans="2:11">
       <c r="B99" t="s">
+        <v>182</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="D99" t="s">
+        <v>155</v>
+      </c>
+      <c r="E99" t="s">
         <v>184</v>
-      </c>
-      <c r="C99" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="D99" t="s">
-        <v>157</v>
-      </c>
-      <c r="E99" t="s">
-        <v>186</v>
       </c>
       <c r="G99" t="str">
         <f t="shared" si="18"/>
@@ -4043,16 +4196,16 @@
     </row>
     <row r="100" spans="2:11">
       <c r="B100" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D100" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E100" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G100" t="str">
         <f t="shared" si="18"/>
@@ -4073,16 +4226,16 @@
     </row>
     <row r="101" spans="2:11">
       <c r="B101" t="s">
+        <v>193</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D101" t="s">
+        <v>155</v>
+      </c>
+      <c r="E101" t="s">
         <v>195</v>
-      </c>
-      <c r="C101" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="D101" t="s">
-        <v>157</v>
-      </c>
-      <c r="E101" t="s">
-        <v>197</v>
       </c>
       <c r="G101" t="str">
         <f t="shared" si="18"/>
@@ -4103,16 +4256,16 @@
     </row>
     <row r="102" spans="2:11">
       <c r="B102" t="s">
+        <v>196</v>
+      </c>
+      <c r="C102" t="s">
+        <v>197</v>
+      </c>
+      <c r="D102" t="s">
+        <v>155</v>
+      </c>
+      <c r="E102" t="s">
         <v>198</v>
-      </c>
-      <c r="C102" t="s">
-        <v>199</v>
-      </c>
-      <c r="D102" t="s">
-        <v>157</v>
-      </c>
-      <c r="E102" t="s">
-        <v>200</v>
       </c>
       <c r="G102" t="str">
         <f t="shared" si="18"/>
@@ -4133,16 +4286,16 @@
     </row>
     <row r="103" spans="2:11">
       <c r="B103" t="s">
+        <v>199</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="D103" t="s">
+        <v>155</v>
+      </c>
+      <c r="E103" t="s">
         <v>201</v>
-      </c>
-      <c r="C103" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="D103" t="s">
-        <v>157</v>
-      </c>
-      <c r="E103" t="s">
-        <v>203</v>
       </c>
       <c r="G103" t="str">
         <f t="shared" si="18"/>
@@ -4163,16 +4316,16 @@
     </row>
     <row r="104" spans="2:11">
       <c r="B104" s="1" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D104" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="G104" t="str">
         <f t="shared" si="18"/>
@@ -4193,16 +4346,16 @@
     </row>
     <row r="105" spans="2:11">
       <c r="B105" t="s">
+        <v>202</v>
+      </c>
+      <c r="C105" t="s">
+        <v>203</v>
+      </c>
+      <c r="D105" t="s">
+        <v>155</v>
+      </c>
+      <c r="E105" t="s">
         <v>204</v>
-      </c>
-      <c r="C105" t="s">
-        <v>205</v>
-      </c>
-      <c r="D105" t="s">
-        <v>157</v>
-      </c>
-      <c r="E105" t="s">
-        <v>206</v>
       </c>
       <c r="G105" t="str">
         <f t="shared" si="18"/>
@@ -4223,16 +4376,16 @@
     </row>
     <row r="106" spans="2:11">
       <c r="B106" s="1" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="D106" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="G106" t="str">
         <f t="shared" si="18"/>
@@ -4253,16 +4406,16 @@
     </row>
     <row r="107" spans="2:11">
       <c r="B107" t="s">
+        <v>205</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="D107" t="s">
+        <v>155</v>
+      </c>
+      <c r="E107" t="s">
         <v>207</v>
-      </c>
-      <c r="C107" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="D107" t="s">
-        <v>157</v>
-      </c>
-      <c r="E107" t="s">
-        <v>209</v>
       </c>
       <c r="G107" t="str">
         <f t="shared" si="18"/>
@@ -4283,16 +4436,16 @@
     </row>
     <row r="108" spans="2:11">
       <c r="B108" t="s">
+        <v>208</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="D108" t="s">
+        <v>155</v>
+      </c>
+      <c r="E108" t="s">
         <v>210</v>
-      </c>
-      <c r="C108" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="D108" t="s">
-        <v>157</v>
-      </c>
-      <c r="E108" t="s">
-        <v>212</v>
       </c>
       <c r="G108" t="str">
         <f t="shared" si="18"/>
@@ -4313,16 +4466,16 @@
     </row>
     <row r="109" spans="2:11">
       <c r="B109" t="s">
+        <v>211</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="D109" t="s">
+        <v>155</v>
+      </c>
+      <c r="E109" t="s">
         <v>213</v>
-      </c>
-      <c r="C109" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="D109" t="s">
-        <v>157</v>
-      </c>
-      <c r="E109" t="s">
-        <v>215</v>
       </c>
       <c r="G109" t="str">
         <f t="shared" si="18"/>
@@ -4343,16 +4496,16 @@
     </row>
     <row r="110" spans="2:11">
       <c r="B110" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D110" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E110" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="G110" t="str">
         <f t="shared" si="18"/>
@@ -4373,16 +4526,16 @@
     </row>
     <row r="111" spans="2:11">
       <c r="B111" t="s">
+        <v>216</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="D111" t="s">
+        <v>155</v>
+      </c>
+      <c r="E111" t="s">
         <v>218</v>
-      </c>
-      <c r="C111" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="D111" t="s">
-        <v>157</v>
-      </c>
-      <c r="E111" t="s">
-        <v>220</v>
       </c>
       <c r="G111" t="str">
         <f t="shared" si="18"/>
@@ -4403,16 +4556,16 @@
     </row>
     <row r="112" spans="2:11">
       <c r="B112" t="s">
+        <v>219</v>
+      </c>
+      <c r="C112" t="s">
+        <v>220</v>
+      </c>
+      <c r="D112" t="s">
+        <v>155</v>
+      </c>
+      <c r="E112" t="s">
         <v>221</v>
-      </c>
-      <c r="C112" t="s">
-        <v>222</v>
-      </c>
-      <c r="D112" t="s">
-        <v>157</v>
-      </c>
-      <c r="E112" t="s">
-        <v>223</v>
       </c>
       <c r="G112" t="str">
         <f t="shared" si="18"/>
@@ -4433,16 +4586,16 @@
     </row>
     <row r="113" spans="2:11">
       <c r="B113" t="s">
+        <v>222</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="D113" t="s">
+        <v>155</v>
+      </c>
+      <c r="E113" t="s">
         <v>224</v>
-      </c>
-      <c r="C113" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="D113" t="s">
-        <v>157</v>
-      </c>
-      <c r="E113" t="s">
-        <v>226</v>
       </c>
       <c r="G113" t="str">
         <f t="shared" si="18"/>
@@ -4463,16 +4616,16 @@
     </row>
     <row r="114" spans="2:11">
       <c r="B114" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C114" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="D114" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E114" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="G114" t="str">
         <f t="shared" si="18"/>
@@ -4493,16 +4646,16 @@
     </row>
     <row r="115" spans="2:11">
       <c r="B115" s="1" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="D115" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E115" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="G115" t="str">
         <f t="shared" si="18"/>
@@ -4523,16 +4676,16 @@
     </row>
     <row r="116" spans="2:11">
       <c r="B116" t="s">
+        <v>227</v>
+      </c>
+      <c r="C116" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="D116" t="s">
+        <v>155</v>
+      </c>
+      <c r="E116" t="s">
         <v>229</v>
-      </c>
-      <c r="C116" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="D116" t="s">
-        <v>157</v>
-      </c>
-      <c r="E116" t="s">
-        <v>231</v>
       </c>
       <c r="G116" t="str">
         <f t="shared" si="18"/>
@@ -4553,16 +4706,16 @@
     </row>
     <row r="117" spans="2:11">
       <c r="B117" t="s">
+        <v>230</v>
+      </c>
+      <c r="C117" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="D117" t="s">
+        <v>155</v>
+      </c>
+      <c r="E117" t="s">
         <v>232</v>
-      </c>
-      <c r="C117" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="D117" t="s">
-        <v>157</v>
-      </c>
-      <c r="E117" t="s">
-        <v>234</v>
       </c>
       <c r="G117" t="str">
         <f t="shared" si="18"/>
@@ -4583,16 +4736,16 @@
     </row>
     <row r="118" spans="2:11">
       <c r="B118" t="s">
+        <v>233</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="D118" t="s">
+        <v>155</v>
+      </c>
+      <c r="E118" t="s">
         <v>235</v>
-      </c>
-      <c r="C118" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="D118" t="s">
-        <v>157</v>
-      </c>
-      <c r="E118" t="s">
-        <v>237</v>
       </c>
       <c r="G118" t="str">
         <f t="shared" si="18"/>
@@ -4613,16 +4766,16 @@
     </row>
     <row r="119" spans="2:11">
       <c r="B119" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C119" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D119" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E119" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="G119" t="str">
         <f t="shared" si="18"/>
@@ -4643,16 +4796,16 @@
     </row>
     <row r="120" spans="2:11">
       <c r="B120" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D120" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E120" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="G120" t="str">
         <f t="shared" si="18"/>
@@ -4673,16 +4826,16 @@
     </row>
     <row r="121" spans="2:11">
       <c r="B121" t="s">
+        <v>240</v>
+      </c>
+      <c r="C121" t="s">
+        <v>241</v>
+      </c>
+      <c r="D121" t="s">
+        <v>155</v>
+      </c>
+      <c r="E121" t="s">
         <v>242</v>
-      </c>
-      <c r="C121" t="s">
-        <v>243</v>
-      </c>
-      <c r="D121" t="s">
-        <v>157</v>
-      </c>
-      <c r="E121" t="s">
-        <v>244</v>
       </c>
       <c r="G121" t="str">
         <f t="shared" si="18"/>
@@ -4703,16 +4856,16 @@
     </row>
     <row r="122" spans="2:11">
       <c r="B122" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C122" t="s">
+        <v>189</v>
+      </c>
+      <c r="D122" t="s">
+        <v>155</v>
+      </c>
+      <c r="E122" t="s">
         <v>191</v>
-      </c>
-      <c r="D122" t="s">
-        <v>157</v>
-      </c>
-      <c r="E122" t="s">
-        <v>193</v>
       </c>
       <c r="G122" t="str">
         <f t="shared" si="18"/>
@@ -4733,16 +4886,16 @@
     </row>
     <row r="123" spans="2:11">
       <c r="B123" t="s">
+        <v>243</v>
+      </c>
+      <c r="C123" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="D123" t="s">
+        <v>155</v>
+      </c>
+      <c r="E123" t="s">
         <v>245</v>
-      </c>
-      <c r="C123" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="D123" t="s">
-        <v>157</v>
-      </c>
-      <c r="E123" t="s">
-        <v>247</v>
       </c>
       <c r="G123" t="str">
         <f t="shared" si="18"/>
@@ -4763,16 +4916,16 @@
     </row>
     <row r="124" spans="2:11">
       <c r="B124" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="D124" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E124" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="G124" t="str">
         <f t="shared" si="18"/>
@@ -4793,16 +4946,16 @@
     </row>
     <row r="125" spans="2:11">
       <c r="B125" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C125" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="D125" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E125" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="G125" t="str">
         <f t="shared" si="18"/>
@@ -4823,16 +4976,16 @@
     </row>
     <row r="126" spans="2:11">
       <c r="B126" t="s">
+        <v>248</v>
+      </c>
+      <c r="C126" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="D126" t="s">
+        <v>155</v>
+      </c>
+      <c r="E126" t="s">
         <v>250</v>
-      </c>
-      <c r="C126" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="D126" t="s">
-        <v>157</v>
-      </c>
-      <c r="E126" t="s">
-        <v>252</v>
       </c>
       <c r="G126" t="str">
         <f t="shared" si="18"/>
@@ -4853,16 +5006,16 @@
     </row>
     <row r="127" spans="2:11">
       <c r="B127" t="s">
+        <v>251</v>
+      </c>
+      <c r="C127" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="D127" t="s">
+        <v>155</v>
+      </c>
+      <c r="E127" t="s">
         <v>253</v>
-      </c>
-      <c r="C127" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="D127" t="s">
-        <v>157</v>
-      </c>
-      <c r="E127" t="s">
-        <v>255</v>
       </c>
       <c r="G127" t="str">
         <f t="shared" si="18"/>
@@ -4883,16 +5036,16 @@
     </row>
     <row r="128" spans="2:11">
       <c r="B128" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="D128" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E128" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="G128" t="str">
         <f t="shared" si="18"/>
@@ -4913,16 +5066,16 @@
     </row>
     <row r="129" spans="2:11">
       <c r="B129" s="1" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="D129" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E129" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="G129" t="str">
         <f t="shared" si="18"/>
@@ -4943,16 +5096,16 @@
     </row>
     <row r="130" spans="2:11">
       <c r="B130" t="s">
+        <v>254</v>
+      </c>
+      <c r="C130" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="D130" t="s">
+        <v>155</v>
+      </c>
+      <c r="E130" t="s">
         <v>256</v>
-      </c>
-      <c r="C130" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="D130" t="s">
-        <v>157</v>
-      </c>
-      <c r="E130" t="s">
-        <v>258</v>
       </c>
       <c r="G130" t="str">
         <f t="shared" si="18"/>
@@ -4973,16 +5126,16 @@
     </row>
     <row r="131" spans="2:11">
       <c r="B131" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C131" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="D131" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E131" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G131" t="str">
         <f t="shared" si="18"/>
@@ -5003,16 +5156,16 @@
     </row>
     <row r="132" spans="2:11">
       <c r="B132" t="s">
+        <v>257</v>
+      </c>
+      <c r="C132" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="D132" t="s">
+        <v>155</v>
+      </c>
+      <c r="E132" t="s">
         <v>259</v>
-      </c>
-      <c r="C132" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="D132" t="s">
-        <v>157</v>
-      </c>
-      <c r="E132" t="s">
-        <v>261</v>
       </c>
       <c r="G132" t="str">
         <f t="shared" si="18"/>
@@ -5033,16 +5186,16 @@
     </row>
     <row r="133" spans="2:11">
       <c r="B133" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="D133" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E133" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="G133" t="str">
         <f t="shared" si="18"/>
@@ -5063,16 +5216,16 @@
     </row>
     <row r="134" spans="2:11">
       <c r="B134" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="D134" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E134" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="G134" t="str">
         <f t="shared" si="18"/>
@@ -5093,16 +5246,16 @@
     </row>
     <row r="135" spans="2:11">
       <c r="B135" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="D135" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E135" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="G135" t="str">
         <f t="shared" si="18"/>
@@ -5123,16 +5276,16 @@
     </row>
     <row r="136" spans="2:11">
       <c r="B136" t="s">
+        <v>262</v>
+      </c>
+      <c r="C136" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="D136" t="s">
+        <v>155</v>
+      </c>
+      <c r="E136" t="s">
         <v>264</v>
-      </c>
-      <c r="C136" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="D136" t="s">
-        <v>157</v>
-      </c>
-      <c r="E136" t="s">
-        <v>266</v>
       </c>
       <c r="G136" t="str">
         <f t="shared" si="18"/>
@@ -5156,13 +5309,13 @@
         <v>9</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="D137" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E137" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="G137" t="str">
         <f t="shared" si="18"/>
@@ -5183,16 +5336,16 @@
     </row>
     <row r="138" spans="2:11">
       <c r="B138" t="s">
+        <v>265</v>
+      </c>
+      <c r="C138" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="D138" t="s">
+        <v>155</v>
+      </c>
+      <c r="E138" t="s">
         <v>267</v>
-      </c>
-      <c r="C138" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="D138" t="s">
-        <v>157</v>
-      </c>
-      <c r="E138" t="s">
-        <v>269</v>
       </c>
       <c r="G138" t="str">
         <f t="shared" si="18"/>
@@ -5213,16 +5366,16 @@
     </row>
     <row r="139" spans="2:11">
       <c r="B139" s="1" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D139" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E139" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="G139" t="str">
         <f t="shared" si="18"/>
@@ -5243,16 +5396,16 @@
     </row>
     <row r="140" spans="2:11">
       <c r="B140" s="1" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="D140" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E140" s="1" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="G140" t="str">
         <f t="shared" si="18"/>
@@ -5273,16 +5426,16 @@
     </row>
     <row r="141" spans="2:11">
       <c r="B141" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="D141" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E141" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="G141" t="str">
         <f t="shared" ref="G141:G143" si="21">CONCATENATE(B141," ",C141,K141,"\\")</f>
@@ -5303,16 +5456,16 @@
     </row>
     <row r="142" spans="2:11">
       <c r="B142" t="s">
+        <v>268</v>
+      </c>
+      <c r="C142" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="D142" t="s">
+        <v>155</v>
+      </c>
+      <c r="E142" t="s">
         <v>270</v>
-      </c>
-      <c r="C142" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="D142" t="s">
-        <v>157</v>
-      </c>
-      <c r="E142" t="s">
-        <v>272</v>
       </c>
       <c r="G142" t="str">
         <f t="shared" si="21"/>
@@ -5333,16 +5486,16 @@
     </row>
     <row r="143" spans="2:11">
       <c r="B143" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D143" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E143" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G143" t="str">
         <f t="shared" si="21"/>
@@ -5417,13 +5570,13 @@
     </row>
     <row r="147" spans="2:11">
       <c r="B147" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C147" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D147" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G147" t="str">
         <f t="shared" ref="G147:G188" si="24">CONCATENATE(B147," ",C147,K147,"\\")</f>
@@ -5480,16 +5633,16 @@
     </row>
     <row r="150" spans="2:11">
       <c r="B150" s="1" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D150" t="s">
         <v>8</v>
       </c>
       <c r="E150" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="G150" t="str">
         <f t="shared" si="24"/>

</xml_diff>